<commit_message>
added pick state UI control to editor
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="172">
   <si>
     <t>Q</t>
   </si>
@@ -538,6 +538,15 @@
   </si>
   <si>
     <t>toggle labels</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>toggle draw</t>
+  </si>
+  <si>
+    <t>toggle smart</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1115,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1117,7 +1126,7 @@
   <dimension ref="B2:AD40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U44" sqref="U44"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,7 +1199,9 @@
         <v>98</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="9" t="s">
+        <v>169</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
@@ -1229,7 +1240,9 @@
       <c r="B4" s="1"/>
       <c r="C4" s="24"/>
       <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24" t="s">
+        <v>171</v>
+      </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -1256,13 +1269,15 @@
       <c r="AC4" s="22"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="12" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
       <c r="H5" s="1"/>
@@ -1293,7 +1308,7 @@
       <c r="AC5" s="13"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>

</xml_diff>

<commit_message>
copying empty patterns is faster
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -543,10 +543,10 @@
     <t>F1</t>
   </si>
   <si>
-    <t>toggle draw</t>
-  </si>
-  <si>
     <t>toggle smart</t>
+  </si>
+  <si>
+    <t>toggle drawing</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1115,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1126,7 +1126,7 @@
   <dimension ref="B2:AD40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,7 +1241,7 @@
       <c r="C4" s="24"/>
       <c r="D4" s="23"/>
       <c r="E4" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>

</xml_diff>

<commit_message>
hex or von Neumann rule letter can be before Generations postfix
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1118,7 +1118,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1129,7 +1129,7 @@
   <dimension ref="B2:AD40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
square cells cell borders, triangular neighbourhood square bounded grid, triangular digits to XYZ
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="174">
   <si>
     <t>Q</t>
   </si>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t>toggle hexagon</t>
+  </si>
+  <si>
+    <t>cell borders</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1121,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1129,7 +1132,7 @@
   <dimension ref="B2:AD40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2084,7 +2087,9 @@
       <c r="D23" s="1"/>
       <c r="E23" s="31"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="31"/>
+      <c r="G23" s="33" t="s">
+        <v>173</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
added toggle [R]History display hotkeys and toggle kill gliders hotkey
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
   <si>
     <t>Q</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>zoom 8x</t>
+  </si>
+  <si>
+    <t>[R]History on</t>
+  </si>
+  <si>
+    <t>[R]History off</t>
+  </si>
+  <si>
+    <t>toggle glider kill</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1133,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1135,7 +1144,7 @@
   <dimension ref="B2:AD40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+      <selection activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,7 +1884,7 @@
       <c r="AC17" s="4"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
@@ -1889,11 +1898,17 @@
       <c r="L18" s="1"/>
       <c r="M18" s="31"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="31"/>
+      <c r="O18" s="33" t="s">
+        <v>175</v>
+      </c>
       <c r="P18" s="1"/>
-      <c r="Q18" s="31"/>
+      <c r="Q18" s="33" t="s">
+        <v>176</v>
+      </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="31"/>
+      <c r="S18" s="33" t="s">
+        <v>177</v>
+      </c>
       <c r="T18" s="1"/>
       <c r="U18" s="31"/>
       <c r="V18" s="1"/>

</xml_diff>

<commit_message>
step back fix for undo
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="192">
   <si>
     <t>Q</t>
   </si>
@@ -565,6 +565,48 @@
   </si>
   <si>
     <t>toggle glider kill</t>
+  </si>
+  <si>
+    <t>Ctrl Z</t>
+  </si>
+  <si>
+    <t>Undo</t>
+  </si>
+  <si>
+    <t>Ctrl Shift Z</t>
+  </si>
+  <si>
+    <t>Redo</t>
+  </si>
+  <si>
+    <t>Ctrl C</t>
+  </si>
+  <si>
+    <t>Ctrl Shift C</t>
+  </si>
+  <si>
+    <t>Ctrl Alt C</t>
+  </si>
+  <si>
+    <t>undo edit</t>
+  </si>
+  <si>
+    <t>redo edit</t>
+  </si>
+  <si>
+    <t>copy current pattern</t>
+  </si>
+  <si>
+    <t>copy current pattern with comments</t>
+  </si>
+  <si>
+    <t>copy original pattern</t>
+  </si>
+  <si>
+    <t>Ctrl S</t>
+  </si>
+  <si>
+    <t>save pattern</t>
   </si>
 </sst>
 </file>
@@ -628,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -773,6 +815,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -783,7 +840,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -859,6 +915,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1133,7 +1192,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1144,7 +1203,7 @@
   <dimension ref="B2:AD40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,11 +1272,11 @@
     </row>
     <row r="3" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>163</v>
       </c>
       <c r="F3" s="1"/>
@@ -1237,93 +1296,93 @@
       <c r="T3" s="1"/>
       <c r="U3" s="3"/>
       <c r="V3" s="1"/>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="10" t="s">
         <v>79</v>
       </c>
       <c r="X3" s="1"/>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="10" t="s">
         <v>80</v>
       </c>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="11" t="s">
+      <c r="AA3" s="10" t="s">
         <v>81</v>
       </c>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="11" t="s">
+      <c r="AC3" s="10" t="s">
         <v>82</v>
       </c>
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="21"/>
       <c r="AD4" s="1"/>
     </row>
     <row r="5" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>114</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>165</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="6"/>
+      <c r="K5" s="5"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="6"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="6"/>
+      <c r="O5" s="5"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="6"/>
+      <c r="Q5" s="5"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="6"/>
+      <c r="S5" s="5"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="6"/>
+      <c r="U5" s="5"/>
       <c r="V5" s="1"/>
-      <c r="W5" s="13" t="s">
+      <c r="W5" s="12" t="s">
         <v>86</v>
       </c>
       <c r="X5" s="1"/>
-      <c r="Y5" s="13" t="s">
+      <c r="Y5" s="12" t="s">
         <v>87</v>
       </c>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="13"/>
+      <c r="AA5" s="12"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="13"/>
+      <c r="AC5" s="12"/>
       <c r="AD5" s="1"/>
     </row>
     <row r="6" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1359,212 +1418,212 @@
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="8" t="s">
         <v>28</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="8" t="s">
         <v>30</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="8" t="s">
         <v>31</v>
       </c>
       <c r="R7" s="1"/>
-      <c r="S7" s="9" t="s">
+      <c r="S7" s="8" t="s">
         <v>32</v>
       </c>
       <c r="T7" s="1"/>
-      <c r="U7" s="9" t="s">
+      <c r="U7" s="8" t="s">
         <v>33</v>
       </c>
       <c r="V7" s="1"/>
-      <c r="W7" s="9" t="s">
+      <c r="W7" s="8" t="s">
         <v>34</v>
       </c>
       <c r="X7" s="1"/>
-      <c r="Y7" s="9" t="s">
+      <c r="Y7" s="8" t="s">
         <v>35</v>
       </c>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="9" t="s">
+      <c r="AA7" s="8" t="s">
         <v>36</v>
       </c>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="11" t="s">
+      <c r="AC7" s="10" t="s">
         <v>85</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
     <row r="8" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="32" t="s">
         <v>145</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="32" t="s">
         <v>147</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="32" t="s">
         <v>148</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="32" t="s">
         <v>149</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="32" t="s">
         <v>150</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="33" t="s">
+      <c r="O8" s="32" t="s">
         <v>151</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="32" t="s">
         <v>152</v>
       </c>
       <c r="R8" s="1"/>
-      <c r="S8" s="33" t="s">
+      <c r="S8" s="32" t="s">
         <v>153</v>
       </c>
       <c r="T8" s="1"/>
-      <c r="U8" s="33" t="s">
+      <c r="U8" s="32" t="s">
         <v>154</v>
       </c>
       <c r="V8" s="1"/>
-      <c r="W8" s="32"/>
+      <c r="W8" s="31"/>
       <c r="X8" s="1"/>
-      <c r="Y8" s="32"/>
+      <c r="Y8" s="31"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="32"/>
+      <c r="AA8" s="31"/>
       <c r="AB8" s="1"/>
-      <c r="AC8" s="31"/>
+      <c r="AC8" s="30"/>
       <c r="AD8" s="1"/>
     </row>
     <row r="9" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24" t="s">
+      <c r="H9" s="22"/>
+      <c r="I9" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24" t="s">
+      <c r="J9" s="22"/>
+      <c r="K9" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="24" t="s">
+      <c r="L9" s="22"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="24" t="s">
+      <c r="P9" s="22"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="T9" s="23"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="24" t="s">
+      <c r="T9" s="22"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="24" t="s">
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="21"/>
       <c r="AD9" s="1"/>
     </row>
     <row r="10" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
-      <c r="C10" s="13"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>169</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>170</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>171</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>172</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="11" t="s">
         <v>94</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="11" t="s">
         <v>173</v>
       </c>
       <c r="P10" s="1"/>
-      <c r="Q10" s="12" t="s">
+      <c r="Q10" s="11" t="s">
         <v>139</v>
       </c>
       <c r="R10" s="1"/>
-      <c r="S10" s="12" t="s">
+      <c r="S10" s="11" t="s">
         <v>174</v>
       </c>
       <c r="T10" s="1"/>
-      <c r="U10" s="12" t="s">
+      <c r="U10" s="11" t="s">
         <v>138</v>
       </c>
       <c r="V10" s="1"/>
-      <c r="W10" s="12" t="s">
+      <c r="W10" s="11" t="s">
         <v>134</v>
       </c>
       <c r="X10" s="1"/>
-      <c r="Y10" s="12" t="s">
+      <c r="Y10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="12" t="s">
+      <c r="AA10" s="11" t="s">
         <v>49</v>
       </c>
       <c r="AB10" s="1"/>
-      <c r="AC10" s="13"/>
+      <c r="AC10" s="12"/>
       <c r="AD10" s="1"/>
     </row>
     <row r="11" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1600,200 +1659,200 @@
     </row>
     <row r="12" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="10" t="s">
         <v>2</v>
       </c>
       <c r="J12" s="1"/>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="10" t="s">
         <v>3</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="10" t="s">
         <v>4</v>
       </c>
       <c r="N12" s="1"/>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="10" t="s">
         <v>5</v>
       </c>
       <c r="P12" s="1"/>
-      <c r="Q12" s="11" t="s">
+      <c r="Q12" s="10" t="s">
         <v>142</v>
       </c>
       <c r="R12" s="1"/>
-      <c r="S12" s="11" t="s">
+      <c r="S12" s="10" t="s">
         <v>6</v>
       </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="11" t="s">
+      <c r="U12" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V12" s="1"/>
-      <c r="W12" s="11" t="s">
+      <c r="W12" s="10" t="s">
         <v>8</v>
       </c>
       <c r="X12" s="1"/>
-      <c r="Y12" s="11" t="s">
+      <c r="Y12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="11" t="s">
+      <c r="AA12" s="10" t="s">
         <v>38</v>
       </c>
       <c r="AB12" s="1"/>
-      <c r="AC12" s="11" t="s">
+      <c r="AC12" s="10" t="s">
         <v>46</v>
       </c>
       <c r="AD12" s="1"/>
     </row>
     <row r="13" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="31"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="31"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="31"/>
+      <c r="I13" s="30"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="31"/>
+      <c r="K13" s="30"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="31"/>
+      <c r="M13" s="30"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="31"/>
+      <c r="O13" s="30"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="31"/>
+      <c r="Q13" s="30"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="31"/>
+      <c r="S13" s="30"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="31"/>
+      <c r="U13" s="30"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="31"/>
+      <c r="W13" s="30"/>
       <c r="X13" s="1"/>
-      <c r="Y13" s="31"/>
+      <c r="Y13" s="30"/>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="31"/>
+      <c r="AA13" s="30"/>
       <c r="AB13" s="1"/>
-      <c r="AC13" s="31"/>
+      <c r="AC13" s="30"/>
       <c r="AD13" s="1"/>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="22" t="s">
+      <c r="D14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="22" t="s">
+      <c r="J14" s="22"/>
+      <c r="K14" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="22" t="s">
+      <c r="L14" s="22"/>
+      <c r="M14" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="22" t="s">
+      <c r="N14" s="22"/>
+      <c r="O14" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="22" t="s">
+      <c r="P14" s="22"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="T14" s="23"/>
-      <c r="U14" s="22" t="s">
+      <c r="T14" s="22"/>
+      <c r="U14" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="V14" s="23"/>
-      <c r="W14" s="22" t="s">
+      <c r="V14" s="22"/>
+      <c r="W14" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="22" t="s">
+      <c r="X14" s="22"/>
+      <c r="Y14" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="22" t="s">
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="22"/>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="21"/>
       <c r="AD14" s="1"/>
     </row>
     <row r="15" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>132</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>126</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="12" t="s">
         <v>75</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="12" t="s">
         <v>47</v>
       </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="12" t="s">
         <v>70</v>
       </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="13" t="s">
+      <c r="O15" s="12" t="s">
         <v>136</v>
       </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="13" t="s">
+      <c r="Q15" s="12" t="s">
         <v>159</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="13" t="s">
+      <c r="S15" s="12" t="s">
         <v>71</v>
       </c>
       <c r="T15" s="1"/>
-      <c r="U15" s="13" t="s">
+      <c r="U15" s="12" t="s">
         <v>141</v>
       </c>
       <c r="V15" s="1"/>
-      <c r="W15" s="13" t="s">
+      <c r="W15" s="12" t="s">
         <v>66</v>
       </c>
       <c r="X15" s="1"/>
-      <c r="Y15" s="13" t="s">
+      <c r="Y15" s="12" t="s">
         <v>51</v>
       </c>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="13" t="s">
+      <c r="AA15" s="12" t="s">
         <v>52</v>
       </c>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="13" t="s">
+      <c r="AC15" s="12" t="s">
         <v>96</v>
       </c>
       <c r="AD15" s="1"/>
@@ -1833,51 +1892,51 @@
       <c r="B17" s="1"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L17" s="1"/>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="10" t="s">
         <v>13</v>
       </c>
       <c r="N17" s="1"/>
-      <c r="O17" s="11" t="s">
+      <c r="O17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="P17" s="1"/>
-      <c r="Q17" s="11" t="s">
+      <c r="Q17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="R17" s="1"/>
-      <c r="S17" s="11" t="s">
+      <c r="S17" s="10" t="s">
         <v>16</v>
       </c>
       <c r="T17" s="1"/>
-      <c r="U17" s="11" t="s">
+      <c r="U17" s="10" t="s">
         <v>17</v>
       </c>
       <c r="V17" s="1"/>
-      <c r="W17" s="11" t="s">
+      <c r="W17" s="10" t="s">
         <v>39</v>
       </c>
       <c r="X17" s="1"/>
-      <c r="Y17" s="9" t="s">
+      <c r="Y17" s="8" t="s">
         <v>41</v>
       </c>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="11" t="s">
+      <c r="AA17" s="10" t="s">
         <v>40</v>
       </c>
       <c r="AB17" s="1"/>
@@ -1888,133 +1947,133 @@
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="31"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="31"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="31"/>
+      <c r="I18" s="30"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="31"/>
+      <c r="K18" s="30"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="31"/>
+      <c r="M18" s="30"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="33" t="s">
+      <c r="O18" s="32" t="s">
         <v>175</v>
       </c>
       <c r="P18" s="1"/>
-      <c r="Q18" s="33" t="s">
+      <c r="Q18" s="32" t="s">
         <v>176</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="33" t="s">
+      <c r="S18" s="32" t="s">
         <v>177</v>
       </c>
       <c r="T18" s="1"/>
-      <c r="U18" s="31"/>
+      <c r="U18" s="30"/>
       <c r="V18" s="1"/>
-      <c r="W18" s="31"/>
+      <c r="W18" s="30"/>
       <c r="X18" s="1"/>
-      <c r="Y18" s="32"/>
+      <c r="Y18" s="31"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="31"/>
+      <c r="AA18" s="30"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="4"/>
       <c r="AD18" s="1"/>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="22" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="22" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="22" t="s">
+      <c r="J19" s="22"/>
+      <c r="K19" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="L19" s="23"/>
-      <c r="M19" s="22" t="s">
+      <c r="L19" s="22"/>
+      <c r="M19" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="23"/>
-      <c r="O19" s="22" t="s">
+      <c r="N19" s="22"/>
+      <c r="O19" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="22" t="s">
+      <c r="P19" s="22"/>
+      <c r="Q19" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="R19" s="23"/>
-      <c r="S19" s="22" t="s">
+      <c r="R19" s="22"/>
+      <c r="S19" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="T19" s="23"/>
-      <c r="U19" s="22" t="s">
+      <c r="T19" s="22"/>
+      <c r="U19" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="V19" s="23"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="22"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="26"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="25"/>
       <c r="AD19" s="1"/>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="12" t="s">
         <v>93</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>76</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="12" t="s">
         <v>53</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="13" t="s">
+      <c r="M20" s="12" t="s">
         <v>69</v>
       </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="13" t="s">
+      <c r="O20" s="12" t="s">
         <v>73</v>
       </c>
       <c r="P20" s="1"/>
-      <c r="Q20" s="13" t="s">
+      <c r="Q20" s="12" t="s">
         <v>120</v>
       </c>
       <c r="R20" s="1"/>
-      <c r="S20" s="13" t="s">
+      <c r="S20" s="12" t="s">
         <v>160</v>
       </c>
       <c r="T20" s="1"/>
-      <c r="U20" s="13" t="s">
+      <c r="U20" s="12" t="s">
         <v>67</v>
       </c>
       <c r="V20" s="1"/>
-      <c r="W20" s="13"/>
+      <c r="W20" s="12"/>
       <c r="X20" s="1"/>
-      <c r="Y20" s="13"/>
+      <c r="Y20" s="12"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="13"/>
+      <c r="AA20" s="12"/>
       <c r="AB20" s="1"/>
-      <c r="AC20" s="8"/>
+      <c r="AC20" s="7"/>
       <c r="AD20" s="1"/>
     </row>
     <row r="21" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2050,188 +2109,188 @@
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>90</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="10" t="s">
         <v>22</v>
       </c>
       <c r="N22" s="1"/>
-      <c r="O22" s="11" t="s">
+      <c r="O22" s="10" t="s">
         <v>23</v>
       </c>
       <c r="P22" s="1"/>
-      <c r="Q22" s="11" t="s">
+      <c r="Q22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="R22" s="1"/>
-      <c r="S22" s="11" t="s">
+      <c r="S22" s="10" t="s">
         <v>42</v>
       </c>
       <c r="T22" s="1"/>
-      <c r="U22" s="11" t="s">
+      <c r="U22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="V22" s="1"/>
-      <c r="W22" s="11" t="s">
+      <c r="W22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="X22" s="1"/>
-      <c r="Y22" s="14"/>
+      <c r="Y22" s="13"/>
       <c r="Z22" s="1"/>
-      <c r="AA22" s="14"/>
+      <c r="AA22" s="13"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="1"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23" s="31"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="31"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="32" t="s">
         <v>167</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="32" t="s">
         <v>119</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="31"/>
+      <c r="K23" s="30"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="31"/>
+      <c r="M23" s="30"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="31"/>
+      <c r="O23" s="30"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="31"/>
+      <c r="Q23" s="30"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="31"/>
+      <c r="S23" s="30"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="31"/>
+      <c r="U23" s="30"/>
       <c r="V23" s="1"/>
-      <c r="W23" s="33" t="s">
+      <c r="W23" s="32" t="s">
         <v>166</v>
       </c>
       <c r="X23" s="1"/>
-      <c r="Y23" s="14"/>
+      <c r="Y23" s="13"/>
       <c r="Z23" s="1"/>
-      <c r="AA23" s="14"/>
+      <c r="AA23" s="13"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="1"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="22" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="22" t="s">
+      <c r="F24" s="22"/>
+      <c r="G24" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="22" t="s">
+      <c r="H24" s="22"/>
+      <c r="I24" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="22" t="s">
+      <c r="J24" s="22"/>
+      <c r="K24" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="L24" s="23"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="22" t="s">
+      <c r="L24" s="22"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="T24" s="23"/>
-      <c r="U24" s="22" t="s">
+      <c r="T24" s="22"/>
+      <c r="U24" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="V24" s="23"/>
-      <c r="W24" s="22" t="s">
+      <c r="V24" s="22"/>
+      <c r="W24" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="X24" s="23"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="23"/>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="23"/>
-      <c r="AC24" s="23"/>
+      <c r="X24" s="22"/>
+      <c r="Y24" s="26"/>
+      <c r="Z24" s="22"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="22"/>
+      <c r="AC24" s="22"/>
       <c r="AD24" s="1"/>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="12" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="12" t="s">
         <v>72</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="12" t="s">
         <v>68</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="13" t="s">
+      <c r="K25" s="12" t="s">
         <v>117</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="13" t="s">
+      <c r="M25" s="12" t="s">
         <v>118</v>
       </c>
       <c r="N25" s="1"/>
-      <c r="O25" s="13" t="s">
+      <c r="O25" s="12" t="s">
         <v>91</v>
       </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="13" t="s">
+      <c r="Q25" s="12" t="s">
         <v>77</v>
       </c>
       <c r="R25" s="1"/>
-      <c r="S25" s="13" t="s">
+      <c r="S25" s="12" t="s">
         <v>54</v>
       </c>
       <c r="T25" s="1"/>
-      <c r="U25" s="13" t="s">
+      <c r="U25" s="12" t="s">
         <v>55</v>
       </c>
       <c r="V25" s="1"/>
-      <c r="W25" s="13" t="s">
+      <c r="W25" s="12" t="s">
         <v>122</v>
       </c>
       <c r="X25" s="1"/>
-      <c r="Y25" s="15"/>
+      <c r="Y25" s="14"/>
       <c r="Z25" s="1"/>
-      <c r="AA25" s="15"/>
+      <c r="AA25" s="14"/>
       <c r="AB25" s="1"/>
-      <c r="AC25" s="6"/>
+      <c r="AC25" s="5"/>
       <c r="AD25" s="1"/>
     </row>
     <row r="26" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2267,27 +2326,27 @@
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>143</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="3"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="18"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="17"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="1"/>
@@ -2295,95 +2354,95 @@
       <c r="V27" s="1"/>
       <c r="W27" s="3"/>
       <c r="X27" s="1"/>
-      <c r="Y27" s="11" t="s">
+      <c r="Y27" s="10" t="s">
         <v>83</v>
       </c>
       <c r="Z27" s="1"/>
-      <c r="AA27" s="11" t="s">
+      <c r="AA27" s="10" t="s">
         <v>56</v>
       </c>
       <c r="AB27" s="1"/>
-      <c r="AC27" s="11" t="s">
+      <c r="AC27" s="10" t="s">
         <v>84</v>
       </c>
       <c r="AD27" s="1"/>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="34" t="s">
+      <c r="D28" s="22"/>
+      <c r="E28" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="23"/>
-      <c r="Y28" s="22" t="s">
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="Z28" s="23"/>
-      <c r="AA28" s="22" t="s">
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AB28" s="23"/>
-      <c r="AC28" s="22" t="s">
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="21" t="s">
         <v>158</v>
       </c>
       <c r="AD28" s="1"/>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
-      <c r="C29" s="13"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="5"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="19" t="s">
+      <c r="I29" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
       <c r="T29" s="1"/>
-      <c r="U29" s="6"/>
+      <c r="U29" s="5"/>
       <c r="V29" s="1"/>
-      <c r="W29" s="6"/>
+      <c r="W29" s="5"/>
       <c r="X29" s="1"/>
-      <c r="Y29" s="13" t="s">
+      <c r="Y29" s="12" t="s">
         <v>88</v>
       </c>
       <c r="Z29" s="1"/>
-      <c r="AA29" s="13" t="s">
+      <c r="AA29" s="12" t="s">
         <v>60</v>
       </c>
       <c r="AB29" s="1"/>
-      <c r="AC29" s="13" t="s">
+      <c r="AC29" s="12" t="s">
         <v>89</v>
       </c>
       <c r="AD29" s="1"/>
@@ -2443,102 +2502,132 @@
       <c r="V31" s="1"/>
       <c r="W31" s="3"/>
       <c r="X31" s="1"/>
-      <c r="Y31" s="11" t="s">
+      <c r="Y31" s="10" t="s">
         <v>57</v>
       </c>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="11" t="s">
+      <c r="AA31" s="10" t="s">
         <v>58</v>
       </c>
       <c r="AB31" s="1"/>
-      <c r="AC31" s="11" t="s">
+      <c r="AC31" s="10" t="s">
         <v>59</v>
       </c>
       <c r="AD31" s="1"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="22" t="s">
+      <c r="C32" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H32" s="22"/>
+      <c r="I32" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
+      <c r="Y32" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="22" t="s">
+      <c r="Z32" s="22"/>
+      <c r="AA32" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="AB32" s="23"/>
-      <c r="AC32" s="22" t="s">
+      <c r="AB32" s="22"/>
+      <c r="AC32" s="21" t="s">
         <v>112</v>
       </c>
       <c r="AD32" s="1"/>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="6"/>
+      <c r="C33" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>186</v>
+      </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="6"/>
+      <c r="G33" s="34" t="s">
+        <v>183</v>
+      </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
+      <c r="I33" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
       <c r="T33" s="1"/>
-      <c r="U33" s="6"/>
+      <c r="U33" s="5"/>
       <c r="V33" s="1"/>
-      <c r="W33" s="6"/>
+      <c r="W33" s="5"/>
       <c r="X33" s="1"/>
-      <c r="Y33" s="13" t="s">
+      <c r="Y33" s="12" t="s">
         <v>61</v>
       </c>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="13" t="s">
+      <c r="AA33" s="12" t="s">
         <v>62</v>
       </c>
       <c r="AB33" s="1"/>
-      <c r="AC33" s="13" t="s">
+      <c r="AC33" s="12" t="s">
         <v>63</v>
       </c>
       <c r="AD33" s="1"/>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="C34" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="34" t="s">
+        <v>184</v>
+      </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="I34" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -2561,8 +2650,39 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
+    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+    </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="G40" s="5"/>
+      <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grey out icons, improve settings menu buttons, cancel Pick mode on mode change
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
   <si>
     <t>Q</t>
   </si>
@@ -607,6 +607,30 @@
   </si>
   <si>
     <t>save pattern</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>draw mode</t>
+  </si>
+  <si>
+    <t>select mode</t>
+  </si>
+  <si>
+    <t>pick mode</t>
+  </si>
+  <si>
+    <t>pan mode</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1216,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1203,7 +1227,7 @@
   <dimension ref="B2:AD40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,13 +1304,21 @@
         <v>163</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="8" t="s">
+        <v>192</v>
+      </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="8" t="s">
+        <v>193</v>
+      </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="3"/>
+      <c r="K3" s="8" t="s">
+        <v>194</v>
+      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="3"/>
+      <c r="M3" s="8" t="s">
+        <v>195</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="3"/>
       <c r="P3" s="1"/>
@@ -1321,13 +1353,13 @@
         <v>164</v>
       </c>
       <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
@@ -1356,13 +1388,21 @@
         <v>165</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="5"/>
+      <c r="I5" s="11" t="s">
+        <v>198</v>
+      </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="5"/>
+      <c r="M5" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="5"/>
       <c r="P5" s="1"/>

</xml_diff>

<commit_message>
added invert selection button, fixed selecting in bounded grids, fixed popcount at generation 0 while editing with stats off
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="206">
   <si>
     <t>Q</t>
   </si>
@@ -646,6 +646,9 @@
   </si>
   <si>
     <t>select all</t>
+  </si>
+  <si>
+    <t>invert selection</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1260,7 +1263,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1908,7 +1911,9 @@
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
-      <c r="S16" s="35"/>
+      <c r="S16" s="35" t="s">
+        <v>205</v>
+      </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35"/>
       <c r="V16" s="36"/>
@@ -2005,7 +2010,7 @@
       <c r="AC18" s="21"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
         <v>132</v>
@@ -2064,7 +2069,7 @@
       </c>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2095,7 +2100,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>

</xml_diff>

<commit_message>
add new pattern and change rule features, add paste box, selection manipulation commands work on paste box if visible
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="208">
   <si>
     <t>Q</t>
   </si>
@@ -649,6 +649,12 @@
   </si>
   <si>
     <t>invert selection</t>
+  </si>
+  <si>
+    <t>new pattern</t>
+  </si>
+  <si>
+    <t>change rule</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1258,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1263,7 +1269,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,7 +1907,9 @@
       <c r="H16" s="36"/>
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>
-      <c r="K16" s="35"/>
+      <c r="K16" s="35" t="s">
+        <v>207</v>
+      </c>
       <c r="L16" s="36"/>
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
@@ -2431,7 +2439,9 @@
       <c r="L28" s="36"/>
       <c r="M28" s="35"/>
       <c r="N28" s="36"/>
-      <c r="O28" s="35"/>
+      <c r="O28" s="35" t="s">
+        <v>206</v>
+      </c>
       <c r="P28" s="36"/>
       <c r="Q28" s="35"/>
       <c r="R28" s="36"/>

</xml_diff>

<commit_message>
open last saved pattern
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="211">
   <si>
     <t>Q</t>
   </si>
@@ -655,6 +655,15 @@
   </si>
   <si>
     <t>change rule</t>
+  </si>
+  <si>
+    <t>Ctrl Shift 5</t>
+  </si>
+  <si>
+    <t>2 state random fill</t>
+  </si>
+  <si>
+    <t>open pattern</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1267,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,7 +1278,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1923,7 +1932,9 @@
         <v>205</v>
       </c>
       <c r="T16" s="36"/>
-      <c r="U16" s="35"/>
+      <c r="U16" s="35" t="s">
+        <v>210</v>
+      </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
       <c r="X16" s="36"/>
@@ -2831,15 +2842,15 @@
         <v>195</v>
       </c>
       <c r="F38" s="22"/>
-      <c r="G38" s="34" t="s">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="5" t="s">
+      <c r="J38" s="1"/>
+      <c r="K38" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="22"/>
@@ -2868,19 +2879,25 @@
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="C39" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>209</v>
+      </c>
       <c r="F39" s="1"/>
-      <c r="G39" s="34" t="s">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="5" t="s">
+      <c r="J39" s="1"/>
+      <c r="K39" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="5"/>

</xml_diff>

<commit_message>
added sync button, improved select mode button layout, added library button to select active clipboard
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="212">
   <si>
     <t>Q</t>
   </si>
@@ -468,36 +468,9 @@
     <t>command</t>
   </si>
   <si>
-    <t>POI 1</t>
-  </si>
-  <si>
     <t>Shift</t>
   </si>
   <si>
-    <t>POI 2</t>
-  </si>
-  <si>
-    <t>POI 3</t>
-  </si>
-  <si>
-    <t>POI 4</t>
-  </si>
-  <si>
-    <t>POI 5</t>
-  </si>
-  <si>
-    <t>POI 6</t>
-  </si>
-  <si>
-    <t>POI 7</t>
-  </si>
-  <si>
-    <t>POI 8</t>
-  </si>
-  <si>
-    <t>POI 9</t>
-  </si>
-  <si>
     <t>previous theme</t>
   </si>
   <si>
@@ -664,6 +637,36 @@
   </si>
   <si>
     <t>open pattern</t>
+  </si>
+  <si>
+    <t>Clip / POI 1</t>
+  </si>
+  <si>
+    <t>Clip 0</t>
+  </si>
+  <si>
+    <t>Clip / POI 9</t>
+  </si>
+  <si>
+    <t>Clip / POI 8</t>
+  </si>
+  <si>
+    <t>Clip / POI 7</t>
+  </si>
+  <si>
+    <t>Clip / POI 6</t>
+  </si>
+  <si>
+    <t>Clip / POI 5</t>
+  </si>
+  <si>
+    <t>Clip / POI 4</t>
+  </si>
+  <si>
+    <t>Clip / POI 3</t>
+  </si>
+  <si>
+    <t>Clip / POI 2</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1270,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1278,7 +1281,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1352,23 +1355,23 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="8" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="3"/>
@@ -1465,7 +1468,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="23"/>
@@ -1498,23 +1501,23 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="11" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="5"/>
@@ -1536,7 +1539,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1643,7 +1646,7 @@
       <c r="K10" s="37"/>
       <c r="L10" s="36"/>
       <c r="M10" s="38" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37"/>
@@ -1663,47 +1666,49 @@
       <c r="AC10" s="35"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>148</v>
+        <v>210</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>149</v>
+        <v>209</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>151</v>
+        <v>207</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>152</v>
+        <v>206</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="V11" s="1"/>
-      <c r="W11" s="31"/>
+      <c r="W11" s="32" t="s">
+        <v>203</v>
+      </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
       <c r="Z11" s="1"/>
@@ -1725,7 +1730,7 @@
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
@@ -1764,19 +1769,19 @@
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="11" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="11" t="s">
@@ -1784,7 +1789,7 @@
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="11" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11" t="s">
@@ -1792,7 +1797,7 @@
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="11" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="11" t="s">
@@ -1917,23 +1922,23 @@
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>
       <c r="K16" s="35" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="L16" s="36"/>
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -1960,7 +1965,7 @@
       <c r="M17" s="33"/>
       <c r="N17" s="39"/>
       <c r="O17" s="33" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="P17" s="39"/>
       <c r="Q17" s="33"/>
@@ -2015,7 +2020,7 @@
       </c>
       <c r="V18" s="22"/>
       <c r="W18" s="21" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="21" t="s">
@@ -2060,7 +2065,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2179,11 +2184,11 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
@@ -2197,7 +2202,7 @@
       <c r="Q22" s="35"/>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35"/>
@@ -2226,15 +2231,15 @@
       <c r="M23" s="30"/>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="30"/>
@@ -2279,11 +2284,11 @@
       </c>
       <c r="R24" s="22"/>
       <c r="S24" s="21" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2328,7 +2333,7 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="12" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="12" t="s">
@@ -2433,25 +2438,25 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35"/>
       <c r="N28" s="36"/>
       <c r="O28" s="35" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="P28" s="36"/>
       <c r="Q28" s="35"/>
@@ -2476,7 +2481,7 @@
       <c r="E29" s="30"/>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2486,7 +2491,7 @@
       <c r="K29" s="30"/>
       <c r="L29" s="1"/>
       <c r="M29" s="32" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="30"/>
@@ -2498,7 +2503,7 @@
       <c r="U29" s="30"/>
       <c r="V29" s="1"/>
       <c r="W29" s="32" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="X29" s="1"/>
       <c r="Y29" s="13"/>
@@ -2521,7 +2526,7 @@
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="21" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="21" t="s">
@@ -2638,11 +2643,11 @@
     <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2711,7 +2716,7 @@
       <c r="W34" s="22"/>
       <c r="X34" s="22"/>
       <c r="Y34" s="21" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="Z34" s="22"/>
       <c r="AA34" s="21" t="s">
@@ -2719,7 +2724,7 @@
       </c>
       <c r="AB34" s="22"/>
       <c r="AC34" s="21" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="AD34" s="1"/>
     </row>
@@ -2833,23 +2838,23 @@
     <row r="38" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="34" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="34" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
@@ -2880,23 +2885,23 @@
     <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="34" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="34" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>

</xml_diff>

<commit_message>
added hotkey for toggle sync
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="213">
   <si>
     <t>Q</t>
   </si>
@@ -667,6 +667,9 @@
   </si>
   <si>
     <t>Clip / POI 2</t>
+  </si>
+  <si>
+    <t>toggle sync</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1284,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,7 +2225,9 @@
       <c r="D23" s="1"/>
       <c r="E23" s="30"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="30"/>
+      <c r="G23" s="33" t="s">
+        <v>212</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="30"/>
       <c r="J23" s="1"/>

</xml_diff>

<commit_message>
copy to selection and fixed drawing during playback undo bug
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="217">
   <si>
     <t>Q</t>
   </si>
@@ -552,9 +552,6 @@
     <t>Ctrl Alt C</t>
   </si>
   <si>
-    <t>copy current pattern with comments</t>
-  </si>
-  <si>
     <t>copy original pattern</t>
   </si>
   <si>
@@ -673,6 +670,18 @@
   </si>
   <si>
     <t>toggle shrink</t>
+  </si>
+  <si>
+    <t>copy selection with comments</t>
+  </si>
+  <si>
+    <t>Ctrl Shift V</t>
+  </si>
+  <si>
+    <t>paste to selection</t>
+  </si>
+  <si>
+    <t>LifeViewer Keyboard Controls</t>
   </si>
 </sst>
 </file>
@@ -907,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1004,6 +1013,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1276,7 +1291,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1287,7 +1302,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,19 +1380,19 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="3"/>
@@ -1452,9 +1467,11 @@
       <c r="N5" s="1"/>
       <c r="O5" s="3"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="3"/>
+      <c r="Q5" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="R5" s="41"/>
+      <c r="S5" s="40"/>
       <c r="T5" s="1"/>
       <c r="U5" s="3"/>
       <c r="V5" s="1"/>
@@ -1511,19 +1528,19 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="5"/>
@@ -1545,7 +1562,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1652,7 +1669,7 @@
       <c r="K10" s="37"/>
       <c r="L10" s="36"/>
       <c r="M10" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37"/>
@@ -1677,43 +1694,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1928,23 +1945,23 @@
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>
       <c r="K16" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L16" s="36"/>
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -1971,7 +1988,7 @@
       <c r="M17" s="33"/>
       <c r="N17" s="39"/>
       <c r="O17" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P17" s="39"/>
       <c r="Q17" s="33"/>
@@ -2190,11 +2207,11 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
@@ -2208,7 +2225,7 @@
       <c r="Q22" s="35"/>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35"/>
@@ -2227,11 +2244,11 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="30"/>
@@ -2448,25 +2465,25 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35"/>
       <c r="N28" s="36"/>
       <c r="O28" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P28" s="36"/>
       <c r="Q28" s="35"/>
@@ -2491,7 +2508,7 @@
       <c r="E29" s="30"/>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2657,7 +2674,7 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2854,7 +2871,7 @@
         <v>170</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="5"/>
@@ -2864,14 +2881,18 @@
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="5" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
+      <c r="O38" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
@@ -2895,13 +2916,13 @@
     <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="5"/>
@@ -2911,7 +2932,7 @@
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>

</xml_diff>

<commit_message>
hotkeys to cycle paste mode and location
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="219">
   <si>
     <t>Q</t>
   </si>
@@ -682,6 +682,12 @@
   </si>
   <si>
     <t>LifeViewer Keyboard Controls</t>
+  </si>
+  <si>
+    <t>paste location</t>
+  </si>
+  <si>
+    <t>paste mode</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1297,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1302,7 +1308,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2269,7 +2275,9 @@
         <v>168</v>
       </c>
       <c r="T23" s="1"/>
-      <c r="U23" s="30"/>
+      <c r="U23" s="32" t="s">
+        <v>153</v>
+      </c>
       <c r="V23" s="1"/>
       <c r="W23" s="30"/>
       <c r="X23" s="1"/>
@@ -2315,7 +2323,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2564,7 +2572,9 @@
       <c r="N30" s="22"/>
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
-      <c r="Q30" s="21"/>
+      <c r="Q30" s="21" t="s">
+        <v>218</v>
+      </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
advance outside is now a single undo/redo step, also always uses Copy paste mode
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -694,7 +694,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,6 +733,20 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1019,11 +1033,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1297,7 +1311,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1308,7 +1322,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1375,7 +1389,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
         <v>92</v>
@@ -1440,13 +1454,15 @@
       <c r="L4" s="36"/>
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
+      <c r="O4" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
       <c r="V4" s="36"/>
       <c r="W4" s="35"/>
       <c r="X4" s="36"/>
@@ -1471,15 +1487,13 @@
       <c r="L5" s="1"/>
       <c r="M5" s="31"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="40" t="s">
-        <v>216</v>
-      </c>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="3"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
       <c r="V5" s="1"/>
       <c r="W5" s="30"/>
       <c r="X5" s="1"/>
@@ -1490,7 +1504,7 @@
       <c r="AC5" s="30"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="2:30" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="23"/>
       <c r="D6" s="22"/>
@@ -1506,13 +1520,13 @@
       <c r="L6" s="22"/>
       <c r="M6" s="23"/>
       <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
       <c r="V6" s="22"/>
       <c r="W6" s="21"/>
       <c r="X6" s="22"/>
@@ -3006,6 +3020,9 @@
       <c r="H45" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O4:U6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
fixed Generations colours, fixed switching from history to no-history Theme, AutoHide button, UI improvements
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="217">
   <si>
     <t>Q</t>
   </si>
@@ -397,12 +397,6 @@
   </si>
   <si>
     <t>previous POI</t>
-  </si>
-  <si>
-    <t>toggle hex</t>
-  </si>
-  <si>
-    <t>pattern default</t>
   </si>
   <si>
     <t>integer zoom</t>
@@ -1311,7 +1305,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1322,7 +1316,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1396,23 +1390,23 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="3"/>
@@ -1455,7 +1449,7 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P4" s="41"/>
       <c r="Q4" s="41"/>
@@ -1511,7 +1505,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="23"/>
@@ -1544,23 +1538,23 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="5"/>
@@ -1582,7 +1576,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1689,7 +1683,7 @@
       <c r="K10" s="37"/>
       <c r="L10" s="36"/>
       <c r="M10" s="38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37"/>
@@ -1714,43 +1708,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1765,7 +1759,7 @@
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
       <c r="E12" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="23" t="s">
@@ -1773,7 +1767,7 @@
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
@@ -1812,19 +1806,19 @@
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="11" t="s">
@@ -1832,23 +1826,23 @@
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="11" t="s">
@@ -1926,7 +1920,7 @@
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="10" t="s">
@@ -1965,23 +1959,23 @@
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>
       <c r="K16" s="35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L16" s="36"/>
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -2008,7 +2002,7 @@
       <c r="M17" s="33"/>
       <c r="N17" s="39"/>
       <c r="O17" s="33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="P17" s="39"/>
       <c r="Q17" s="33"/>
@@ -2029,7 +2023,7 @@
     <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
@@ -2041,29 +2035,29 @@
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L18" s="22"/>
       <c r="M18" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N18" s="22"/>
       <c r="O18" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P18" s="22"/>
       <c r="Q18" s="21"/>
       <c r="R18" s="22"/>
       <c r="S18" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T18" s="22"/>
       <c r="U18" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="V18" s="22"/>
       <c r="W18" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="21" t="s">
@@ -2080,7 +2074,7 @@
     <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="12" t="s">
@@ -2088,7 +2082,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="12" t="s">
@@ -2104,11 +2098,11 @@
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2116,7 +2110,7 @@
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="12" t="s">
@@ -2227,11 +2221,11 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
@@ -2245,7 +2239,7 @@
       <c r="Q22" s="35"/>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35"/>
@@ -2264,11 +2258,11 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="30"/>
@@ -2278,19 +2272,19 @@
       <c r="M23" s="30"/>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="30"/>
@@ -2309,7 +2303,7 @@
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="21" t="s">
@@ -2321,11 +2315,11 @@
       </c>
       <c r="L24" s="22"/>
       <c r="M24" s="21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N24" s="22"/>
       <c r="O24" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P24" s="22"/>
       <c r="Q24" s="21" t="s">
@@ -2333,11 +2327,11 @@
       </c>
       <c r="R24" s="22"/>
       <c r="S24" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2382,7 +2376,7 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="12" t="s">
@@ -2487,25 +2481,25 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35"/>
       <c r="N28" s="36"/>
       <c r="O28" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P28" s="36"/>
       <c r="Q28" s="35"/>
@@ -2530,7 +2524,7 @@
       <c r="E29" s="30"/>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2540,7 +2534,7 @@
       <c r="K29" s="30"/>
       <c r="L29" s="1"/>
       <c r="M29" s="32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="30"/>
@@ -2551,9 +2545,7 @@
       <c r="T29" s="1"/>
       <c r="U29" s="30"/>
       <c r="V29" s="1"/>
-      <c r="W29" s="32" t="s">
-        <v>157</v>
-      </c>
+      <c r="W29" s="32"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="13"/>
       <c r="Z29" s="1"/>
@@ -2571,11 +2563,11 @@
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="21" t="s">
@@ -2587,7 +2579,7 @@
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
@@ -2598,9 +2590,7 @@
         <v>101</v>
       </c>
       <c r="V30" s="22"/>
-      <c r="W30" s="21" t="s">
-        <v>123</v>
-      </c>
+      <c r="W30" s="21"/>
       <c r="X30" s="22"/>
       <c r="Y30" s="26"/>
       <c r="Z30" s="22"/>
@@ -2650,7 +2640,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="12" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="14"/>
@@ -2694,15 +2684,15 @@
     <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="15" t="s">
@@ -2739,15 +2729,15 @@
     <row r="34" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="27"/>
@@ -2767,7 +2757,7 @@
       <c r="W34" s="22"/>
       <c r="X34" s="22"/>
       <c r="Y34" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Z34" s="22"/>
       <c r="AA34" s="21" t="s">
@@ -2775,7 +2765,7 @@
       </c>
       <c r="AB34" s="22"/>
       <c r="AC34" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AD34" s="1"/>
     </row>
@@ -2889,33 +2879,33 @@
     <row r="38" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="22"/>
       <c r="O38" s="34" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
@@ -2940,23 +2930,23 @@
     <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="34" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>

</xml_diff>

<commit_message>
delete drawing state, delete [R]History states, drawing state shortcuts
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="210">
   <si>
     <t>Q</t>
   </si>
@@ -630,36 +630,6 @@
     <t>open pattern</t>
   </si>
   <si>
-    <t>Clip / POI 1</t>
-  </si>
-  <si>
-    <t>Clip 0</t>
-  </si>
-  <si>
-    <t>Clip / POI 9</t>
-  </si>
-  <si>
-    <t>Clip / POI 8</t>
-  </si>
-  <si>
-    <t>Clip / POI 7</t>
-  </si>
-  <si>
-    <t>Clip / POI 6</t>
-  </si>
-  <si>
-    <t>Clip / POI 5</t>
-  </si>
-  <si>
-    <t>Clip / POI 4</t>
-  </si>
-  <si>
-    <t>Clip / POI 3</t>
-  </si>
-  <si>
-    <t>Clip / POI 2</t>
-  </si>
-  <si>
     <t>toggle sync</t>
   </si>
   <si>
@@ -682,6 +652,15 @@
   </si>
   <si>
     <t>paste mode</t>
+  </si>
+  <si>
+    <t>pen / clip / POI</t>
+  </si>
+  <si>
+    <t>pen / clip</t>
+  </si>
+  <si>
+    <t>clear [R]History</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1284,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1316,7 +1295,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1449,7 +1428,7 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="40" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="P4" s="41"/>
       <c r="Q4" s="41"/>
@@ -1528,7 +1507,9 @@
       <c r="Z6" s="22"/>
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
-      <c r="AC6" s="21"/>
+      <c r="AC6" s="21" t="s">
+        <v>209</v>
+      </c>
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1708,11 +1689,11 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
@@ -1720,31 +1701,31 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -2258,11 +2239,11 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="30"/>
@@ -2331,7 +2312,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2579,7 +2560,7 @@
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
@@ -2895,17 +2876,17 @@
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="5" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="22"/>
       <c r="O38" s="34" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="5" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>

</xml_diff>

<commit_message>
hexagons and triangles now respect [R]History colours, [R]History COLOR commands were being ignored, toggle throttling
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="211">
   <si>
     <t>Q</t>
   </si>
@@ -661,6 +661,9 @@
   </si>
   <si>
     <t>clear [R]History</t>
+  </si>
+  <si>
+    <t>toggle throttling</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1287,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1295,7 +1298,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1943,7 +1946,9 @@
         <v>195</v>
       </c>
       <c r="L16" s="36"/>
-      <c r="M16" s="35"/>
+      <c r="M16" s="35" t="s">
+        <v>210</v>
+      </c>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
         <v>183</v>

</xml_diff>

<commit_message>
new aliases, added Throttle button, fixed HROT/LtL shrink, close Settings when changing mode
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1287,7 +1287,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1298,7 +1298,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,7 +1446,9 @@
       <c r="Z4" s="36"/>
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
-      <c r="AC4" s="35"/>
+      <c r="AC4" s="35" t="s">
+        <v>209</v>
+      </c>
       <c r="AD4" s="1"/>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.3">
@@ -1510,9 +1512,7 @@
       <c r="Z6" s="22"/>
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
-      <c r="AC6" s="21" t="s">
-        <v>209</v>
-      </c>
+      <c r="AC6" s="21"/>
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
PerfWarn button and more aliases
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="212">
   <si>
     <t>Q</t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t>toggle throttling</t>
+  </si>
+  <si>
+    <t>toggle lag warn</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1290,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1298,7 +1301,7 @@
   <dimension ref="B2:AD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,7 +2017,9 @@
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="21"/>
+      <c r="G18" s="21" t="s">
+        <v>211</v>
+      </c>
       <c r="H18" s="22"/>
       <c r="I18" s="21" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
hotkey shift+A shrinks selection
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="216">
   <si>
     <t>Q</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>advance outside</t>
+  </si>
+  <si>
+    <t>shrink selection</t>
   </si>
 </sst>
 </file>
@@ -1021,20 +1024,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1308,7 +1311,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1319,7 +1322,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF22" sqref="AF22"/>
+      <selection activeCell="AI23" sqref="AI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,15 +1454,15 @@
       <c r="L4" s="36"/>
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
       <c r="V4" s="36"/>
       <c r="W4" s="35"/>
       <c r="X4" s="36"/>
@@ -1486,13 +1489,13 @@
       <c r="L5" s="1"/>
       <c r="M5" s="31"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
       <c r="V5" s="1"/>
       <c r="W5" s="30"/>
       <c r="X5" s="1"/>
@@ -1519,13 +1522,13 @@
       <c r="L6" s="22"/>
       <c r="M6" s="23"/>
       <c r="N6" s="22"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
       <c r="V6" s="22"/>
       <c r="W6" s="21"/>
       <c r="X6" s="22"/>
@@ -2311,7 +2314,9 @@
       <c r="B24" s="1"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
-      <c r="E24" s="21"/>
+      <c r="E24" s="21" t="s">
+        <v>215</v>
+      </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
         <v>133</v>
@@ -2747,17 +2752,17 @@
       <c r="F34" s="1"/>
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="44" t="s">
+      <c r="I34" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="43"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="41"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="1"/>
@@ -2782,15 +2787,15 @@
         <v>142</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="43"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="40"/>
+      <c r="N35" s="40"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="40"/>
+      <c r="Q35" s="41"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="1"/>

</xml_diff>

<commit_message>
clear [R]History marked cells
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="220">
   <si>
     <t>Q</t>
   </si>
@@ -688,6 +688,9 @@
   </si>
   <si>
     <t>set draw state</t>
+  </si>
+  <si>
+    <t>clear marked</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1320,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1328,7 +1331,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="AC50" sqref="AC50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1509,7 +1512,9 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="30"/>
+      <c r="AC5" s="32" t="s">
+        <v>219</v>
+      </c>
       <c r="AD5" s="1"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
make START and STOP toggle buttons, fix screenshots
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="222">
   <si>
     <t>Q</t>
   </si>
@@ -691,6 +691,12 @@
   </si>
   <si>
     <t>clear marked</t>
+  </si>
+  <si>
+    <t>toggle autostart</t>
+  </si>
+  <si>
+    <t>toggle stop</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1337,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC50" sqref="AC50"/>
+      <selection activeCell="S49" sqref="S49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1999,13 +2005,9 @@
       <c r="H16" s="36"/>
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>
-      <c r="K16" s="35" t="s">
-        <v>194</v>
-      </c>
+      <c r="K16" s="35"/>
       <c r="L16" s="36"/>
-      <c r="M16" s="35" t="s">
-        <v>207</v>
-      </c>
+      <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
         <v>183</v>
@@ -2040,9 +2042,13 @@
       <c r="H17" s="38"/>
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
-      <c r="K17" s="33"/>
+      <c r="K17" s="33" t="s">
+        <v>194</v>
+      </c>
       <c r="L17" s="38"/>
-      <c r="M17" s="33"/>
+      <c r="M17" s="33" t="s">
+        <v>207</v>
+      </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
         <v>190</v>
@@ -2052,9 +2058,13 @@
       <c r="R17" s="38"/>
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
-      <c r="U17" s="33"/>
+      <c r="U17" s="33" t="s">
+        <v>220</v>
+      </c>
       <c r="V17" s="38"/>
-      <c r="W17" s="33"/>
+      <c r="W17" s="33" t="s">
+        <v>221</v>
+      </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
       <c r="Z17" s="38"/>
@@ -2547,9 +2557,7 @@
       <c r="L28" s="36"/>
       <c r="M28" s="35"/>
       <c r="N28" s="36"/>
-      <c r="O28" s="35" t="s">
-        <v>193</v>
-      </c>
+      <c r="O28" s="35"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="35"/>
       <c r="R28" s="36"/>
@@ -2586,7 +2594,9 @@
         <v>156</v>
       </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="30"/>
+      <c r="O29" s="32" t="s">
+        <v>193</v>
+      </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
       <c r="R29" s="1"/>

</xml_diff>

<commit_message>
new auto grid lines toggle
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="223">
   <si>
     <t>Q</t>
   </si>
@@ -697,6 +697,9 @@
   </si>
   <si>
     <t>toggle stop</t>
+  </si>
+  <si>
+    <t>toggle autogrid</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1337,7 +1340,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S49" sqref="S49"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2287,7 +2290,9 @@
       <c r="J22" s="36"/>
       <c r="K22" s="35"/>
       <c r="L22" s="36"/>
-      <c r="M22" s="35"/>
+      <c r="M22" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
       <c r="P22" s="36"/>

</xml_diff>

<commit_message>
reverse playback for Margolus rules
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="224">
   <si>
     <t>Q</t>
   </si>
@@ -700,6 +700,9 @@
   </si>
   <si>
     <t>toggle autogrid</t>
+  </si>
+  <si>
+    <t>toggle direction</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1332,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1340,7 +1343,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2104,7 +2107,9 @@
         <v>135</v>
       </c>
       <c r="P18" s="22"/>
-      <c r="Q18" s="21"/>
+      <c r="Q18" s="21" t="s">
+        <v>148</v>
+      </c>
       <c r="R18" s="22"/>
       <c r="S18" s="21" t="s">
         <v>127</v>
@@ -2160,7 +2165,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>148</v>
+        <v>223</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">

</xml_diff>

<commit_message>
added Alternating GridLines button, Change Rule and New Pattern now allow Bounded Grid specification
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="225">
   <si>
     <t>Q</t>
   </si>
@@ -703,6 +703,9 @@
   </si>
   <si>
     <t>toggle direction</t>
+  </si>
+  <si>
+    <t>toggle alt grid</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1335,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1343,7 +1346,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="AD51" sqref="AD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2330,7 +2333,9 @@
         <v>198</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="30"/>
+      <c r="I23" s="33" t="s">
+        <v>224</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>

</xml_diff>

<commit_message>
added oscillator and spaceship period detection, adjusted close button position, fix multi-state patterns with invalid rules displaying as two state
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="228">
   <si>
     <t>Q</t>
   </si>
@@ -709,13 +709,19 @@
   </si>
   <si>
     <t>randomize</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>toggle identify</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,13 +767,6 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1063,7 +1062,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1338,7 +1337,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1349,7 +1348,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="W42" sqref="W42"/>
+      <selection activeCell="AG51" sqref="AG51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1442,7 +1441,9 @@
         <v>176</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="3"/>
+      <c r="O3" s="8" t="s">
+        <v>226</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="1"/>
@@ -1481,11 +1482,11 @@
       <c r="L4" s="36"/>
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="42" t="s">
+      <c r="O4" s="37"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
       <c r="T4" s="43"/>
@@ -1516,8 +1517,8 @@
       <c r="L5" s="1"/>
       <c r="M5" s="31"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="1"/>
       <c r="Q5" s="43"/>
       <c r="R5" s="43"/>
       <c r="S5" s="43"/>
@@ -1551,8 +1552,8 @@
       <c r="L6" s="22"/>
       <c r="M6" s="23"/>
       <c r="N6" s="22"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="22"/>
       <c r="Q6" s="43"/>
       <c r="R6" s="43"/>
       <c r="S6" s="43"/>
@@ -1596,7 +1597,9 @@
         <v>180</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="5"/>
+      <c r="O7" s="11" t="s">
+        <v>227</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="1"/>
@@ -3224,7 +3227,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="O4:U6"/>
+    <mergeCell ref="Q4:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change PatternManager from singleton to instance
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="229">
   <si>
     <t>Q</t>
   </si>
@@ -715,6 +715,9 @@
   </si>
   <si>
     <t>toggle identify</t>
+  </si>
+  <si>
+    <t>fast identify</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1340,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1348,7 +1351,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG51" sqref="AG51"/>
+      <selection activeCell="AF48" sqref="AF48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1482,7 +1485,9 @@
       <c r="L4" s="36"/>
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
-      <c r="O4" s="37"/>
+      <c r="O4" s="37" t="s">
+        <v>228</v>
+      </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
         <v>203</v>

</xml_diff>

<commit_message>
quality render is now a toggle, added some aliases
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="230">
   <si>
     <t>Q</t>
   </si>
@@ -718,6 +718,9 @@
   </si>
   <si>
     <t>fast identify</t>
+  </si>
+  <si>
+    <t>render quality</t>
   </si>
 </sst>
 </file>
@@ -1340,7 +1343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1351,7 +1354,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF48" sqref="AF48"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2019,7 +2022,9 @@
       <c r="B16" s="1"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
-      <c r="E16" s="35"/>
+      <c r="E16" s="35" t="s">
+        <v>229</v>
+      </c>
       <c r="F16" s="36"/>
       <c r="G16" s="35"/>
       <c r="H16" s="36"/>

</xml_diff>

<commit_message>
hide select actions, fix paste mode UI, add Dying states to Generations bounding box
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="236">
   <si>
     <t>Q</t>
   </si>
@@ -733,6 +733,12 @@
   </si>
   <si>
     <t>nudge right</t>
+  </si>
+  <si>
+    <t>Ctrl Alt Z</t>
+  </si>
+  <si>
+    <t>random pattern fixed rule</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1361,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1366,7 +1372,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,9 +3095,13 @@
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
-      <c r="C41" s="3"/>
+      <c r="C41" s="34" t="s">
+        <v>234</v>
+      </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="3"/>
+      <c r="E41" s="5" t="s">
+        <v>235</v>
+      </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>

</xml_diff>

<commit_message>
added Fit Selection, remove period 1 from simplified Speed, more aliases, Evolve Selection fixes
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13335" windowHeight="5730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13332" windowHeight="5736"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="237">
   <si>
     <t>Q</t>
   </si>
@@ -192,9 +192,6 @@
     <t>zoom in</t>
   </si>
   <si>
-    <t>fit zoom</t>
-  </si>
-  <si>
     <t>rotate left</t>
   </si>
   <si>
@@ -739,6 +736,12 @@
   </si>
   <si>
     <t>random pattern fixed rule</t>
+  </si>
+  <si>
+    <t>fit pattern</t>
+  </si>
+  <si>
+    <t>fit selection</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1364,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1372,43 +1375,43 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="0.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="0.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="0.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="0.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="0.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="0.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="16" max="16" width="0.42578125" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
-    <col min="18" max="18" width="0.42578125" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="20" max="20" width="0.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15" customWidth="1"/>
-    <col min="22" max="22" width="0.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="24" max="24" width="0.42578125" customWidth="1"/>
-    <col min="25" max="25" width="15" customWidth="1"/>
-    <col min="26" max="26" width="0.42578125" customWidth="1"/>
-    <col min="27" max="27" width="15" customWidth="1"/>
-    <col min="28" max="28" width="0.42578125" customWidth="1"/>
-    <col min="29" max="29" width="15" customWidth="1"/>
-    <col min="30" max="30" width="2.7109375" customWidth="1"/>
+    <col min="1" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="0.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="0.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="0.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="10" max="10" width="0.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" customWidth="1"/>
+    <col min="12" max="12" width="0.44140625" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" customWidth="1"/>
+    <col min="14" max="14" width="0.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" customWidth="1"/>
+    <col min="16" max="16" width="0.44140625" customWidth="1"/>
+    <col min="17" max="17" width="13.77734375" customWidth="1"/>
+    <col min="18" max="18" width="0.44140625" customWidth="1"/>
+    <col min="19" max="19" width="13.77734375" customWidth="1"/>
+    <col min="20" max="20" width="0.44140625" customWidth="1"/>
+    <col min="21" max="21" width="13.77734375" customWidth="1"/>
+    <col min="22" max="22" width="0.44140625" customWidth="1"/>
+    <col min="23" max="23" width="13.77734375" customWidth="1"/>
+    <col min="24" max="24" width="0.44140625" customWidth="1"/>
+    <col min="25" max="25" width="13.77734375" customWidth="1"/>
+    <col min="26" max="26" width="0.44140625" customWidth="1"/>
+    <col min="27" max="27" width="13.77734375" customWidth="1"/>
+    <col min="28" max="28" width="0.44140625" customWidth="1"/>
+    <col min="29" max="29" width="13.77734375" customWidth="1"/>
+    <col min="30" max="30" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" ht="14.65" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:30" ht="14.7" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1439,34 +1442,34 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
@@ -1476,23 +1479,23 @@
       <c r="U3" s="3"/>
       <c r="V3" s="1"/>
       <c r="W3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="37"/>
       <c r="D4" s="36"/>
@@ -1507,11 +1510,11 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
@@ -1525,11 +1528,11 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="31"/>
       <c r="D5" s="1"/>
@@ -1558,18 +1561,18 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="23"/>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="23"/>
@@ -1593,38 +1596,38 @@
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
@@ -1634,21 +1637,21 @@
       <c r="U7" s="5"/>
       <c r="V7" s="1"/>
       <c r="W7" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1679,10 +1682,10 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="8" t="s">
@@ -1734,52 +1737,52 @@
       </c>
       <c r="AB9" s="1"/>
       <c r="AC9" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P10" s="36"/>
       <c r="Q10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R10" s="36"/>
       <c r="S10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T10" s="36"/>
       <c r="U10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V10" s="36"/>
       <c r="W10" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="37"/>
@@ -1789,48 +1792,48 @@
       <c r="AC10" s="35"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1840,38 +1843,38 @@
       <c r="AC11" s="30"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="2:30" ht="14.65" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:30" ht="14.7" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
       <c r="E12" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P12" s="22"/>
       <c r="Q12" s="23"/>
       <c r="R12" s="22"/>
       <c r="S12" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T12" s="22"/>
       <c r="U12" s="23"/>
@@ -1879,58 +1882,58 @@
       <c r="W12" s="23"/>
       <c r="X12" s="22"/>
       <c r="Y12" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Z12" s="22"/>
       <c r="AA12" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AB12" s="22"/>
       <c r="AC12" s="21"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="2:30" ht="14.65" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:30" ht="14.7" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="11" t="s">
@@ -1942,11 +1945,11 @@
       </c>
       <c r="AB13" s="1"/>
       <c r="AC13" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1977,10 +1980,10 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="10" t="s">
@@ -2008,7 +2011,7 @@
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="10" t="s">
@@ -2036,12 +2039,12 @@
       </c>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="35"/>
@@ -2055,17 +2058,17 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -2077,7 +2080,7 @@
       <c r="AC16" s="35"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="33"/>
       <c r="D17" s="38"/>
@@ -2088,15 +2091,15 @@
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
       <c r="K17" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="33"/>
@@ -2104,11 +2107,11 @@
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
       <c r="U17" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="V17" s="38"/>
       <c r="W17" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
@@ -2118,77 +2121,77 @@
       <c r="AC17" s="33"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="2:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L18" s="22"/>
       <c r="M18" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N18" s="22"/>
       <c r="O18" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P18" s="22"/>
       <c r="Q18" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R18" s="22"/>
       <c r="S18" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T18" s="22"/>
       <c r="U18" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="V18" s="22"/>
       <c r="W18" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z18" s="22"/>
       <c r="AA18" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB18" s="22"/>
       <c r="AC18" s="21"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="12" t="s">
@@ -2196,27 +2199,27 @@
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="X19" s="1"/>
       <c r="Y19" s="12" t="s">
@@ -2228,11 +2231,11 @@
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2263,7 +2266,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
@@ -2318,24 +2321,26 @@
       <c r="AC21" s="4"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
       <c r="J22" s="36"/>
-      <c r="K22" s="35"/>
+      <c r="K22" s="35" t="s">
+        <v>236</v>
+      </c>
       <c r="L22" s="36"/>
       <c r="M22" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
@@ -2343,7 +2348,7 @@
       <c r="Q22" s="35"/>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35"/>
@@ -2357,42 +2362,42 @@
       <c r="AC22" s="4"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>
       <c r="M23" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="30"/>
@@ -2404,44 +2409,44 @@
       <c r="AC23" s="4"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J24" s="22"/>
       <c r="K24" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L24" s="22"/>
       <c r="M24" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N24" s="22"/>
       <c r="O24" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P24" s="22"/>
       <c r="Q24" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R24" s="22"/>
       <c r="S24" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2453,44 +2458,44 @@
       <c r="AC24" s="25"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="5"/>
       <c r="D25" s="1"/>
       <c r="E25" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="12" t="s">
-        <v>53</v>
+        <v>235</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V25" s="1"/>
       <c r="W25" s="12"/>
@@ -2502,7 +2507,7 @@
       <c r="AC25" s="7"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2533,10 +2538,10 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="10" t="s">
@@ -2586,24 +2591,24 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35"/>
@@ -2625,30 +2630,30 @@
       <c r="AC28" s="3"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="30"/>
       <c r="D29" s="1"/>
       <c r="E29" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="30"/>
       <c r="L29" s="1"/>
       <c r="M29" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
@@ -2666,24 +2671,24 @@
       <c r="AC29" s="3"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="21"/>
       <c r="D30" s="22"/>
       <c r="E30" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="21"/>
@@ -2691,15 +2696,15 @@
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T30" s="22"/>
       <c r="U30" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V30" s="22"/>
       <c r="W30" s="21"/>
@@ -2711,7 +2716,7 @@
       <c r="AC30" s="22"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="6"/>
       <c r="D31" s="1"/>
@@ -2720,39 +2725,39 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T31" s="1"/>
       <c r="U31" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="14"/>
@@ -2762,7 +2767,7 @@
       <c r="AC31" s="5"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2793,18 +2798,18 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="15" t="s">
@@ -2826,30 +2831,30 @@
       <c r="W33" s="3"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z33" s="1"/>
       <c r="AA33" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AB33" s="1"/>
       <c r="AC33" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="30"/>
       <c r="D34" s="1"/>
       <c r="E34" s="35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
       <c r="I34" s="41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -2873,14 +2878,14 @@
       <c r="AC34" s="30"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="30"/>
       <c r="D35" s="1"/>
       <c r="E35" s="35"/>
       <c r="F35" s="1"/>
       <c r="G35" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="41"/>
@@ -2902,16 +2907,16 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="30"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="35"/>
@@ -2919,7 +2924,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="22"/>
       <c r="I36" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
@@ -2937,19 +2942,19 @@
       <c r="W36" s="22"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z36" s="22"/>
       <c r="AA36" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AB36" s="22"/>
       <c r="AC36" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="12"/>
       <c r="D37" s="1"/>
@@ -2958,7 +2963,7 @@
       <c r="G37" s="12"/>
       <c r="H37" s="1"/>
       <c r="I37" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
@@ -2976,19 +2981,19 @@
       <c r="W37" s="5"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z37" s="1"/>
       <c r="AA37" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB37" s="1"/>
       <c r="AC37" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -3019,7 +3024,7 @@
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1"/>
@@ -3044,19 +3049,19 @@
       <c r="W39" s="3"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z39" s="1"/>
       <c r="AA39" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB39" s="1"/>
       <c r="AC39" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="1"/>
@@ -3081,26 +3086,26 @@
       <c r="W40" s="3"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Z40" s="1"/>
       <c r="AA40" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AB40" s="1"/>
       <c r="AC40" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
@@ -3128,36 +3133,36 @@
       <c r="AC41" s="30"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
@@ -3167,48 +3172,48 @@
       <c r="W42" s="22"/>
       <c r="X42" s="22"/>
       <c r="Y42" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z42" s="22"/>
       <c r="AA42" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB42" s="22"/>
       <c r="AC42" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="5"/>
       <c r="O43" s="34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
@@ -3218,19 +3223,19 @@
       <c r="W43" s="5"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Z43" s="1"/>
       <c r="AA43" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB43" s="1"/>
       <c r="AC43" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -3261,7 +3266,7 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>

</xml_diff>

<commit_message>
added [[ RANDOMIZE ]] command, attempted to fix ignored touch events on iPad
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82FABF8-1C62-4CCE-A9FE-6951663DB212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13332" windowHeight="5736"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="238">
   <si>
     <t>Q</t>
   </si>
@@ -742,12 +748,15 @@
   </si>
   <si>
     <t>fit selection</t>
+  </si>
+  <si>
+    <t>center pattern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1364,18 +1373,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+      <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1843,7 +1852,7 @@
       <c r="AC11" s="30"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="2:30" ht="14.7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
@@ -1892,7 +1901,7 @@
       <c r="AC12" s="21"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="2:30" ht="14.7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
@@ -2615,7 +2624,9 @@
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>
-      <c r="Q28" s="35"/>
+      <c r="Q28" s="35" t="s">
+        <v>237</v>
+      </c>
       <c r="R28" s="36"/>
       <c r="S28" s="35"/>
       <c r="T28" s="36"/>

</xml_diff>

<commit_message>
added Tripod, Triangular Inner and Triangular Outer
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82FABF8-1C62-4CCE-A9FE-6951663DB212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA549AE-920C-46EE-BD94-695FB01B9C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="240">
   <si>
     <t>Q</t>
   </si>
@@ -751,6 +751,12 @@
   </si>
   <si>
     <t>center pattern</t>
+  </si>
+  <si>
+    <t>Ctrl Shift O</t>
+  </si>
+  <si>
+    <t>open clipboard as pattern</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1390,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W49" sqref="W49"/>
+      <selection activeCell="AE50" sqref="AE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3121,9 +3127,13 @@
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="I41" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="J41" s="1"/>
+      <c r="K41" s="5" t="s">
+        <v>201</v>
+      </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -3169,11 +3179,11 @@
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>

</xml_diff>

<commit_message>
ctrl-b create CoordCA neighbourhood string from selection, allow hex postfix for Custom neighbourhoods
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA549AE-920C-46EE-BD94-695FB01B9C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA4150B-EBE6-440A-BABB-112530965567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="4104" windowWidth="24600" windowHeight="10668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="241">
   <si>
     <t>Q</t>
   </si>
@@ -757,6 +757,9 @@
   </si>
   <si>
     <t>open clipboard as pattern</t>
+  </si>
+  <si>
+    <t>copy CoordCA</t>
   </si>
 </sst>
 </file>
@@ -1389,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE50" sqref="AE50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2626,7 +2629,9 @@
         <v>185</v>
       </c>
       <c r="L28" s="36"/>
-      <c r="M28" s="35"/>
+      <c r="M28" s="35" t="s">
+        <v>240</v>
+      </c>
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>

</xml_diff>

<commit_message>
added toggle for rainbow mode, rainbow now works with layers
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA4150B-EBE6-440A-BABB-112530965567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BE8B62-B542-495F-9EAE-9053794DB09B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="4104" windowWidth="24600" windowHeight="10668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="242">
   <si>
     <t>Q</t>
   </si>
@@ -759,7 +759,10 @@
     <t>open clipboard as pattern</t>
   </si>
   <si>
-    <t>copy CoordCA</t>
+    <t>copy nbrhood</t>
+  </si>
+  <si>
+    <t>toggle rainbow</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH49" sqref="AH49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2065,7 +2068,9 @@
         <v>228</v>
       </c>
       <c r="F16" s="36"/>
-      <c r="G16" s="35"/>
+      <c r="G16" s="35" t="s">
+        <v>241</v>
+      </c>
       <c r="H16" s="36"/>
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>

</xml_diff>

<commit_message>
fixed broken 8 bit rules and a couple of tests
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BE8B62-B542-495F-9EAE-9053794DB09B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F462D8-7DD3-4DCF-A745-BFC0D92EB84B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,12 +528,6 @@
     <t>zoom 8x</t>
   </si>
   <si>
-    <t>[R]History on</t>
-  </si>
-  <si>
-    <t>[R]History off</t>
-  </si>
-  <si>
     <t>toggle glider kill</t>
   </si>
   <si>
@@ -763,6 +757,12 @@
   </si>
   <si>
     <t>toggle rainbow</t>
+  </si>
+  <si>
+    <t>[R] cells off</t>
+  </si>
+  <si>
+    <t>[R] cells on</t>
   </si>
 </sst>
 </file>
@@ -1396,7 +1396,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH49" sqref="AH49"/>
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,23 +1474,23 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
@@ -1531,11 +1531,11 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
@@ -1549,7 +1549,7 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1582,7 +1582,7 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1617,7 +1617,7 @@
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
@@ -1632,23 +1632,23 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
@@ -1668,7 +1668,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1767,43 +1767,43 @@
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P10" s="36"/>
       <c r="Q10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="R10" s="36"/>
       <c r="S10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="T10" s="36"/>
       <c r="U10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="V10" s="36"/>
       <c r="W10" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="37"/>
@@ -1818,43 +1818,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="23" t="s">
@@ -2065,11 +2065,11 @@
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="35" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H16" s="36"/>
       <c r="I16" s="35"/>
@@ -2081,17 +2081,17 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -2114,15 +2114,15 @@
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
       <c r="K17" s="33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="33"/>
@@ -2130,11 +2130,11 @@
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
       <c r="U17" s="33" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="V17" s="38"/>
       <c r="W17" s="33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
@@ -2153,7 +2153,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="21" t="s">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2349,21 +2349,21 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
       <c r="J22" s="36"/>
       <c r="K22" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L22" s="36"/>
       <c r="M22" s="35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
@@ -2371,7 +2371,7 @@
       <c r="Q22" s="35"/>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35"/>
@@ -2390,33 +2390,33 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>
       <c r="M23" s="32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>163</v>
+        <v>241</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>164</v>
+        <v>240</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
@@ -2437,7 +2437,7 @@
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2498,7 +2498,7 @@
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="12" t="s">
@@ -2619,29 +2619,29 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R28" s="36"/>
       <c r="S28" s="35"/>
@@ -2662,11 +2662,11 @@
       <c r="C29" s="30"/>
       <c r="D29" s="1"/>
       <c r="E29" s="32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2680,7 +2680,7 @@
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
@@ -2723,7 +2723,7 @@
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
@@ -2832,7 +2832,7 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2881,7 +2881,7 @@
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
       <c r="I34" s="41" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -2934,7 +2934,7 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="30"/>
@@ -2951,7 +2951,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="22"/>
       <c r="I36" s="27" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
@@ -3113,36 +3113,36 @@
       <c r="W40" s="3"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Z40" s="1"/>
       <c r="AA40" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AB40" s="1"/>
       <c r="AC40" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AD40" s="1"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="34" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="34" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3167,33 +3167,33 @@
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
@@ -3218,33 +3218,33 @@
     <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="5"/>
       <c r="O43" s="34" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>

</xml_diff>

<commit_message>
fixed tiling issue with RuleTable rules
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F462D8-7DD3-4DCF-A745-BFC0D92EB84B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1EDEBA-A5FD-4180-95F0-73DA6F27C6F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="243">
   <si>
     <t>Q</t>
   </si>
@@ -528,9 +528,6 @@
     <t>zoom 8x</t>
   </si>
   <si>
-    <t>toggle glider kill</t>
-  </si>
-  <si>
     <t>Ctrl Shift Z</t>
   </si>
   <si>
@@ -759,10 +756,16 @@
     <t>toggle rainbow</t>
   </si>
   <si>
-    <t>[R] cells off</t>
-  </si>
-  <si>
-    <t>[R] cells on</t>
+    <t>toggle kill gliders</t>
+  </si>
+  <si>
+    <t>[R]Super</t>
+  </si>
+  <si>
+    <t>[R]History</t>
+  </si>
+  <si>
+    <t>[R] Standard</t>
   </si>
 </sst>
 </file>
@@ -1396,7 +1399,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,23 +1477,23 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
@@ -1531,11 +1534,11 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
@@ -1549,7 +1552,7 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1582,7 +1585,7 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1617,7 +1620,7 @@
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
@@ -1632,23 +1635,23 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
@@ -1668,7 +1671,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1767,43 +1770,43 @@
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P10" s="36"/>
       <c r="Q10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="R10" s="36"/>
       <c r="S10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T10" s="36"/>
       <c r="U10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V10" s="36"/>
       <c r="W10" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="37"/>
@@ -1818,43 +1821,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1885,7 +1888,7 @@
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="23" t="s">
@@ -2065,11 +2068,11 @@
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H16" s="36"/>
       <c r="I16" s="35"/>
@@ -2081,17 +2084,17 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -2114,15 +2117,15 @@
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
       <c r="K17" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="33"/>
@@ -2130,11 +2133,11 @@
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
       <c r="U17" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="V17" s="38"/>
       <c r="W17" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
@@ -2153,7 +2156,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="21" t="s">
@@ -2230,7 +2233,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2349,21 +2352,21 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
       <c r="J22" s="36"/>
       <c r="K22" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L22" s="36"/>
       <c r="M22" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
@@ -2371,10 +2374,12 @@
       <c r="Q22" s="35"/>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T22" s="36"/>
-      <c r="U22" s="35"/>
+      <c r="U22" s="35" t="s">
+        <v>239</v>
+      </c>
       <c r="V22" s="36"/>
       <c r="W22" s="35"/>
       <c r="X22" s="36"/>
@@ -2390,21 +2395,21 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>
       <c r="M23" s="32" t="s">
-        <v>163</v>
+        <v>240</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
@@ -2412,11 +2417,11 @@
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
@@ -2437,7 +2442,7 @@
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
@@ -2469,7 +2474,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2498,7 +2503,7 @@
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="12" t="s">
@@ -2619,29 +2624,29 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R28" s="36"/>
       <c r="S28" s="35"/>
@@ -2662,11 +2667,11 @@
       <c r="C29" s="30"/>
       <c r="D29" s="1"/>
       <c r="E29" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2680,7 +2685,7 @@
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
@@ -2723,7 +2728,7 @@
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
@@ -2832,7 +2837,7 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2881,7 +2886,7 @@
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
       <c r="I34" s="41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -2934,7 +2939,7 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="30"/>
@@ -2951,7 +2956,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="22"/>
       <c r="I36" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
@@ -3113,36 +3118,36 @@
       <c r="W40" s="3"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z40" s="1"/>
       <c r="AA40" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AB40" s="1"/>
       <c r="AC40" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AD40" s="1"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3167,33 +3172,33 @@
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
@@ -3218,33 +3223,33 @@
     <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="5"/>
       <c r="O43" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>

</xml_diff>

<commit_message>
copy rule definition, POIADDLABELS, AGESTATES
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1EDEBA-A5FD-4180-95F0-73DA6F27C6F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8238C21-E4F8-4847-B80C-B1FD062ADC23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="244">
   <si>
     <t>Q</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>[R] Standard</t>
+  </si>
+  <si>
+    <t>copy rule</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1402,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2371,7 +2374,9 @@
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
       <c r="P22" s="36"/>
-      <c r="Q22" s="35"/>
+      <c r="Q22" s="35" t="s">
+        <v>243</v>
+      </c>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
         <v>184</v>

</xml_diff>

<commit_message>
improved [[ KILLGLIDERS ]]
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8238C21-E4F8-4847-B80C-B1FD062ADC23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ECC4D7-6C89-4477-8A8E-2902176A2774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,9 +501,6 @@
     <t>toggle drawing</t>
   </si>
   <si>
-    <t>toggle hexagon</t>
-  </si>
-  <si>
     <t>cell borders</t>
   </si>
   <si>
@@ -765,10 +762,13 @@
     <t>[R]History</t>
   </si>
   <si>
-    <t>[R] Standard</t>
-  </si>
-  <si>
     <t>copy rule</t>
+  </si>
+  <si>
+    <t>toggle cell type</t>
+  </si>
+  <si>
+    <t>[R]Standard</t>
   </si>
 </sst>
 </file>
@@ -1402,7 +1402,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,23 +1480,23 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
@@ -1537,11 +1537,11 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
@@ -1555,7 +1555,7 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1588,7 +1588,7 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1623,7 +1623,7 @@
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
@@ -1638,23 +1638,23 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
@@ -1674,7 +1674,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1773,43 +1773,43 @@
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P10" s="36"/>
       <c r="Q10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R10" s="36"/>
       <c r="S10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="T10" s="36"/>
       <c r="U10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V10" s="36"/>
       <c r="W10" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="37"/>
@@ -1824,43 +1824,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="23" t="s">
@@ -1924,19 +1924,19 @@
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="11" t="s">
@@ -1944,7 +1944,7 @@
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11" t="s">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="11" t="s">
@@ -2071,11 +2071,11 @@
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H16" s="36"/>
       <c r="I16" s="35"/>
@@ -2087,17 +2087,17 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -2120,15 +2120,15 @@
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
       <c r="K17" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="33"/>
@@ -2136,11 +2136,11 @@
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
       <c r="U17" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V17" s="38"/>
       <c r="W17" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
@@ -2159,7 +2159,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="21" t="s">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2355,35 +2355,35 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
       <c r="J22" s="36"/>
       <c r="K22" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L22" s="36"/>
       <c r="M22" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
       <c r="P22" s="36"/>
       <c r="Q22" s="35" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="V22" s="36"/>
       <c r="W22" s="35"/>
@@ -2400,33 +2400,33 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>
       <c r="M23" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
@@ -2447,7 +2447,7 @@
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2508,7 +2508,7 @@
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="12" t="s">
@@ -2629,29 +2629,29 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R28" s="36"/>
       <c r="S28" s="35"/>
@@ -2672,11 +2672,11 @@
       <c r="C29" s="30"/>
       <c r="D29" s="1"/>
       <c r="E29" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2686,11 +2686,11 @@
       <c r="K29" s="30"/>
       <c r="L29" s="1"/>
       <c r="M29" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
@@ -2733,7 +2733,7 @@
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="12" t="s">
-        <v>154</v>
+        <v>242</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="14"/>
@@ -2842,7 +2842,7 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2891,7 +2891,7 @@
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
       <c r="I34" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -2944,7 +2944,7 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="30"/>
@@ -2961,7 +2961,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="22"/>
       <c r="I36" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
@@ -3123,36 +3123,36 @@
       <c r="W40" s="3"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Z40" s="1"/>
       <c r="AA40" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AB40" s="1"/>
       <c r="AC40" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AD40" s="1"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3177,33 +3177,33 @@
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
@@ -3228,33 +3228,33 @@
     <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="5"/>
       <c r="O43" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>

</xml_diff>

<commit_message>
fixed an issue with HROT Weighted neighborhoods and negative counts
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ECC4D7-6C89-4477-8A8E-2902176A2774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5784C1A5-0F34-4FD9-AE4F-FA5413F8C4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,9 +408,6 @@
     <t>toggle gen</t>
   </si>
   <si>
-    <t>loop / track</t>
-  </si>
-  <si>
     <t>reset all</t>
   </si>
   <si>
@@ -769,6 +766,9 @@
   </si>
   <si>
     <t>[R]Standard</t>
+  </si>
+  <si>
+    <t>toggle loop/wp</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -1476,27 +1476,27 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
@@ -1537,11 +1537,11 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
@@ -1555,7 +1555,7 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1588,7 +1588,7 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1599,7 +1599,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="23"/>
@@ -1623,7 +1623,7 @@
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
@@ -1634,27 +1634,27 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
@@ -1674,7 +1674,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1773,43 +1773,43 @@
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P10" s="36"/>
       <c r="Q10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R10" s="36"/>
       <c r="S10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T10" s="36"/>
       <c r="U10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V10" s="36"/>
       <c r="W10" s="37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="37"/>
@@ -1824,43 +1824,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="23" t="s">
@@ -1924,19 +1924,19 @@
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="11" t="s">
@@ -1944,23 +1944,23 @@
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="11" t="s">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="10" t="s">
@@ -2071,12 +2071,10 @@
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F16" s="36"/>
-      <c r="G16" s="35" t="s">
-        <v>237</v>
-      </c>
+      <c r="G16" s="35"/>
       <c r="H16" s="36"/>
       <c r="I16" s="35"/>
       <c r="J16" s="36"/>
@@ -2087,17 +2085,17 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35"/>
@@ -2115,20 +2113,22 @@
       <c r="D17" s="38"/>
       <c r="E17" s="33"/>
       <c r="F17" s="38"/>
-      <c r="G17" s="33"/>
+      <c r="G17" s="32" t="s">
+        <v>236</v>
+      </c>
       <c r="H17" s="38"/>
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
       <c r="K17" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="33"/>
@@ -2136,11 +2136,11 @@
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
       <c r="U17" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V17" s="38"/>
       <c r="W17" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
@@ -2153,13 +2153,13 @@
     <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="21" t="s">
@@ -2167,31 +2167,31 @@
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L18" s="22"/>
       <c r="M18" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N18" s="22"/>
       <c r="O18" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P18" s="22"/>
       <c r="Q18" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R18" s="22"/>
       <c r="S18" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T18" s="22"/>
       <c r="U18" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="V18" s="22"/>
       <c r="W18" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="21" t="s">
@@ -2208,7 +2208,7 @@
     <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="12" t="s">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>123</v>
+        <v>243</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="12" t="s">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="12" t="s">
@@ -2355,35 +2355,35 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35"/>
       <c r="J22" s="36"/>
       <c r="K22" s="35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L22" s="36"/>
       <c r="M22" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
       <c r="P22" s="36"/>
       <c r="Q22" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="V22" s="36"/>
       <c r="W22" s="35"/>
@@ -2400,37 +2400,37 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>
       <c r="M23" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="30"/>
@@ -2447,11 +2447,11 @@
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="21" t="s">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="N24" s="22"/>
       <c r="O24" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P24" s="22"/>
       <c r="Q24" s="21" t="s">
@@ -2475,11 +2475,11 @@
       </c>
       <c r="R24" s="22"/>
       <c r="S24" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2508,7 +2508,7 @@
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="12" t="s">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="12" t="s">
@@ -2629,29 +2629,29 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="R28" s="36"/>
       <c r="S28" s="35"/>
@@ -2672,11 +2672,11 @@
       <c r="C29" s="30"/>
       <c r="D29" s="1"/>
       <c r="E29" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2686,11 +2686,11 @@
       <c r="K29" s="30"/>
       <c r="L29" s="1"/>
       <c r="M29" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
@@ -2717,11 +2717,11 @@
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="21" t="s">
@@ -2733,7 +2733,7 @@
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="14"/>
@@ -2838,15 +2838,15 @@
     <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="15" t="s">
@@ -2885,13 +2885,13 @@
       <c r="C34" s="30"/>
       <c r="D34" s="1"/>
       <c r="E34" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
       <c r="I34" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -2922,7 +2922,7 @@
       <c r="E35" s="35"/>
       <c r="F35" s="1"/>
       <c r="G35" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="41"/>
@@ -2944,7 +2944,7 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="30"/>
@@ -2953,7 +2953,7 @@
     <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="35"/>
@@ -2961,7 +2961,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="22"/>
       <c r="I36" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
@@ -2979,7 +2979,7 @@
       <c r="W36" s="22"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Z36" s="22"/>
       <c r="AA36" s="21" t="s">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="AB36" s="22"/>
       <c r="AC36" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AD36" s="1"/>
     </row>
@@ -3123,36 +3123,36 @@
       <c r="W40" s="3"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z40" s="1"/>
       <c r="AA40" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AB40" s="1"/>
       <c r="AC40" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AD40" s="1"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3177,33 +3177,33 @@
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
@@ -3228,33 +3228,33 @@
     <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>191</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="5"/>
       <c r="O43" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>

</xml_diff>

<commit_message>
added colours to hotkeys in tooltips and a few new hotkeys
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5784C1A5-0F34-4FD9-AE4F-FA5413F8C4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC686046-B7DB-4FC7-B9A3-211A04C65546}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="247">
   <si>
     <t>Q</t>
   </si>
@@ -769,6 +769,15 @@
   </si>
   <si>
     <t>toggle loop/wp</t>
+  </si>
+  <si>
+    <t>autohide UI</t>
+  </si>
+  <si>
+    <t>toggle states</t>
+  </si>
+  <si>
+    <t>drawing pause</t>
   </si>
 </sst>
 </file>
@@ -1401,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y51" sqref="Y51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2098,7 +2107,9 @@
         <v>191</v>
       </c>
       <c r="V16" s="36"/>
-      <c r="W16" s="35"/>
+      <c r="W16" s="35" t="s">
+        <v>246</v>
+      </c>
       <c r="X16" s="36"/>
       <c r="Y16" s="35"/>
       <c r="Z16" s="36"/>
@@ -2131,7 +2142,9 @@
         <v>184</v>
       </c>
       <c r="P17" s="38"/>
-      <c r="Q17" s="33"/>
+      <c r="Q17" s="33" t="s">
+        <v>244</v>
+      </c>
       <c r="R17" s="38"/>
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
@@ -2362,7 +2375,9 @@
         <v>166</v>
       </c>
       <c r="H22" s="36"/>
-      <c r="I22" s="35"/>
+      <c r="I22" s="35" t="s">
+        <v>245</v>
+      </c>
       <c r="J22" s="36"/>
       <c r="K22" s="35" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
added save image buttons, experimental touch focus removal
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC686046-B7DB-4FC7-B9A3-211A04C65546}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC6FA32-57AC-4B36-8766-A2B1A5686756}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="248">
   <si>
     <t>Q</t>
   </si>
@@ -778,6 +778,9 @@
   </si>
   <si>
     <t>drawing pause</t>
+  </si>
+  <si>
+    <t>toggle clip list</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1414,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y51" sqref="Y51"/>
+      <selection activeCell="AD47" sqref="AD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2743,7 +2746,9 @@
         <v>115</v>
       </c>
       <c r="L30" s="22"/>
-      <c r="M30" s="21"/>
+      <c r="M30" s="21" t="s">
+        <v>247</v>
+      </c>
       <c r="N30" s="22"/>
       <c r="O30" s="21"/>
       <c r="P30" s="22"/>

</xml_diff>

<commit_message>
[R]History snapshots, [[ STARTFROM ]], Go To Gen command
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC6FA32-57AC-4B36-8766-A2B1A5686756}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7063D0-1E26-423B-8298-D2FA90CAA44E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="249">
   <si>
     <t>Q</t>
   </si>
@@ -781,6 +781,9 @@
   </si>
   <si>
     <t>toggle clip list</t>
+  </si>
+  <si>
+    <t>go to generation</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1417,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD47" sqref="AD47"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2750,7 +2753,9 @@
         <v>247</v>
       </c>
       <c r="N30" s="22"/>
-      <c r="O30" s="21"/>
+      <c r="O30" s="21" t="s">
+        <v>248</v>
+      </c>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
added experimental camera tilt
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7063D0-1E26-423B-8298-D2FA90CAA44E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B69556E-233D-4AD5-AFB4-1A6715BD0963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="252">
   <si>
     <t>Q</t>
   </si>
@@ -784,6 +784,15 @@
   </si>
   <si>
     <t>go to generation</t>
+  </si>
+  <si>
+    <t>tilt down</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>tilt up</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1426,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="X52" sqref="X52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2554,7 +2563,9 @@
       <c r="V25" s="1"/>
       <c r="W25" s="12"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="12"/>
+      <c r="Y25" s="12" t="s">
+        <v>249</v>
+      </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="12"/>
       <c r="AB25" s="1"/>
@@ -2769,7 +2780,9 @@
         <v>100</v>
       </c>
       <c r="V30" s="22"/>
-      <c r="W30" s="21"/>
+      <c r="W30" s="21" t="s">
+        <v>241</v>
+      </c>
       <c r="X30" s="22"/>
       <c r="Y30" s="26"/>
       <c r="Z30" s="22"/>
@@ -2819,7 +2832,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="12" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="14"/>
@@ -2851,7 +2864,9 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
+      <c r="W32" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
@@ -3147,17 +3162,11 @@
       <c r="V40" s="1"/>
       <c r="W40" s="3"/>
       <c r="X40" s="1"/>
-      <c r="Y40" s="33" t="s">
-        <v>224</v>
-      </c>
+      <c r="Y40" s="33"/>
       <c r="Z40" s="1"/>
-      <c r="AA40" s="33" t="s">
-        <v>226</v>
-      </c>
+      <c r="AA40" s="33"/>
       <c r="AB40" s="1"/>
-      <c r="AC40" s="33" t="s">
-        <v>227</v>
-      </c>
+      <c r="AC40" s="33"/>
       <c r="AD40" s="1"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
@@ -3192,11 +3201,17 @@
       <c r="V41" s="1"/>
       <c r="W41" s="3"/>
       <c r="X41" s="1"/>
-      <c r="Y41" s="30"/>
+      <c r="Y41" s="33" t="s">
+        <v>224</v>
+      </c>
       <c r="Z41" s="1"/>
-      <c r="AA41" s="30"/>
+      <c r="AA41" s="33" t="s">
+        <v>226</v>
+      </c>
       <c r="AB41" s="1"/>
-      <c r="AC41" s="30"/>
+      <c r="AC41" s="33" t="s">
+        <v>227</v>
+      </c>
       <c r="AD41" s="1"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix GPS specification for STEP of 1x, don't jump to Script Help when Help opened and there are script errors
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B69556E-233D-4AD5-AFB4-1A6715BD0963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0B378-0075-4455-894F-B0E26535A3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="248">
   <si>
     <t>Q</t>
   </si>
@@ -261,12 +261,6 @@
     <t>`    ¬</t>
   </si>
   <si>
-    <t>step size up</t>
-  </si>
-  <si>
-    <t>step size down</t>
-  </si>
-  <si>
     <t>toggle menu</t>
   </si>
   <si>
@@ -325,12 +319,6 @@
   </si>
   <si>
     <t>play / pause</t>
-  </si>
-  <si>
-    <t>max step size</t>
-  </si>
-  <si>
-    <t>min step size</t>
   </si>
   <si>
     <t>toggle autofit</t>
@@ -1426,7 +1414,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X52" sqref="X52"/>
+      <selection activeCell="AI39" sqref="AI39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1496,31 +1484,31 @@
     <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
@@ -1530,19 +1518,19 @@
       <c r="U3" s="3"/>
       <c r="V3" s="1"/>
       <c r="W3" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AD3" s="1"/>
     </row>
@@ -1561,11 +1549,11 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="37" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
@@ -1579,7 +1567,7 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="35" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1612,7 +1600,7 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="32" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1623,7 +1611,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="22"/>
       <c r="G6" s="23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="23"/>
@@ -1647,38 +1635,38 @@
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="21" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
@@ -1688,17 +1676,17 @@
       <c r="U7" s="5"/>
       <c r="V7" s="1"/>
       <c r="W7" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1788,7 +1776,7 @@
       </c>
       <c r="AB9" s="1"/>
       <c r="AC9" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AD9" s="1"/>
     </row>
@@ -1797,43 +1785,43 @@
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="P10" s="36"/>
       <c r="Q10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="R10" s="36"/>
       <c r="S10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="T10" s="36"/>
       <c r="U10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="V10" s="36"/>
       <c r="W10" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="37"/>
@@ -1848,43 +1836,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1899,33 +1887,33 @@
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
       <c r="E12" s="23" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="24" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="P12" s="22"/>
       <c r="Q12" s="23"/>
       <c r="R12" s="22"/>
       <c r="S12" s="23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="T12" s="22"/>
       <c r="U12" s="23"/>
@@ -1933,11 +1921,11 @@
       <c r="W12" s="23"/>
       <c r="X12" s="22"/>
       <c r="Y12" s="23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Z12" s="22"/>
       <c r="AA12" s="23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AB12" s="22"/>
       <c r="AC12" s="21"/>
@@ -1948,43 +1936,43 @@
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="11" t="s">
@@ -1996,7 +1984,7 @@
       </c>
       <c r="AB13" s="1"/>
       <c r="AC13" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="AD13" s="1"/>
     </row>
@@ -2034,7 +2022,7 @@
     <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="10" t="s">
@@ -2062,7 +2050,7 @@
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="10" t="s">
@@ -2095,7 +2083,7 @@
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="35" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="35"/>
@@ -2109,21 +2097,21 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="X16" s="36"/>
       <c r="Y16" s="35"/>
@@ -2140,35 +2128,35 @@
       <c r="E17" s="33"/>
       <c r="F17" s="38"/>
       <c r="G17" s="32" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H17" s="38"/>
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
       <c r="K17" s="33" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="33" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="33" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="R17" s="38"/>
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
       <c r="U17" s="33" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="V17" s="38"/>
       <c r="W17" s="33" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
@@ -2181,53 +2169,51 @@
     <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="21" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H18" s="22"/>
-      <c r="I18" s="21" t="s">
-        <v>96</v>
-      </c>
+      <c r="I18" s="21"/>
       <c r="J18" s="22"/>
       <c r="K18" s="21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="L18" s="22"/>
       <c r="M18" s="21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N18" s="22"/>
       <c r="O18" s="21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="P18" s="22"/>
       <c r="Q18" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R18" s="22"/>
       <c r="S18" s="21" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="T18" s="22"/>
       <c r="U18" s="21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="V18" s="22"/>
       <c r="W18" s="21" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="X18" s="22"/>
       <c r="Y18" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="Z18" s="22"/>
       <c r="AA18" s="21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="AB18" s="22"/>
       <c r="AC18" s="21"/>
@@ -2236,7 +2222,7 @@
     <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="12" t="s">
@@ -2244,12 +2230,10 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="12" t="s">
-        <v>74</v>
-      </c>
+      <c r="I19" s="12"/>
       <c r="J19" s="1"/>
       <c r="K19" s="12" t="s">
         <v>47</v>
@@ -2260,11 +2244,11 @@
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2272,7 +2256,7 @@
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="12" t="s">
@@ -2288,7 +2272,7 @@
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AD19" s="1"/>
     </row>
@@ -2383,37 +2367,37 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="J22" s="36"/>
       <c r="K22" s="35" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="L22" s="36"/>
       <c r="M22" s="35" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
       <c r="P22" s="36"/>
       <c r="Q22" s="35" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="V22" s="36"/>
       <c r="W22" s="35"/>
@@ -2430,37 +2414,37 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>
       <c r="M23" s="32" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="30"/>
@@ -2477,39 +2461,37 @@
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H24" s="22"/>
-      <c r="I24" s="21" t="s">
-        <v>97</v>
-      </c>
+      <c r="I24" s="21"/>
       <c r="J24" s="22"/>
       <c r="K24" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L24" s="22"/>
       <c r="M24" s="21" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N24" s="22"/>
       <c r="O24" s="21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="P24" s="22"/>
       <c r="Q24" s="21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="R24" s="22"/>
       <c r="S24" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2530,15 +2512,13 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="12" t="s">
-        <v>75</v>
-      </c>
+      <c r="I25" s="12"/>
       <c r="J25" s="1"/>
       <c r="K25" s="12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="12" t="s">
@@ -2550,11 +2530,11 @@
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="12" t="s">
@@ -2564,7 +2544,7 @@
       <c r="W25" s="12"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="12"/>
@@ -2606,7 +2586,7 @@
     <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="10" t="s">
@@ -2661,29 +2641,29 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="35" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="R28" s="36"/>
       <c r="S28" s="35"/>
@@ -2704,25 +2684,25 @@
       <c r="C29" s="30"/>
       <c r="D29" s="1"/>
       <c r="E29" s="32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="30"/>
       <c r="L29" s="1"/>
       <c r="M29" s="32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="32" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
@@ -2745,43 +2725,43 @@
       <c r="C30" s="21"/>
       <c r="D30" s="22"/>
       <c r="E30" s="21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="21" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="N30" s="22"/>
       <c r="O30" s="21" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T30" s="22"/>
       <c r="U30" s="21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="V30" s="22"/>
       <c r="W30" s="21" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="X30" s="22"/>
       <c r="Y30" s="26"/>
@@ -2808,19 +2788,19 @@
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="12" t="s">
@@ -2832,7 +2812,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="12" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="14"/>
@@ -2865,7 +2845,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -2878,15 +2858,15 @@
     <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="15" t="s">
@@ -2908,7 +2888,7 @@
       <c r="W33" s="3"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z33" s="1"/>
       <c r="AA33" s="10" t="s">
@@ -2916,7 +2896,7 @@
       </c>
       <c r="AB33" s="1"/>
       <c r="AC33" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AD33" s="1"/>
     </row>
@@ -2925,13 +2905,13 @@
       <c r="C34" s="30"/>
       <c r="D34" s="1"/>
       <c r="E34" s="35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
       <c r="I34" s="41" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -2962,7 +2942,7 @@
       <c r="E35" s="35"/>
       <c r="F35" s="1"/>
       <c r="G35" s="33" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="41"/>
@@ -2984,7 +2964,7 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="33" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="30"/>
@@ -2993,7 +2973,7 @@
     <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="21" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="35"/>
@@ -3001,7 +2981,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="22"/>
       <c r="I36" s="27" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
@@ -3019,15 +2999,15 @@
       <c r="W36" s="22"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="21" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Z36" s="22"/>
       <c r="AA36" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AB36" s="22"/>
       <c r="AC36" s="21" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AD36" s="1"/>
     </row>
@@ -3040,7 +3020,7 @@
       <c r="G37" s="12"/>
       <c r="H37" s="1"/>
       <c r="I37" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
@@ -3058,7 +3038,7 @@
       <c r="W37" s="5"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Z37" s="1"/>
       <c r="AA37" s="12" t="s">
@@ -3066,7 +3046,7 @@
       </c>
       <c r="AB37" s="1"/>
       <c r="AC37" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AD37" s="1"/>
     </row>
@@ -3172,21 +3152,21 @@
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="34" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="34" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3202,48 +3182,48 @@
       <c r="W41" s="3"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="33" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41" s="33" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="33" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="AD41" s="1"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="34" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
@@ -3253,48 +3233,48 @@
       <c r="W42" s="22"/>
       <c r="X42" s="22"/>
       <c r="Y42" s="21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="Z42" s="22"/>
       <c r="AA42" s="21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AB42" s="22"/>
       <c r="AC42" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AD42" s="1"/>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="34" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="5"/>
       <c r="O43" s="34" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>

</xml_diff>

<commit_message>
Speed slider dead zone, Zoom -32x, fixes
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0B378-0075-4455-894F-B0E26535A3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC9FA9D-BF39-4809-928E-91223F82733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,9 +489,6 @@
     <t>cell borders</t>
   </si>
   <si>
-    <t>zoom x64</t>
-  </si>
-  <si>
     <t>zoom 1x</t>
   </si>
   <si>
@@ -781,6 +778,9 @@
   </si>
   <si>
     <t>tilt up</t>
+  </si>
+  <si>
+    <t>zoom -32x</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1414,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI39" sqref="AI39"/>
+      <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,23 +1492,23 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
@@ -1549,11 +1549,11 @@
       <c r="M4" s="37"/>
       <c r="N4" s="36"/>
       <c r="O4" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P4" s="36"/>
       <c r="Q4" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R4" s="43"/>
       <c r="S4" s="43"/>
@@ -1567,7 +1567,7 @@
       <c r="AA4" s="35"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1600,7 +1600,7 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1635,7 +1635,7 @@
       <c r="AA6" s="21"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
@@ -1650,23 +1650,23 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="5"/>
@@ -1686,7 +1686,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1785,43 +1785,43 @@
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P10" s="36"/>
       <c r="Q10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R10" s="36"/>
       <c r="S10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="T10" s="36"/>
       <c r="U10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="V10" s="36"/>
       <c r="W10" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="37"/>
@@ -1836,43 +1836,43 @@
       <c r="C11" s="30"/>
       <c r="D11" s="1"/>
       <c r="E11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="31"/>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23" t="s">
-        <v>150</v>
+        <v>247</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N12" s="22"/>
       <c r="O12" s="23" t="s">
@@ -1936,19 +1936,19 @@
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="11" t="s">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11" t="s">
@@ -1964,7 +1964,7 @@
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="11" t="s">
@@ -2083,7 +2083,7 @@
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
       <c r="E16" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="35"/>
@@ -2097,21 +2097,21 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="35"/>
       <c r="R16" s="36"/>
       <c r="S16" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T16" s="36"/>
       <c r="U16" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="V16" s="36"/>
       <c r="W16" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X16" s="36"/>
       <c r="Y16" s="35"/>
@@ -2128,35 +2128,35 @@
       <c r="E17" s="33"/>
       <c r="F17" s="38"/>
       <c r="G17" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H17" s="38"/>
       <c r="I17" s="33"/>
       <c r="J17" s="38"/>
       <c r="K17" s="33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N17" s="38"/>
       <c r="O17" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P17" s="38"/>
       <c r="Q17" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R17" s="38"/>
       <c r="S17" s="33"/>
       <c r="T17" s="38"/>
       <c r="U17" s="33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V17" s="38"/>
       <c r="W17" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X17" s="38"/>
       <c r="Y17" s="33"/>
@@ -2175,7 +2175,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="12"/>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="12" t="s">
@@ -2367,37 +2367,37 @@
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F22" s="36"/>
       <c r="G22" s="35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H22" s="36"/>
       <c r="I22" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J22" s="36"/>
       <c r="K22" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L22" s="36"/>
       <c r="M22" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="35"/>
       <c r="P22" s="36"/>
       <c r="Q22" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R22" s="36"/>
       <c r="S22" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T22" s="36"/>
       <c r="U22" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="V22" s="36"/>
       <c r="W22" s="35"/>
@@ -2414,33 +2414,33 @@
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="30"/>
       <c r="L23" s="1"/>
       <c r="M23" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="32" t="s">
@@ -2461,7 +2461,7 @@
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
@@ -2518,7 +2518,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="1"/>
       <c r="K25" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="12" t="s">
@@ -2544,7 +2544,7 @@
       <c r="W25" s="12"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="12"/>
@@ -2641,29 +2641,29 @@
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
       <c r="E28" s="35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J28" s="36"/>
       <c r="K28" s="35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N28" s="36"/>
       <c r="O28" s="35"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="R28" s="36"/>
       <c r="S28" s="35"/>
@@ -2684,11 +2684,11 @@
       <c r="C29" s="30"/>
       <c r="D29" s="1"/>
       <c r="E29" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="32" t="s">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
@@ -2741,15 +2741,15 @@
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N30" s="22"/>
       <c r="O30" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P30" s="22"/>
       <c r="Q30" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="R30" s="22"/>
       <c r="S30" s="21" t="s">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="V30" s="22"/>
       <c r="W30" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X30" s="22"/>
       <c r="Y30" s="26"/>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="14"/>
@@ -2845,7 +2845,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2911,7 +2911,7 @@
       <c r="G34" s="33"/>
       <c r="H34" s="1"/>
       <c r="I34" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="39"/>
@@ -2964,7 +2964,7 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="30"/>
@@ -2981,7 +2981,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="22"/>
       <c r="I36" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
@@ -3152,21 +3152,21 @@
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3182,48 +3182,48 @@
       <c r="W41" s="3"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AD41" s="1"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="22"/>
       <c r="O42" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
@@ -3248,33 +3248,33 @@
     <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="5"/>
       <c r="O43" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>

</xml_diff>

<commit_message>
added more missing UI controls
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC9FA9D-BF39-4809-928E-91223F82733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA690534-F43C-4B1B-85D8-4D4B56E33C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1414,7 +1414,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI13" sqref="AI13"/>
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3209,7 +3209,7 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
@@ -3260,7 +3260,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">

</xml_diff>

<commit_message>
extended Tilt from -5 to +5, fixed cell and selection info boxes appearing during init
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA690534-F43C-4B1B-85D8-4D4B56E33C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9C97F2-5AA3-4D61-A308-03490FFE11C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="249">
   <si>
     <t>Q</t>
   </si>
@@ -781,6 +781,9 @@
   </si>
   <si>
     <t>zoom -32x</t>
+  </si>
+  <si>
+    <t>reset tilt</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1417,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2496,7 +2499,9 @@
       <c r="V24" s="22"/>
       <c r="W24" s="21"/>
       <c r="X24" s="22"/>
-      <c r="Y24" s="23"/>
+      <c r="Y24" s="23" t="s">
+        <v>248</v>
+      </c>
       <c r="Z24" s="22"/>
       <c r="AA24" s="21"/>
       <c r="AB24" s="22"/>

</xml_diff>

<commit_message>
add new UI controls for multi-viewer functions and rotate camera 45 degrees, add neighbourhood name to rule label tooltip and window title and waypoint messages
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9C97F2-5AA3-4D61-A308-03490FFE11C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B845A6B-F2AC-41BB-AC14-DC36AB9B7090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="252">
   <si>
     <t>Q</t>
   </si>
@@ -784,6 +784,15 @@
   </si>
   <si>
     <t>reset tilt</t>
+  </si>
+  <si>
+    <t>rotate left 45</t>
+  </si>
+  <si>
+    <t>rotate right 45</t>
+  </si>
+  <si>
+    <t>snap angle 45</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1426,7 @@
   <dimension ref="B2:AD49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2712,11 +2721,17 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="30"/>
       <c r="R29" s="1"/>
-      <c r="S29" s="30"/>
+      <c r="S29" s="32" t="s">
+        <v>249</v>
+      </c>
       <c r="T29" s="1"/>
-      <c r="U29" s="30"/>
+      <c r="U29" s="32" t="s">
+        <v>250</v>
+      </c>
       <c r="V29" s="1"/>
-      <c r="W29" s="32"/>
+      <c r="W29" s="32" t="s">
+        <v>251</v>
+      </c>
       <c r="X29" s="1"/>
       <c r="Y29" s="13"/>
       <c r="Z29" s="1"/>

</xml_diff>

<commit_message>
cell period map improvements and fixes
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B845A6B-F2AC-41BB-AC14-DC36AB9B7090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D1BDD2-B5ED-4419-BBB9-1AE83A97E4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="254">
   <si>
     <t>Q</t>
   </si>
@@ -793,6 +793,12 @@
   </si>
   <si>
     <t>snap angle 45</t>
+  </si>
+  <si>
+    <t>toggle periods</t>
+  </si>
+  <si>
+    <t>last identify</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1040,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1099,7 +1104,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1128,7 +1133,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1423,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AD49"/>
+  <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,209 +1500,211 @@
     </row>
     <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>162</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>163</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>164</v>
       </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>165</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>215</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="3"/>
+      <c r="Q3" s="2"/>
       <c r="R3" s="1"/>
-      <c r="S3" s="3"/>
+      <c r="S3" s="2"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="3"/>
+      <c r="U3" s="2"/>
       <c r="V3" s="1"/>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="9" t="s">
         <v>76</v>
       </c>
       <c r="X3" s="1"/>
-      <c r="Y3" s="10" t="s">
+      <c r="Y3" s="9" t="s">
         <v>77</v>
       </c>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="10" t="s">
+      <c r="AA3" s="9" t="s">
         <v>78</v>
       </c>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="10" t="s">
+      <c r="AC3" s="9" t="s">
         <v>79</v>
       </c>
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="37" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="42" t="s">
+      <c r="P4" s="35"/>
+      <c r="Q4" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="35" t="s">
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="34" t="s">
         <v>195</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
-      <c r="C5" s="31"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="31"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="31"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="31"/>
+      <c r="I5" s="30"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="31"/>
+      <c r="K5" s="30"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="31"/>
+      <c r="M5" s="30"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="31"/>
+      <c r="O5" s="30"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
       <c r="V5" s="1"/>
-      <c r="W5" s="30"/>
+      <c r="W5" s="29"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="30"/>
+      <c r="Y5" s="29"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="30"/>
+      <c r="AA5" s="29"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="32" t="s">
+      <c r="AC5" s="31" t="s">
         <v>208</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="21" t="s">
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="42"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="20" t="s">
         <v>198</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>109</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>148</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>166</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>168</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="10" t="s">
         <v>167</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="10" t="s">
         <v>169</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="11" t="s">
+      <c r="O7" s="10" t="s">
         <v>216</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="5"/>
+      <c r="Q7" s="4"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="5"/>
+      <c r="S7" s="4"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="5"/>
+      <c r="U7" s="4"/>
       <c r="V7" s="1"/>
-      <c r="W7" s="12" t="s">
+      <c r="W7" s="11" t="s">
         <v>83</v>
       </c>
       <c r="X7" s="1"/>
-      <c r="Y7" s="12" t="s">
+      <c r="Y7" s="11" t="s">
         <v>84</v>
       </c>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="12"/>
+      <c r="AA7" s="11"/>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="12" t="s">
+      <c r="AC7" s="11" t="s">
         <v>203</v>
       </c>
       <c r="AD7" s="1"/>
@@ -1735,267 +1742,267 @@
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="8" t="s">
         <v>29</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="8" t="s">
+      <c r="O9" s="7" t="s">
         <v>30</v>
       </c>
       <c r="P9" s="1"/>
-      <c r="Q9" s="8" t="s">
+      <c r="Q9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="8" t="s">
+      <c r="S9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="8" t="s">
+      <c r="U9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="V9" s="1"/>
-      <c r="W9" s="8" t="s">
+      <c r="W9" s="7" t="s">
         <v>34</v>
       </c>
       <c r="X9" s="1"/>
-      <c r="Y9" s="8" t="s">
+      <c r="Y9" s="7" t="s">
         <v>35</v>
       </c>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="8" t="s">
+      <c r="AA9" s="7" t="s">
         <v>36</v>
       </c>
       <c r="AB9" s="1"/>
-      <c r="AC9" s="10" t="s">
+      <c r="AC9" s="9" t="s">
         <v>82</v>
       </c>
       <c r="AD9" s="1"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37" t="s">
+      <c r="F10" s="35"/>
+      <c r="G10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37" t="s">
+      <c r="H10" s="35"/>
+      <c r="I10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37" t="s">
+      <c r="J10" s="35"/>
+      <c r="K10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="L10" s="36"/>
-      <c r="M10" s="37" t="s">
+      <c r="L10" s="35"/>
+      <c r="M10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="N10" s="36"/>
-      <c r="O10" s="37" t="s">
+      <c r="N10" s="35"/>
+      <c r="O10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="37" t="s">
+      <c r="P10" s="35"/>
+      <c r="Q10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="R10" s="36"/>
-      <c r="S10" s="37" t="s">
+      <c r="R10" s="35"/>
+      <c r="S10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="T10" s="36"/>
-      <c r="U10" s="37" t="s">
+      <c r="T10" s="35"/>
+      <c r="U10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="V10" s="36"/>
-      <c r="W10" s="37" t="s">
+      <c r="V10" s="35"/>
+      <c r="W10" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="36"/>
-      <c r="AA10" s="37"/>
-      <c r="AB10" s="36"/>
-      <c r="AC10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="36"/>
+      <c r="Z10" s="35"/>
+      <c r="AA10" s="36"/>
+      <c r="AB10" s="35"/>
+      <c r="AC10" s="34"/>
       <c r="AD10" s="1"/>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="30"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="32" t="s">
+      <c r="K11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="32" t="s">
+      <c r="M11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="32" t="s">
+      <c r="O11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="P11" s="1"/>
-      <c r="Q11" s="32" t="s">
+      <c r="Q11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="R11" s="1"/>
-      <c r="S11" s="32" t="s">
+      <c r="S11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="T11" s="1"/>
-      <c r="U11" s="32" t="s">
+      <c r="U11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="V11" s="1"/>
-      <c r="W11" s="32" t="s">
+      <c r="W11" s="31" t="s">
         <v>206</v>
       </c>
       <c r="X11" s="1"/>
-      <c r="Y11" s="31"/>
+      <c r="Y11" s="30"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="31"/>
+      <c r="AA11" s="30"/>
       <c r="AB11" s="1"/>
-      <c r="AC11" s="30"/>
+      <c r="AC11" s="29"/>
       <c r="AD11" s="1"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23" t="s">
+      <c r="H12" s="21"/>
+      <c r="I12" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23" t="s">
+      <c r="J12" s="21"/>
+      <c r="K12" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="22"/>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="21"/>
+      <c r="M12" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="23" t="s">
+      <c r="N12" s="21"/>
+      <c r="O12" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="23" t="s">
+      <c r="P12" s="21"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="T12" s="22"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="23" t="s">
+      <c r="T12" s="21"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="23" t="s">
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="21"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="20"/>
       <c r="AD12" s="1"/>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>150</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="10" t="s">
         <v>152</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="10" t="s">
         <v>153</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="10" t="s">
         <v>91</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="11" t="s">
+      <c r="O13" s="10" t="s">
         <v>154</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="Q13" s="11" t="s">
+      <c r="Q13" s="10" t="s">
         <v>131</v>
       </c>
       <c r="R13" s="1"/>
-      <c r="S13" s="11" t="s">
+      <c r="S13" s="10" t="s">
         <v>155</v>
       </c>
       <c r="T13" s="1"/>
-      <c r="U13" s="11" t="s">
+      <c r="U13" s="10" t="s">
         <v>130</v>
       </c>
       <c r="V13" s="1"/>
-      <c r="W13" s="11" t="s">
+      <c r="W13" s="10" t="s">
         <v>126</v>
       </c>
       <c r="X13" s="1"/>
-      <c r="Y13" s="11" t="s">
+      <c r="Y13" s="10" t="s">
         <v>48</v>
       </c>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="11" t="s">
+      <c r="AA13" s="10" t="s">
         <v>49</v>
       </c>
       <c r="AB13" s="1"/>
-      <c r="AC13" s="12" t="s">
+      <c r="AC13" s="11" t="s">
         <v>113</v>
       </c>
       <c r="AD13" s="1"/>
@@ -2033,257 +2040,257 @@
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>2</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="9" t="s">
         <v>3</v>
       </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="10" t="s">
+      <c r="M15" s="9" t="s">
         <v>4</v>
       </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="10" t="s">
+      <c r="O15" s="9" t="s">
         <v>5</v>
       </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="10" t="s">
+      <c r="Q15" s="9" t="s">
         <v>134</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="10" t="s">
+      <c r="S15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="T15" s="1"/>
-      <c r="U15" s="10" t="s">
+      <c r="U15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="V15" s="1"/>
-      <c r="W15" s="10" t="s">
+      <c r="W15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="X15" s="1"/>
-      <c r="Y15" s="10" t="s">
+      <c r="Y15" s="9" t="s">
         <v>37</v>
       </c>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="10" t="s">
+      <c r="AA15" s="9" t="s">
         <v>38</v>
       </c>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="10" t="s">
+      <c r="AC15" s="9" t="s">
         <v>46</v>
       </c>
       <c r="AD15" s="1"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="35" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="35" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="36"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="35" t="s">
+      <c r="L16" s="35"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="35" t="s">
+      <c r="P16" s="35"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="T16" s="36"/>
-      <c r="U16" s="35" t="s">
+      <c r="T16" s="35"/>
+      <c r="U16" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="V16" s="36"/>
-      <c r="W16" s="35" t="s">
+      <c r="V16" s="35"/>
+      <c r="W16" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="36"/>
-      <c r="AC16" s="35"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="34"/>
+      <c r="Z16" s="35"/>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="35"/>
+      <c r="AC16" s="34"/>
       <c r="AD16" s="1"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="32" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="H17" s="38"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="33" t="s">
+      <c r="H17" s="37"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="L17" s="38"/>
-      <c r="M17" s="33" t="s">
+      <c r="L17" s="37"/>
+      <c r="M17" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="N17" s="38"/>
-      <c r="O17" s="33" t="s">
+      <c r="N17" s="37"/>
+      <c r="O17" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="33" t="s">
+      <c r="P17" s="37"/>
+      <c r="Q17" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="R17" s="38"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="33" t="s">
+      <c r="R17" s="37"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="V17" s="38"/>
-      <c r="W17" s="33" t="s">
+      <c r="V17" s="37"/>
+      <c r="W17" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="33"/>
-      <c r="AB17" s="38"/>
-      <c r="AC17" s="33"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="37"/>
+      <c r="AA17" s="32"/>
+      <c r="AB17" s="37"/>
+      <c r="AC17" s="32"/>
       <c r="AD17" s="1"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="21" t="s">
+      <c r="D18" s="21"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="21" t="s">
+      <c r="H18" s="21"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="L18" s="22"/>
-      <c r="M18" s="21" t="s">
+      <c r="L18" s="21"/>
+      <c r="M18" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="N18" s="22"/>
-      <c r="O18" s="21" t="s">
+      <c r="N18" s="21"/>
+      <c r="O18" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="21" t="s">
+      <c r="P18" s="21"/>
+      <c r="Q18" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="21" t="s">
+      <c r="R18" s="21"/>
+      <c r="S18" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="T18" s="22"/>
-      <c r="U18" s="21" t="s">
+      <c r="T18" s="21"/>
+      <c r="U18" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="V18" s="22"/>
-      <c r="W18" s="21" t="s">
+      <c r="V18" s="21"/>
+      <c r="W18" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="21" t="s">
+      <c r="X18" s="21"/>
+      <c r="Y18" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="21" t="s">
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="21"/>
+      <c r="AB18" s="21"/>
+      <c r="AC18" s="20"/>
       <c r="AD18" s="1"/>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>124</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>63</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="11" t="s">
         <v>238</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="12"/>
+      <c r="I19" s="11"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="11" t="s">
         <v>47</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="12" t="s">
+      <c r="M19" s="11" t="s">
         <v>69</v>
       </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="12" t="s">
+      <c r="O19" s="11" t="s">
         <v>128</v>
       </c>
       <c r="P19" s="1"/>
-      <c r="Q19" s="12" t="s">
+      <c r="Q19" s="11" t="s">
         <v>212</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="12" t="s">
+      <c r="S19" s="11" t="s">
         <v>70</v>
       </c>
       <c r="T19" s="1"/>
-      <c r="U19" s="12" t="s">
+      <c r="U19" s="11" t="s">
         <v>133</v>
       </c>
       <c r="V19" s="1"/>
-      <c r="W19" s="12" t="s">
+      <c r="W19" s="11" t="s">
         <v>65</v>
       </c>
       <c r="X19" s="1"/>
-      <c r="Y19" s="12" t="s">
+      <c r="Y19" s="11" t="s">
         <v>51</v>
       </c>
       <c r="Z19" s="1"/>
-      <c r="AA19" s="12" t="s">
+      <c r="AA19" s="11" t="s">
         <v>52</v>
       </c>
       <c r="AB19" s="1"/>
-      <c r="AC19" s="12" t="s">
+      <c r="AC19" s="11" t="s">
         <v>93</v>
       </c>
       <c r="AD19" s="1"/>
@@ -2321,249 +2328,251 @@
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="9" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="1"/>
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="9" t="s">
         <v>12</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="10" t="s">
+      <c r="M21" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="10" t="s">
+      <c r="O21" s="9" t="s">
         <v>14</v>
       </c>
       <c r="P21" s="1"/>
-      <c r="Q21" s="10" t="s">
+      <c r="Q21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="S21" s="10" t="s">
+      <c r="S21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="T21" s="1"/>
-      <c r="U21" s="10" t="s">
+      <c r="U21" s="9" t="s">
         <v>17</v>
       </c>
       <c r="V21" s="1"/>
-      <c r="W21" s="10" t="s">
+      <c r="W21" s="9" t="s">
         <v>39</v>
       </c>
       <c r="X21" s="1"/>
-      <c r="Y21" s="8" t="s">
+      <c r="Y21" s="7" t="s">
         <v>41</v>
       </c>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="10" t="s">
+      <c r="AA21" s="9" t="s">
         <v>40</v>
       </c>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="4"/>
+      <c r="AC21" s="3"/>
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="35" t="s">
+      <c r="F22" s="35"/>
+      <c r="G22" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="H22" s="36"/>
-      <c r="I22" s="35" t="s">
+      <c r="H22" s="35"/>
+      <c r="I22" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="J22" s="36"/>
-      <c r="K22" s="35" t="s">
+      <c r="J22" s="35"/>
+      <c r="K22" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="L22" s="36"/>
-      <c r="M22" s="35" t="s">
+      <c r="L22" s="35"/>
+      <c r="M22" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="N22" s="36"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="35" t="s">
+      <c r="N22" s="35"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="R22" s="36"/>
-      <c r="S22" s="35" t="s">
+      <c r="R22" s="35"/>
+      <c r="S22" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="T22" s="36"/>
-      <c r="U22" s="35" t="s">
+      <c r="T22" s="35"/>
+      <c r="U22" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="V22" s="36"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="36"/>
-      <c r="AA22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="35"/>
+      <c r="AA22" s="34"/>
       <c r="AB22" s="1"/>
-      <c r="AC22" s="4"/>
+      <c r="AC22" s="3"/>
       <c r="AD22" s="1"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="32" t="s">
         <v>188</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="32" t="s">
         <v>187</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="32" t="s">
         <v>213</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="30"/>
+      <c r="K23" s="29"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="32" t="s">
+      <c r="M23" s="31" t="s">
         <v>233</v>
       </c>
       <c r="N23" s="1"/>
-      <c r="O23" s="32" t="s">
+      <c r="O23" s="31" t="s">
         <v>234</v>
       </c>
       <c r="P23" s="1"/>
-      <c r="Q23" s="32" t="s">
+      <c r="Q23" s="31" t="s">
         <v>237</v>
       </c>
       <c r="R23" s="1"/>
-      <c r="S23" s="32" t="s">
+      <c r="S23" s="31" t="s">
         <v>202</v>
       </c>
       <c r="T23" s="1"/>
-      <c r="U23" s="32" t="s">
+      <c r="U23" s="31" t="s">
         <v>145</v>
       </c>
       <c r="V23" s="1"/>
-      <c r="W23" s="30"/>
+      <c r="W23" s="29"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="31"/>
+      <c r="Y23" s="30"/>
       <c r="Z23" s="1"/>
-      <c r="AA23" s="30"/>
+      <c r="AA23" s="29"/>
       <c r="AB23" s="1"/>
-      <c r="AC23" s="4"/>
+      <c r="AC23" s="3"/>
       <c r="AD23" s="1"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="21" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="21" t="s">
+      <c r="F24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="21" t="s">
+      <c r="H24" s="21"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="L24" s="22"/>
-      <c r="M24" s="21" t="s">
+      <c r="L24" s="21"/>
+      <c r="M24" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="N24" s="22"/>
-      <c r="O24" s="21" t="s">
+      <c r="N24" s="21"/>
+      <c r="O24" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="21" t="s">
+      <c r="P24" s="21"/>
+      <c r="Q24" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="R24" s="22"/>
-      <c r="S24" s="21" t="s">
+      <c r="R24" s="21"/>
+      <c r="S24" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="T24" s="22"/>
-      <c r="U24" s="21" t="s">
+      <c r="T24" s="21"/>
+      <c r="U24" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="V24" s="22"/>
-      <c r="W24" s="21"/>
-      <c r="X24" s="22"/>
-      <c r="Y24" s="23" t="s">
+      <c r="V24" s="21"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="Z24" s="22"/>
-      <c r="AA24" s="21"/>
-      <c r="AB24" s="22"/>
-      <c r="AC24" s="25"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="24"/>
       <c r="AD24" s="1"/>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="11" t="s">
         <v>90</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="12"/>
+      <c r="I25" s="11" t="s">
+        <v>252</v>
+      </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="11" t="s">
         <v>225</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="12" t="s">
+      <c r="M25" s="11" t="s">
         <v>68</v>
       </c>
       <c r="N25" s="1"/>
-      <c r="O25" s="12" t="s">
+      <c r="O25" s="11" t="s">
         <v>72</v>
       </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="12" t="s">
+      <c r="Q25" s="11" t="s">
         <v>115</v>
       </c>
       <c r="R25" s="1"/>
-      <c r="S25" s="12" t="s">
+      <c r="S25" s="11" t="s">
         <v>143</v>
       </c>
       <c r="T25" s="1"/>
-      <c r="U25" s="12" t="s">
+      <c r="U25" s="11" t="s">
         <v>66</v>
       </c>
       <c r="V25" s="1"/>
-      <c r="W25" s="12"/>
+      <c r="W25" s="11"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="12" t="s">
+      <c r="Y25" s="11" t="s">
         <v>244</v>
       </c>
       <c r="Z25" s="1"/>
-      <c r="AA25" s="12"/>
+      <c r="AA25" s="11"/>
       <c r="AB25" s="1"/>
-      <c r="AC25" s="7"/>
+      <c r="AC25" s="6"/>
       <c r="AD25" s="1"/>
     </row>
     <row r="26" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2599,247 +2608,247 @@
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>87</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>18</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="1"/>
-      <c r="K27" s="10" t="s">
+      <c r="K27" s="9" t="s">
         <v>21</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="10" t="s">
+      <c r="M27" s="9" t="s">
         <v>22</v>
       </c>
       <c r="N27" s="1"/>
-      <c r="O27" s="10" t="s">
+      <c r="O27" s="9" t="s">
         <v>23</v>
       </c>
       <c r="P27" s="1"/>
-      <c r="Q27" s="10" t="s">
+      <c r="Q27" s="9" t="s">
         <v>24</v>
       </c>
       <c r="R27" s="1"/>
-      <c r="S27" s="10" t="s">
+      <c r="S27" s="9" t="s">
         <v>42</v>
       </c>
       <c r="T27" s="1"/>
-      <c r="U27" s="10" t="s">
+      <c r="U27" s="9" t="s">
         <v>43</v>
       </c>
       <c r="V27" s="1"/>
-      <c r="W27" s="10" t="s">
+      <c r="W27" s="9" t="s">
         <v>44</v>
       </c>
       <c r="X27" s="1"/>
-      <c r="Y27" s="13"/>
+      <c r="Y27" s="12"/>
       <c r="Z27" s="1"/>
-      <c r="AA27" s="13"/>
+      <c r="AA27" s="12"/>
       <c r="AB27" s="1"/>
-      <c r="AC27" s="3"/>
+      <c r="AC27" s="2"/>
       <c r="AD27" s="1"/>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="35" t="s">
+      <c r="C28" s="34"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="35" t="s">
+      <c r="F28" s="35"/>
+      <c r="G28" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="H28" s="36"/>
-      <c r="I28" s="35" t="s">
+      <c r="H28" s="35"/>
+      <c r="I28" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="J28" s="36"/>
-      <c r="K28" s="35" t="s">
+      <c r="J28" s="35"/>
+      <c r="K28" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="35" t="s">
+      <c r="L28" s="35"/>
+      <c r="M28" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="N28" s="36"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="35" t="s">
+      <c r="N28" s="35"/>
+      <c r="O28" s="34"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="R28" s="36"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="36"/>
-      <c r="W28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="34"/>
       <c r="X28" s="1"/>
-      <c r="Y28" s="13"/>
+      <c r="Y28" s="12"/>
       <c r="Z28" s="1"/>
-      <c r="AA28" s="13"/>
+      <c r="AA28" s="12"/>
       <c r="AB28" s="1"/>
-      <c r="AC28" s="3"/>
+      <c r="AC28" s="2"/>
       <c r="AD28" s="1"/>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
-      <c r="C29" s="30"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="31" t="s">
         <v>214</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="31" t="s">
         <v>178</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="32" t="s">
+      <c r="I29" s="31" t="s">
         <v>114</v>
       </c>
       <c r="J29" s="1"/>
-      <c r="K29" s="30"/>
+      <c r="K29" s="29"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="32" t="s">
+      <c r="M29" s="31" t="s">
         <v>149</v>
       </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="32" t="s">
+      <c r="O29" s="31" t="s">
         <v>182</v>
       </c>
       <c r="P29" s="1"/>
-      <c r="Q29" s="30"/>
+      <c r="Q29" s="29"/>
       <c r="R29" s="1"/>
-      <c r="S29" s="32" t="s">
+      <c r="S29" s="31" t="s">
         <v>249</v>
       </c>
       <c r="T29" s="1"/>
-      <c r="U29" s="32" t="s">
+      <c r="U29" s="31" t="s">
         <v>250</v>
       </c>
       <c r="V29" s="1"/>
-      <c r="W29" s="32" t="s">
+      <c r="W29" s="31" t="s">
         <v>251</v>
       </c>
       <c r="X29" s="1"/>
-      <c r="Y29" s="13"/>
+      <c r="Y29" s="12"/>
       <c r="Z29" s="1"/>
-      <c r="AA29" s="13"/>
+      <c r="AA29" s="12"/>
       <c r="AB29" s="1"/>
-      <c r="AC29" s="3"/>
+      <c r="AC29" s="2"/>
       <c r="AD29" s="1"/>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="21" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="21" t="s">
+      <c r="F30" s="21"/>
+      <c r="G30" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="21" t="s">
+      <c r="H30" s="21"/>
+      <c r="I30" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="22"/>
-      <c r="K30" s="21" t="s">
+      <c r="J30" s="21"/>
+      <c r="K30" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="L30" s="22"/>
-      <c r="M30" s="21" t="s">
+      <c r="L30" s="21"/>
+      <c r="M30" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="N30" s="22"/>
-      <c r="O30" s="21" t="s">
+      <c r="N30" s="21"/>
+      <c r="O30" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="21" t="s">
+      <c r="P30" s="21"/>
+      <c r="Q30" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="R30" s="22"/>
-      <c r="S30" s="21" t="s">
+      <c r="R30" s="21"/>
+      <c r="S30" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="T30" s="22"/>
-      <c r="U30" s="21" t="s">
+      <c r="T30" s="21"/>
+      <c r="U30" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="V30" s="22"/>
-      <c r="W30" s="21" t="s">
+      <c r="V30" s="21"/>
+      <c r="W30" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="X30" s="22"/>
-      <c r="Y30" s="26"/>
-      <c r="Z30" s="22"/>
-      <c r="AA30" s="26"/>
-      <c r="AB30" s="22"/>
-      <c r="AC30" s="22"/>
+      <c r="X30" s="21"/>
+      <c r="Y30" s="25"/>
+      <c r="Z30" s="21"/>
+      <c r="AA30" s="25"/>
+      <c r="AB30" s="21"/>
+      <c r="AC30" s="21"/>
       <c r="AD30" s="1"/>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
-      <c r="C31" s="6"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="11" t="s">
         <v>71</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="12" t="s">
+      <c r="I31" s="11" t="s">
         <v>67</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="12" t="s">
+      <c r="K31" s="11" t="s">
         <v>112</v>
       </c>
       <c r="L31" s="1"/>
-      <c r="M31" s="12" t="s">
+      <c r="M31" s="11" t="s">
         <v>113</v>
       </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="12" t="s">
+      <c r="O31" s="11" t="s">
         <v>88</v>
       </c>
       <c r="P31" s="1"/>
-      <c r="Q31" s="12" t="s">
+      <c r="Q31" s="11" t="s">
         <v>74</v>
       </c>
       <c r="R31" s="1"/>
-      <c r="S31" s="12" t="s">
+      <c r="S31" s="11" t="s">
         <v>53</v>
       </c>
       <c r="T31" s="1"/>
-      <c r="U31" s="12" t="s">
+      <c r="U31" s="11" t="s">
         <v>54</v>
       </c>
       <c r="V31" s="1"/>
-      <c r="W31" s="12" t="s">
+      <c r="W31" s="11" t="s">
         <v>246</v>
       </c>
       <c r="X31" s="1"/>
-      <c r="Y31" s="14"/>
+      <c r="Y31" s="13"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="14"/>
+      <c r="AA31" s="13"/>
       <c r="AB31" s="1"/>
-      <c r="AC31" s="5"/>
+      <c r="AC31" s="4"/>
       <c r="AD31" s="1"/>
     </row>
     <row r="32" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2877,195 +2886,195 @@
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>137</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>170</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="9" t="s">
         <v>135</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="15" t="s">
+      <c r="I33" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
       <c r="T33" s="1"/>
-      <c r="U33" s="3"/>
+      <c r="U33" s="2"/>
       <c r="V33" s="1"/>
-      <c r="W33" s="3"/>
+      <c r="W33" s="2"/>
       <c r="X33" s="1"/>
-      <c r="Y33" s="10" t="s">
+      <c r="Y33" s="9" t="s">
         <v>80</v>
       </c>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="10" t="s">
+      <c r="AA33" s="9" t="s">
         <v>55</v>
       </c>
       <c r="AB33" s="1"/>
-      <c r="AC33" s="10" t="s">
+      <c r="AC33" s="9" t="s">
         <v>81</v>
       </c>
       <c r="AD33" s="1"/>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
-      <c r="C34" s="30"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="34" t="s">
         <v>136</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="33"/>
+      <c r="G34" s="32"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
       <c r="T34" s="1"/>
-      <c r="U34" s="3"/>
+      <c r="U34" s="2"/>
       <c r="V34" s="1"/>
-      <c r="W34" s="3"/>
+      <c r="W34" s="2"/>
       <c r="X34" s="1"/>
-      <c r="Y34" s="30"/>
+      <c r="Y34" s="29"/>
       <c r="Z34" s="1"/>
-      <c r="AA34" s="30"/>
+      <c r="AA34" s="29"/>
       <c r="AB34" s="1"/>
-      <c r="AC34" s="30"/>
+      <c r="AC34" s="29"/>
       <c r="AD34" s="1"/>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
-      <c r="C35" s="30"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="35"/>
+      <c r="E35" s="34"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="33" t="s">
+      <c r="G35" s="32" t="s">
         <v>136</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="40"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="39"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
       <c r="T35" s="1"/>
-      <c r="U35" s="3"/>
+      <c r="U35" s="2"/>
       <c r="V35" s="1"/>
-      <c r="W35" s="3"/>
+      <c r="W35" s="2"/>
       <c r="X35" s="1"/>
-      <c r="Y35" s="30"/>
+      <c r="Y35" s="29"/>
       <c r="Z35" s="1"/>
-      <c r="AA35" s="33" t="s">
+      <c r="AA35" s="32" t="s">
         <v>220</v>
       </c>
       <c r="AB35" s="1"/>
-      <c r="AC35" s="30"/>
+      <c r="AC35" s="29"/>
       <c r="AD35" s="1"/>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="27" t="s">
+      <c r="D36" s="21"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
-      <c r="N36" s="28"/>
-      <c r="O36" s="28"/>
-      <c r="P36" s="28"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="22"/>
-      <c r="U36" s="22"/>
-      <c r="V36" s="22"/>
-      <c r="W36" s="22"/>
-      <c r="X36" s="22"/>
-      <c r="Y36" s="21" t="s">
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="21"/>
+      <c r="V36" s="21"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="Z36" s="22"/>
-      <c r="AA36" s="21" t="s">
+      <c r="Z36" s="21"/>
+      <c r="AA36" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="AB36" s="22"/>
-      <c r="AC36" s="21" t="s">
+      <c r="AB36" s="21"/>
+      <c r="AC36" s="20" t="s">
         <v>141</v>
       </c>
       <c r="AD36" s="1"/>
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
-      <c r="C37" s="12"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="12"/>
+      <c r="E37" s="11"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="12"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="18" t="s">
+      <c r="I37" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="5"/>
+      <c r="U37" s="4"/>
       <c r="V37" s="1"/>
-      <c r="W37" s="5"/>
+      <c r="W37" s="4"/>
       <c r="X37" s="1"/>
-      <c r="Y37" s="12" t="s">
+      <c r="Y37" s="11" t="s">
         <v>85</v>
       </c>
       <c r="Z37" s="1"/>
-      <c r="AA37" s="12" t="s">
+      <c r="AA37" s="11" t="s">
         <v>59</v>
       </c>
       <c r="AB37" s="1"/>
-      <c r="AC37" s="12" t="s">
+      <c r="AC37" s="11" t="s">
         <v>86</v>
       </c>
       <c r="AD37" s="1"/>
@@ -3103,224 +3112,224 @@
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="2"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="3"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="2"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
       <c r="T39" s="1"/>
-      <c r="U39" s="3"/>
+      <c r="U39" s="2"/>
       <c r="V39" s="1"/>
-      <c r="W39" s="3"/>
+      <c r="W39" s="2"/>
       <c r="X39" s="1"/>
-      <c r="Y39" s="10" t="s">
+      <c r="Y39" s="9" t="s">
         <v>56</v>
       </c>
       <c r="Z39" s="1"/>
-      <c r="AA39" s="10" t="s">
+      <c r="AA39" s="9" t="s">
         <v>57</v>
       </c>
       <c r="AB39" s="1"/>
-      <c r="AC39" s="10" t="s">
+      <c r="AC39" s="9" t="s">
         <v>58</v>
       </c>
       <c r="AD39" s="1"/>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="2"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="3"/>
+      <c r="E40" s="2"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="3"/>
+      <c r="G40" s="2"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
       <c r="T40" s="1"/>
-      <c r="U40" s="3"/>
+      <c r="U40" s="2"/>
       <c r="V40" s="1"/>
-      <c r="W40" s="3"/>
+      <c r="W40" s="2"/>
       <c r="X40" s="1"/>
-      <c r="Y40" s="33"/>
+      <c r="Y40" s="32"/>
       <c r="Z40" s="1"/>
-      <c r="AA40" s="33"/>
+      <c r="AA40" s="32"/>
       <c r="AB40" s="1"/>
-      <c r="AC40" s="33"/>
+      <c r="AC40" s="32"/>
       <c r="AD40" s="1"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="33" t="s">
         <v>223</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="4" t="s">
         <v>224</v>
       </c>
       <c r="F41" s="1"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="2"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="34" t="s">
+      <c r="I41" s="33" t="s">
         <v>190</v>
       </c>
       <c r="J41" s="1"/>
-      <c r="K41" s="5" t="s">
+      <c r="K41" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
       <c r="T41" s="1"/>
-      <c r="U41" s="3"/>
+      <c r="U41" s="2"/>
       <c r="V41" s="1"/>
-      <c r="W41" s="3"/>
+      <c r="W41" s="2"/>
       <c r="X41" s="1"/>
-      <c r="Y41" s="33" t="s">
+      <c r="Y41" s="32" t="s">
         <v>219</v>
       </c>
       <c r="Z41" s="1"/>
-      <c r="AA41" s="33" t="s">
+      <c r="AA41" s="32" t="s">
         <v>221</v>
       </c>
       <c r="AB41" s="1"/>
-      <c r="AC41" s="33" t="s">
+      <c r="AC41" s="32" t="s">
         <v>222</v>
       </c>
       <c r="AD41" s="1"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="33" t="s">
         <v>156</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="34" t="s">
+      <c r="F42" s="21"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="33" t="s">
         <v>159</v>
       </c>
       <c r="J42" s="1"/>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="34" t="s">
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="33" t="s">
         <v>228</v>
       </c>
       <c r="P42" s="1"/>
-      <c r="Q42" s="5" t="s">
+      <c r="Q42" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="R42" s="22"/>
-      <c r="S42" s="22"/>
-      <c r="T42" s="22"/>
-      <c r="U42" s="22"/>
-      <c r="V42" s="22"/>
-      <c r="W42" s="22"/>
-      <c r="X42" s="22"/>
-      <c r="Y42" s="21" t="s">
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="21"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="Z42" s="22"/>
-      <c r="AA42" s="21" t="s">
+      <c r="Z42" s="21"/>
+      <c r="AA42" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="AB42" s="22"/>
-      <c r="AC42" s="21" t="s">
+      <c r="AB42" s="21"/>
+      <c r="AC42" s="20" t="s">
         <v>107</v>
       </c>
       <c r="AD42" s="1"/>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="33" t="s">
         <v>184</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>185</v>
       </c>
       <c r="F43" s="1"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="34" t="s">
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="33" t="s">
         <v>158</v>
       </c>
       <c r="J43" s="1"/>
-      <c r="K43" s="5" t="s">
+      <c r="K43" s="4" t="s">
         <v>160</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="34" t="s">
+      <c r="N43" s="4"/>
+      <c r="O43" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5" t="s">
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
       <c r="T43" s="1"/>
-      <c r="U43" s="5"/>
+      <c r="U43" s="4"/>
       <c r="V43" s="1"/>
-      <c r="W43" s="5"/>
+      <c r="W43" s="4"/>
       <c r="X43" s="1"/>
-      <c r="Y43" s="12" t="s">
+      <c r="Y43" s="11" t="s">
         <v>60</v>
       </c>
       <c r="Z43" s="1"/>
-      <c r="AA43" s="12" t="s">
+      <c r="AA43" s="11" t="s">
         <v>61</v>
       </c>
       <c r="AB43" s="1"/>
-      <c r="AC43" s="12" t="s">
+      <c r="AC43" s="11" t="s">
         <v>62</v>
       </c>
       <c r="AD43" s="1"/>
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -3347,10 +3356,6 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="Q4:U6"/>

</xml_diff>

<commit_message>
added cell period table, improved cell period map
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D1BDD2-B5ED-4419-BBB9-1AE83A97E4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E57211-A69D-4BFA-BB9F-FADC009BBD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="256">
   <si>
     <t>Q</t>
   </si>
@@ -795,10 +795,16 @@
     <t>snap angle 45</t>
   </si>
   <si>
-    <t>toggle periods</t>
-  </si>
-  <si>
     <t>last identify</t>
+  </si>
+  <si>
+    <t>period map</t>
+  </si>
+  <si>
+    <t>period table</t>
+  </si>
+  <si>
+    <t>save period map</t>
   </si>
 </sst>
 </file>
@@ -1431,7 +1437,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="AC50" sqref="AC50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1638,7 +1644,7 @@
       <c r="M6" s="22"/>
       <c r="N6" s="21"/>
       <c r="O6" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="42"/>
@@ -2252,7 +2258,9 @@
         <v>238</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="11"/>
+      <c r="I19" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="11" t="s">
         <v>47</v>
@@ -2487,7 +2495,9 @@
         <v>127</v>
       </c>
       <c r="H24" s="21"/>
-      <c r="I24" s="20"/>
+      <c r="I24" s="20" t="s">
+        <v>255</v>
+      </c>
       <c r="J24" s="21"/>
       <c r="K24" s="20" t="s">
         <v>94</v>
@@ -2537,7 +2547,7 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="11" t="s">

</xml_diff>

<commit_message>
added data selection to Population Graph
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E57211-A69D-4BFA-BB9F-FADC009BBD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795B60D1-861A-43DB-B47B-20E8F6BD2FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="259">
   <si>
     <t>Q</t>
   </si>
@@ -805,6 +805,15 @@
   </si>
   <si>
     <t>save period map</t>
+  </si>
+  <si>
+    <t>plot population</t>
+  </si>
+  <si>
+    <t>plot births</t>
+  </si>
+  <si>
+    <t>plot deaths</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1446,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC50" sqref="AC50"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1637,11 +1646,17 @@
         <v>147</v>
       </c>
       <c r="H6" s="21"/>
-      <c r="I6" s="22"/>
+      <c r="I6" s="22" t="s">
+        <v>256</v>
+      </c>
       <c r="J6" s="21"/>
-      <c r="K6" s="22"/>
+      <c r="K6" s="22" t="s">
+        <v>257</v>
+      </c>
       <c r="L6" s="21"/>
-      <c r="M6" s="22"/>
+      <c r="M6" s="22" t="s">
+        <v>258</v>
+      </c>
       <c r="N6" s="21"/>
       <c r="O6" s="22" t="s">
         <v>252</v>

</xml_diff>

<commit_message>
performance improvements to Identify, fixed newlines in waypoint messages
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795B60D1-861A-43DB-B47B-20E8F6BD2FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC2815E-A938-4184-BA4E-B231729F1D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="260">
   <si>
     <t>Q</t>
   </si>
@@ -814,6 +814,9 @@
   </si>
   <si>
     <t>plot deaths</t>
+  </si>
+  <si>
+    <t>help sections</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1449,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="AA27" sqref="AA27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1723,7 +1726,9 @@
         <v>84</v>
       </c>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="11"/>
+      <c r="AA7" s="11" t="s">
+        <v>259</v>
+      </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="11" t="s">
         <v>203</v>

</xml_diff>

<commit_message>
fixed a crash during pattern load, improved Identify Mod checking
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC2815E-A938-4184-BA4E-B231729F1D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE43A1C-31D5-477C-82E9-04CBA90811CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="259">
   <si>
     <t>Q</t>
   </si>
@@ -688,9 +688,6 @@
   </si>
   <si>
     <t>toggle identify</t>
-  </si>
-  <si>
-    <t>fast identify</t>
   </si>
   <si>
     <t>render quality</t>
@@ -1449,7 +1446,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1583,9 +1580,7 @@
       <c r="L4" s="35"/>
       <c r="M4" s="36"/>
       <c r="N4" s="35"/>
-      <c r="O4" s="36" t="s">
-        <v>217</v>
-      </c>
+      <c r="O4" s="36"/>
       <c r="P4" s="35"/>
       <c r="Q4" s="41" t="s">
         <v>192</v>
@@ -1650,19 +1645,19 @@
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="42"/>
@@ -1727,7 +1722,7 @@
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="11" t="s">
@@ -1940,7 +1935,7 @@
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22" t="s">
@@ -2128,7 +2123,7 @@
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="E16" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="34"/>
@@ -2156,7 +2151,7 @@
       </c>
       <c r="V16" s="35"/>
       <c r="W16" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X16" s="35"/>
       <c r="Y16" s="34"/>
@@ -2173,7 +2168,7 @@
       <c r="E17" s="32"/>
       <c r="F17" s="37"/>
       <c r="G17" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="32"/>
@@ -2191,7 +2186,7 @@
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="R17" s="37"/>
       <c r="S17" s="32"/>
@@ -2275,11 +2270,11 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="11" t="s">
@@ -2422,11 +2417,11 @@
       </c>
       <c r="H22" s="35"/>
       <c r="I22" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L22" s="35"/>
       <c r="M22" s="34" t="s">
@@ -2436,7 +2431,7 @@
       <c r="O22" s="34"/>
       <c r="P22" s="35"/>
       <c r="Q22" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R22" s="35"/>
       <c r="S22" s="34" t="s">
@@ -2444,7 +2439,7 @@
       </c>
       <c r="T22" s="35"/>
       <c r="U22" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="V22" s="35"/>
       <c r="W22" s="34"/>
@@ -2475,15 +2470,15 @@
       <c r="K23" s="29"/>
       <c r="L23" s="1"/>
       <c r="M23" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="31" t="s">
@@ -2516,7 +2511,7 @@
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J24" s="21"/>
       <c r="K24" s="20" t="s">
@@ -2546,7 +2541,7 @@
       <c r="W24" s="20"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Z24" s="21"/>
       <c r="AA24" s="20"/>
@@ -2567,11 +2562,11 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="11" t="s">
@@ -2597,7 +2592,7 @@
       <c r="W25" s="11"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="11"/>
@@ -2710,13 +2705,13 @@
       </c>
       <c r="L28" s="35"/>
       <c r="M28" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N28" s="35"/>
       <c r="O28" s="34"/>
       <c r="P28" s="35"/>
       <c r="Q28" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R28" s="35"/>
       <c r="S28" s="34"/>
@@ -2761,15 +2756,15 @@
       <c r="Q29" s="29"/>
       <c r="R29" s="1"/>
       <c r="S29" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="T29" s="1"/>
       <c r="U29" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X29" s="1"/>
       <c r="Y29" s="12"/>
@@ -2800,11 +2795,11 @@
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N30" s="21"/>
       <c r="O30" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="20" t="s">
@@ -2820,7 +2815,7 @@
       </c>
       <c r="V30" s="21"/>
       <c r="W30" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X30" s="21"/>
       <c r="Y30" s="25"/>
@@ -2871,7 +2866,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="13"/>
@@ -2904,7 +2899,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -3023,7 +3018,7 @@
       <c r="Y35" s="29"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="29"/>
@@ -3211,11 +3206,11 @@
     <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
@@ -3241,15 +3236,15 @@
       <c r="W41" s="2"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AD41" s="1"/>
     </row>
@@ -3278,11 +3273,11 @@
       <c r="M42" s="4"/>
       <c r="N42" s="21"/>
       <c r="O42" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R42" s="21"/>
       <c r="S42" s="21"/>

</xml_diff>

<commit_message>
added keyboard shortcuts for Mac, switched UI Icons to internal format
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77D42C2-D2D6-479E-B3CD-6021662F7FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AABA097-A499-4DFC-A6BC-6D5520A623D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31380" yWindow="780" windowWidth="24525" windowHeight="21255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -444,9 +444,6 @@
     <t>U</t>
   </si>
   <si>
-    <t>Alt</t>
-  </si>
-  <si>
     <t>command</t>
   </si>
   <si>
@@ -549,9 +546,6 @@
     <t>pan mode</t>
   </si>
   <si>
-    <t>Ctrl</t>
-  </si>
-  <si>
     <t>undo</t>
   </si>
   <si>
@@ -817,6 +811,12 @@
   </si>
   <si>
     <t>copy as MAP</t>
+  </si>
+  <si>
+    <t>Ctrl / Cmd</t>
+  </si>
+  <si>
+    <t>Alt / Option</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1449,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,27 +1523,27 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="2"/>
@@ -1586,7 +1586,7 @@
       <c r="O4" s="36"/>
       <c r="P4" s="35"/>
       <c r="Q4" s="41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R4" s="42"/>
       <c r="S4" s="42"/>
@@ -1600,7 +1600,7 @@
       <c r="AA4" s="34"/>
       <c r="AB4" s="35"/>
       <c r="AC4" s="34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1633,7 +1633,7 @@
       <c r="AA5" s="29"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1644,23 +1644,23 @@
       <c r="E6" s="22"/>
       <c r="F6" s="21"/>
       <c r="G6" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="42"/>
@@ -1676,7 +1676,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="21"/>
       <c r="AC6" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
@@ -1687,27 +1687,27 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="4"/>
@@ -1725,11 +1725,11 @@
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1828,43 +1828,43 @@
       <c r="C10" s="34"/>
       <c r="D10" s="35"/>
       <c r="E10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J10" s="35"/>
       <c r="K10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L10" s="35"/>
       <c r="M10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N10" s="35"/>
       <c r="O10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P10" s="35"/>
       <c r="Q10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R10" s="35"/>
       <c r="S10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="T10" s="35"/>
       <c r="U10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="V10" s="35"/>
       <c r="W10" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="X10" s="35"/>
       <c r="Y10" s="36"/>
@@ -1879,43 +1879,43 @@
       <c r="C11" s="29"/>
       <c r="D11" s="1"/>
       <c r="E11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="30"/>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22" t="s">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N12" s="21"/>
       <c r="O12" s="22" t="s">
@@ -1979,19 +1979,19 @@
       <c r="C13" s="11"/>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="10" t="s">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="10" t="s">
@@ -2007,7 +2007,7 @@
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="10" t="s">
@@ -2126,7 +2126,7 @@
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="E16" s="34" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="34"/>
@@ -2140,21 +2140,21 @@
       <c r="M16" s="34"/>
       <c r="N16" s="35"/>
       <c r="O16" s="34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="P16" s="35"/>
       <c r="Q16" s="34"/>
       <c r="R16" s="35"/>
       <c r="S16" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T16" s="35"/>
       <c r="U16" s="34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="V16" s="35"/>
       <c r="W16" s="34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="X16" s="35"/>
       <c r="Y16" s="34"/>
@@ -2171,35 +2171,35 @@
       <c r="E17" s="32"/>
       <c r="F17" s="37"/>
       <c r="G17" s="31" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="32"/>
       <c r="J17" s="37"/>
       <c r="K17" s="32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L17" s="37"/>
       <c r="M17" s="32" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N17" s="37"/>
       <c r="O17" s="32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="32" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="R17" s="37"/>
       <c r="S17" s="32"/>
       <c r="T17" s="37"/>
       <c r="U17" s="32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="V17" s="37"/>
       <c r="W17" s="32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="X17" s="37"/>
       <c r="Y17" s="32"/>
@@ -2218,7 +2218,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
       <c r="G18" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="20"/>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="P18" s="21"/>
       <c r="Q18" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R18" s="21"/>
       <c r="S18" s="20" t="s">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="V18" s="21"/>
       <c r="W18" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X18" s="21"/>
       <c r="Y18" s="20" t="s">
@@ -2273,11 +2273,11 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="11" t="s">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="11" t="s">
@@ -2412,37 +2412,37 @@
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F22" s="35"/>
       <c r="G22" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H22" s="35"/>
       <c r="I22" s="34" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L22" s="35"/>
       <c r="M22" s="34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N22" s="35"/>
       <c r="O22" s="34"/>
       <c r="P22" s="35"/>
       <c r="Q22" s="34" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="R22" s="35"/>
       <c r="S22" s="34" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T22" s="35"/>
       <c r="U22" s="34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="V22" s="35"/>
       <c r="W22" s="34"/>
@@ -2459,37 +2459,37 @@
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
       <c r="E23" s="32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="29"/>
       <c r="L23" s="1"/>
       <c r="M23" s="31" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="31" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="31" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="29"/>
@@ -2506,7 +2506,7 @@
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="20" t="s">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J24" s="21"/>
       <c r="K24" s="20" t="s">
@@ -2534,17 +2534,17 @@
       </c>
       <c r="R24" s="21"/>
       <c r="S24" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T24" s="21"/>
       <c r="U24" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="V24" s="21"/>
       <c r="W24" s="20"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Z24" s="21"/>
       <c r="AA24" s="20"/>
@@ -2565,11 +2565,11 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="11" t="s">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T25" s="1"/>
       <c r="U25" s="11" t="s">
@@ -2595,7 +2595,7 @@
       <c r="W25" s="11"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="11"/>
@@ -2692,29 +2692,29 @@
       <c r="C28" s="34"/>
       <c r="D28" s="35"/>
       <c r="E28" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F28" s="35"/>
       <c r="G28" s="34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H28" s="35"/>
       <c r="I28" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J28" s="35"/>
       <c r="K28" s="34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L28" s="35"/>
       <c r="M28" s="34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N28" s="35"/>
       <c r="O28" s="34"/>
       <c r="P28" s="35"/>
       <c r="Q28" s="34" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R28" s="35"/>
       <c r="S28" s="34"/>
@@ -2735,11 +2735,11 @@
       <c r="C29" s="29"/>
       <c r="D29" s="1"/>
       <c r="E29" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="31" t="s">
@@ -2749,27 +2749,27 @@
       <c r="K29" s="29"/>
       <c r="L29" s="1"/>
       <c r="M29" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="T29" s="1"/>
       <c r="U29" s="31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="X29" s="1"/>
       <c r="Y29" s="12"/>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="H30" s="21"/>
       <c r="I30" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J30" s="21"/>
       <c r="K30" s="20" t="s">
@@ -2800,15 +2800,15 @@
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N30" s="21"/>
       <c r="O30" s="20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="R30" s="21"/>
       <c r="S30" s="20" t="s">
@@ -2820,7 +2820,7 @@
       </c>
       <c r="V30" s="21"/>
       <c r="W30" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="X30" s="21"/>
       <c r="Y30" s="25"/>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="13"/>
@@ -2904,7 +2904,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -2917,15 +2917,15 @@
     <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="9" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="9" t="s">
-        <v>135</v>
+        <v>259</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="14" t="s">
@@ -2964,13 +2964,13 @@
       <c r="C34" s="29"/>
       <c r="D34" s="1"/>
       <c r="E34" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="32"/>
       <c r="H34" s="1"/>
       <c r="I34" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J34" s="38"/>
       <c r="K34" s="38"/>
@@ -3001,7 +3001,7 @@
       <c r="E35" s="34"/>
       <c r="F35" s="1"/>
       <c r="G35" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="40"/>
@@ -3023,7 +3023,7 @@
       <c r="Y35" s="29"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="29"/>
@@ -3032,7 +3032,7 @@
     <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="34"/>
@@ -3040,7 +3040,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="21"/>
       <c r="I36" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J36" s="27"/>
       <c r="K36" s="27"/>
@@ -3058,7 +3058,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="21"/>
       <c r="Y36" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z36" s="21"/>
       <c r="AA36" s="20" t="s">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="AB36" s="21"/>
       <c r="AC36" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD36" s="1"/>
     </row>
@@ -3211,21 +3211,21 @@
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="33" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
       <c r="H41" s="1"/>
       <c r="I41" s="33" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
@@ -3241,48 +3241,48 @@
       <c r="W41" s="2"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41" s="32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AD41" s="1"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E42" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="21"/>
       <c r="O42" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="R42" s="21"/>
       <c r="S42" s="21"/>
@@ -3307,33 +3307,33 @@
     <row r="43" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="4"/>
       <c r="O43" s="33" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>

</xml_diff>

<commit_message>
support drag and drop of pattern files onto canvas for LifeViewer home page
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AABA097-A499-4DFC-A6BC-6D5520A623D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642B608E-2722-4D7D-BED9-92AC746A3D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="780" windowWidth="24525" windowHeight="21255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="1230" windowWidth="29100" windowHeight="21255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="263">
   <si>
     <t>Q</t>
   </si>
@@ -609,9 +609,6 @@
     <t>paste to selection</t>
   </si>
   <si>
-    <t>LifeViewer Keyboard Controls</t>
-  </si>
-  <si>
     <t>paste location</t>
   </si>
   <si>
@@ -817,13 +814,25 @@
   </si>
   <si>
     <t>Alt / Option</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>toggle y direction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,13 +871,6 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="0.59999389629810485"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1058,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1160,12 +1162,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1449,39 +1446,39 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="AG22" sqref="AF22:AG22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="0.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="0.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="0.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="0.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="0.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="0.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
     <col min="16" max="16" width="0.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
     <col min="18" max="18" width="0.42578125" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
     <col min="20" max="20" width="0.42578125" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
     <col min="22" max="22" width="0.42578125" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" customWidth="1"/>
     <col min="24" max="24" width="0.42578125" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" customWidth="1"/>
     <col min="26" max="26" width="0.42578125" customWidth="1"/>
-    <col min="27" max="27" width="13.7109375" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" customWidth="1"/>
     <col min="28" max="28" width="0.42578125" customWidth="1"/>
-    <col min="29" max="29" width="13.7109375" customWidth="1"/>
+    <col min="29" max="29" width="15.7109375" customWidth="1"/>
     <col min="30" max="30" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1543,14 +1540,20 @@
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="2"/>
+      <c r="Q3" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="R3" s="41"/>
+      <c r="S3" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="T3" s="41"/>
+      <c r="U3" s="7" t="s">
+        <v>261</v>
+      </c>
       <c r="V3" s="1"/>
       <c r="W3" s="9" t="s">
         <v>76</v>
@@ -1585,13 +1588,11 @@
       <c r="N4" s="35"/>
       <c r="O4" s="36"/>
       <c r="P4" s="35"/>
-      <c r="Q4" s="41" t="s">
-        <v>190</v>
-      </c>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="36"/>
       <c r="V4" s="35"/>
       <c r="W4" s="34"/>
       <c r="X4" s="35"/>
@@ -1600,7 +1601,7 @@
       <c r="AA4" s="34"/>
       <c r="AB4" s="35"/>
       <c r="AC4" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
@@ -1620,11 +1621,11 @@
       <c r="N5" s="1"/>
       <c r="O5" s="30"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="30"/>
       <c r="V5" s="1"/>
       <c r="W5" s="29"/>
       <c r="X5" s="1"/>
@@ -1633,7 +1634,7 @@
       <c r="AA5" s="29"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
@@ -1648,26 +1649,28 @@
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P6" s="21"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
+      <c r="Q6" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="R6" s="41"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="22"/>
       <c r="V6" s="21"/>
       <c r="W6" s="20"/>
       <c r="X6" s="21"/>
@@ -1676,7 +1679,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="21"/>
       <c r="AC6" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
@@ -1707,14 +1710,20 @@
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="4"/>
+      <c r="Q7" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="R7" s="41"/>
+      <c r="S7" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="T7" s="41"/>
+      <c r="U7" s="10" t="s">
+        <v>262</v>
+      </c>
       <c r="V7" s="1"/>
       <c r="W7" s="11" t="s">
         <v>83</v>
@@ -1725,11 +1734,11 @@
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
@@ -1828,43 +1837,43 @@
       <c r="C10" s="34"/>
       <c r="D10" s="35"/>
       <c r="E10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J10" s="35"/>
       <c r="K10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L10" s="35"/>
       <c r="M10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N10" s="35"/>
       <c r="O10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P10" s="35"/>
       <c r="Q10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="R10" s="35"/>
       <c r="S10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T10" s="35"/>
       <c r="U10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="V10" s="35"/>
       <c r="W10" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="X10" s="35"/>
       <c r="Y10" s="36"/>
@@ -1879,43 +1888,43 @@
       <c r="C11" s="29"/>
       <c r="D11" s="1"/>
       <c r="E11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="30"/>
@@ -1938,7 +1947,7 @@
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22" t="s">
@@ -2126,7 +2135,7 @@
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="E16" s="34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="34"/>
@@ -2154,7 +2163,7 @@
       </c>
       <c r="V16" s="35"/>
       <c r="W16" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X16" s="35"/>
       <c r="Y16" s="34"/>
@@ -2171,7 +2180,7 @@
       <c r="E17" s="32"/>
       <c r="F17" s="37"/>
       <c r="G17" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="32"/>
@@ -2181,7 +2190,7 @@
       </c>
       <c r="L17" s="37"/>
       <c r="M17" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N17" s="37"/>
       <c r="O17" s="32" t="s">
@@ -2189,17 +2198,17 @@
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R17" s="37"/>
       <c r="S17" s="32"/>
       <c r="T17" s="37"/>
       <c r="U17" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="V17" s="37"/>
       <c r="W17" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X17" s="37"/>
       <c r="Y17" s="32"/>
@@ -2218,7 +2227,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
       <c r="G18" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="20"/>
@@ -2273,11 +2282,11 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="11" t="s">
@@ -2293,7 +2302,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="11" t="s">
@@ -2420,21 +2429,21 @@
       </c>
       <c r="H22" s="35"/>
       <c r="I22" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L22" s="35"/>
       <c r="M22" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N22" s="35"/>
       <c r="O22" s="34"/>
       <c r="P22" s="35"/>
       <c r="Q22" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="R22" s="35"/>
       <c r="S22" s="34" t="s">
@@ -2442,7 +2451,7 @@
       </c>
       <c r="T22" s="35"/>
       <c r="U22" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="V22" s="35"/>
       <c r="W22" s="34"/>
@@ -2467,25 +2476,25 @@
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="29"/>
       <c r="L23" s="1"/>
       <c r="M23" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T23" s="1"/>
       <c r="U23" s="31" t="s">
@@ -2506,7 +2515,7 @@
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="20" t="s">
@@ -2514,7 +2523,7 @@
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J24" s="21"/>
       <c r="K24" s="20" t="s">
@@ -2538,13 +2547,13 @@
       </c>
       <c r="T24" s="21"/>
       <c r="U24" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="V24" s="21"/>
       <c r="W24" s="20"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Z24" s="21"/>
       <c r="AA24" s="20"/>
@@ -2565,11 +2574,11 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="11" t="s">
@@ -2595,7 +2604,7 @@
       <c r="W25" s="11"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="11"/>
@@ -2708,13 +2717,13 @@
       </c>
       <c r="L28" s="35"/>
       <c r="M28" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N28" s="35"/>
       <c r="O28" s="34"/>
       <c r="P28" s="35"/>
       <c r="Q28" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R28" s="35"/>
       <c r="S28" s="34"/>
@@ -2735,7 +2744,7 @@
       <c r="C29" s="29"/>
       <c r="D29" s="1"/>
       <c r="E29" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="31" t="s">
@@ -2757,19 +2766,19 @@
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="T29" s="1"/>
       <c r="U29" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X29" s="1"/>
       <c r="Y29" s="12"/>
@@ -2800,15 +2809,15 @@
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N30" s="21"/>
       <c r="O30" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R30" s="21"/>
       <c r="S30" s="20" t="s">
@@ -2820,7 +2829,7 @@
       </c>
       <c r="V30" s="21"/>
       <c r="W30" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="X30" s="21"/>
       <c r="Y30" s="25"/>
@@ -2871,7 +2880,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="13"/>
@@ -2904,7 +2913,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -2921,11 +2930,11 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="14" t="s">
@@ -2970,7 +2979,7 @@
       <c r="G34" s="32"/>
       <c r="H34" s="1"/>
       <c r="I34" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J34" s="38"/>
       <c r="K34" s="38"/>
@@ -3023,7 +3032,7 @@
       <c r="Y35" s="29"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="29"/>
@@ -3040,7 +3049,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="21"/>
       <c r="I36" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J36" s="27"/>
       <c r="K36" s="27"/>
@@ -3211,11 +3220,11 @@
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
@@ -3241,15 +3250,15 @@
       <c r="W41" s="2"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD41" s="1"/>
     </row>
@@ -3278,11 +3287,11 @@
       <c r="M42" s="4"/>
       <c r="N42" s="21"/>
       <c r="O42" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R42" s="21"/>
       <c r="S42" s="21"/>
@@ -3329,11 +3338,11 @@
       <c r="M43" s="1"/>
       <c r="N43" s="4"/>
       <c r="O43" s="33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
@@ -3387,9 +3396,6 @@
       <c r="AD44" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="Q4:U6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
@ICONS renderer initial work
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642B608E-2722-4D7D-BED9-92AC746A3D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AA0DB0-B4A0-4F5F-A5E1-6DCEF823A0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="1230" windowWidth="29100" windowHeight="21255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="264">
   <si>
     <t>Q</t>
   </si>
@@ -826,6 +826,9 @@
   </si>
   <si>
     <t>toggle y direction</t>
+  </si>
+  <si>
+    <t>toggle icons</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1063,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1162,7 +1165,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1446,7 +1448,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG22" sqref="AF22:AG22"/>
+      <selection activeCell="S54" sqref="S54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,11 +1548,11 @@
       <c r="Q3" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="R3" s="41"/>
+      <c r="R3" s="1"/>
       <c r="S3" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="T3" s="41"/>
+      <c r="T3" s="1"/>
       <c r="U3" s="7" t="s">
         <v>261</v>
       </c>
@@ -1589,9 +1591,9 @@
       <c r="O4" s="36"/>
       <c r="P4" s="35"/>
       <c r="Q4" s="36"/>
-      <c r="R4" s="41"/>
+      <c r="R4" s="1"/>
       <c r="S4" s="36"/>
-      <c r="T4" s="41"/>
+      <c r="T4" s="1"/>
       <c r="U4" s="36"/>
       <c r="V4" s="35"/>
       <c r="W4" s="34"/>
@@ -1622,9 +1624,9 @@
       <c r="O5" s="30"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="41"/>
+      <c r="R5" s="1"/>
       <c r="S5" s="30"/>
-      <c r="T5" s="41"/>
+      <c r="T5" s="1"/>
       <c r="U5" s="30"/>
       <c r="V5" s="1"/>
       <c r="W5" s="29"/>
@@ -1667,9 +1669,9 @@
       <c r="Q6" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="R6" s="41"/>
+      <c r="R6" s="1"/>
       <c r="S6" s="22"/>
-      <c r="T6" s="41"/>
+      <c r="T6" s="1"/>
       <c r="U6" s="22"/>
       <c r="V6" s="21"/>
       <c r="W6" s="20"/>
@@ -1716,11 +1718,11 @@
       <c r="Q7" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="R7" s="41"/>
+      <c r="R7" s="1"/>
       <c r="S7" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="T7" s="41"/>
+      <c r="T7" s="1"/>
       <c r="U7" s="10" t="s">
         <v>262</v>
       </c>
@@ -2201,7 +2203,9 @@
         <v>235</v>
       </c>
       <c r="R17" s="37"/>
-      <c r="S17" s="32"/>
+      <c r="S17" s="32" t="s">
+        <v>263</v>
+      </c>
       <c r="T17" s="37"/>
       <c r="U17" s="32" t="s">
         <v>206</v>

</xml_diff>

<commit_message>
improved handling of different monitor refresh rates
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AA0DB0-B4A0-4F5F-A5E1-6DCEF823A0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9B9409-0814-4EC0-A722-50C56044E688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15900" yWindow="3180" windowWidth="41700" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="265">
   <si>
     <t>Q</t>
   </si>
@@ -829,6 +829,9 @@
   </si>
   <si>
     <t>toggle icons</t>
+  </si>
+  <si>
+    <t>b+w capture</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1451,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S54" sqref="S54"/>
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2605,7 +2608,9 @@
         <v>66</v>
       </c>
       <c r="V25" s="1"/>
-      <c r="W25" s="11"/>
+      <c r="W25" s="11" t="s">
+        <v>264</v>
+      </c>
       <c r="X25" s="1"/>
       <c r="Y25" s="11" t="s">
         <v>240</v>

</xml_diff>

<commit_message>
added option to force 60Hz refresh rate, attempted fix for RS browser
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9B9409-0814-4EC0-A722-50C56044E688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A16E997-2CE6-4B2F-8D9E-AE4479ED27C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="3180" windowWidth="41700" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2445" windowWidth="27885" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="266">
   <si>
     <t>Q</t>
   </si>
@@ -832,6 +832,9 @@
   </si>
   <si>
     <t>b+w capture</t>
+  </si>
+  <si>
+    <t>toggle force 60Hz</t>
   </si>
 </sst>
 </file>
@@ -1450,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,7 +2240,9 @@
         <v>194</v>
       </c>
       <c r="H18" s="21"/>
-      <c r="I18" s="20"/>
+      <c r="I18" s="20" t="s">
+        <v>265</v>
+      </c>
       <c r="J18" s="21"/>
       <c r="K18" s="20" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
you can now set the default playback speed
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A16E997-2CE6-4B2F-8D9E-AE4479ED27C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A7C8F0-EBB1-4032-90B8-36038A691D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2445" windowWidth="27885" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7215" yWindow="6150" windowWidth="27885" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -834,7 +834,7 @@
     <t>b+w capture</t>
   </si>
   <si>
-    <t>toggle force 60Hz</t>
+    <t>toggle speed</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1454,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added Cell Frequency Map and fixed cells disappearing sometimes when changing Themes
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299B51A4-2E80-4D8E-B095-077FFB3D6BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCE973E-2D8C-43E3-BEDB-0322F14E71C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34020" yWindow="4980" windowWidth="20040" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6555" yWindow="3075" windowWidth="31065" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="267">
   <si>
     <t>Q</t>
   </si>
@@ -720,9 +720,6 @@
     <t>copy nbrhood</t>
   </si>
   <si>
-    <t>toggle rainbow</t>
-  </si>
-  <si>
     <t>toggle kill gliders</t>
   </si>
   <si>
@@ -786,15 +783,6 @@
     <t>last identify</t>
   </si>
   <si>
-    <t>period map</t>
-  </si>
-  <si>
-    <t>period table</t>
-  </si>
-  <si>
-    <t>save period map</t>
-  </si>
-  <si>
     <t>plot population</t>
   </si>
   <si>
@@ -841,6 +829,15 @@
   </si>
   <si>
     <t>toggle maximize</t>
+  </si>
+  <si>
+    <t>cycle shader</t>
+  </si>
+  <si>
+    <t>cycle identify</t>
+  </si>
+  <si>
+    <t>save cell map</t>
   </si>
 </sst>
 </file>
@@ -1459,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH46" sqref="AH46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,15 +1555,15 @@
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="9" t="s">
@@ -1663,31 +1660,31 @@
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="22" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="22" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="22" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="22" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="22" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="V6" s="21"/>
       <c r="W6" s="20"/>
@@ -1736,11 +1733,11 @@
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="10" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="11" t="s">
@@ -1752,7 +1749,7 @@
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="11" t="s">
@@ -1965,7 +1962,7 @@
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22" t="s">
@@ -2181,7 +2178,7 @@
       </c>
       <c r="V16" s="35"/>
       <c r="W16" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X16" s="35"/>
       <c r="Y16" s="34"/>
@@ -2198,7 +2195,7 @@
       <c r="E17" s="32"/>
       <c r="F17" s="37"/>
       <c r="G17" s="31" t="s">
-        <v>227</v>
+        <v>264</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="32"/>
@@ -2216,11 +2213,11 @@
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R17" s="37"/>
       <c r="S17" s="32" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="T17" s="37"/>
       <c r="U17" s="32" t="s">
@@ -2251,7 +2248,7 @@
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="20" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="J18" s="21"/>
       <c r="K18" s="20" t="s">
@@ -2304,11 +2301,11 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="11" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="11" t="s">
@@ -2451,7 +2448,7 @@
       </c>
       <c r="H22" s="35"/>
       <c r="I22" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="34" t="s">
@@ -2465,7 +2462,7 @@
       <c r="O22" s="34"/>
       <c r="P22" s="35"/>
       <c r="Q22" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R22" s="35"/>
       <c r="S22" s="34" t="s">
@@ -2473,7 +2470,7 @@
       </c>
       <c r="T22" s="35"/>
       <c r="U22" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="V22" s="35"/>
       <c r="W22" s="34"/>
@@ -2504,15 +2501,15 @@
       <c r="K23" s="29"/>
       <c r="L23" s="1"/>
       <c r="M23" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="31" t="s">
@@ -2544,9 +2541,7 @@
         <v>127</v>
       </c>
       <c r="H24" s="21"/>
-      <c r="I24" s="20" t="s">
-        <v>251</v>
-      </c>
+      <c r="I24" s="20"/>
       <c r="J24" s="21"/>
       <c r="K24" s="20" t="s">
         <v>94</v>
@@ -2575,7 +2570,7 @@
       <c r="W24" s="20"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Z24" s="21"/>
       <c r="AA24" s="20"/>
@@ -2596,7 +2591,7 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="11" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="11" t="s">
@@ -2624,11 +2619,11 @@
       </c>
       <c r="V25" s="1"/>
       <c r="W25" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="X25" s="1"/>
       <c r="Y25" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="11"/>
@@ -2790,19 +2785,19 @@
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="31" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T29" s="1"/>
       <c r="U29" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="X29" s="1"/>
       <c r="Y29" s="12"/>
@@ -2833,11 +2828,11 @@
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N30" s="21"/>
       <c r="O30" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="20" t="s">
@@ -2853,7 +2848,7 @@
       </c>
       <c r="V30" s="21"/>
       <c r="W30" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X30" s="21"/>
       <c r="Y30" s="25"/>
@@ -2904,7 +2899,7 @@
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X31" s="1"/>
       <c r="Y31" s="13"/>
@@ -2937,7 +2932,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -2954,11 +2949,11 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="9" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="9" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="14" t="s">

</xml_diff>

<commit_message>
improvements to Identify Oscillator output, fixed Save Pattern removing new lines
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCE973E-2D8C-43E3-BEDB-0322F14E71C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C3E7C7-8FA8-4B3F-9BE8-4C22684554B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="3075" windowWidth="31065" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="3810" windowWidth="20040" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="268">
   <si>
     <t>Q</t>
   </si>
@@ -834,10 +834,13 @@
     <t>cycle shader</t>
   </si>
   <si>
-    <t>cycle identify</t>
-  </si>
-  <si>
     <t>save cell map</t>
+  </si>
+  <si>
+    <t>identify mode</t>
+  </si>
+  <si>
+    <t>identify type</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1460,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH46" sqref="AH46"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,7 +2201,9 @@
         <v>264</v>
       </c>
       <c r="H17" s="37"/>
-      <c r="I17" s="32"/>
+      <c r="I17" s="32" t="s">
+        <v>267</v>
+      </c>
       <c r="J17" s="37"/>
       <c r="K17" s="32" t="s">
         <v>181</v>
@@ -2305,7 +2310,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="11" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="11" t="s">
@@ -2591,7 +2596,7 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="11" t="s">

</xml_diff>

<commit_message>
F7 will now copy selection as headerless RLE including blank cells, various fixes
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C3E7C7-8FA8-4B3F-9BE8-4C22684554B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ECB76F-86F7-406B-90E7-E4850C5EBE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="3810" windowWidth="20040" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="271">
   <si>
     <t>Q</t>
   </si>
@@ -841,6 +841,15 @@
   </si>
   <si>
     <t>identify type</t>
+  </si>
+  <si>
+    <t>toggle lookup</t>
+  </si>
+  <si>
+    <t>copy with blanks</t>
+  </si>
+  <si>
+    <t>copy no newline</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1469,7 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="AJ30" sqref="AJ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,7 +1644,9 @@
       <c r="N5" s="1"/>
       <c r="O5" s="30"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="30"/>
+      <c r="Q5" s="31" t="s">
+        <v>270</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="30"/>
       <c r="T5" s="1"/>
@@ -1679,7 +1690,7 @@
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="22" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="22" t="s">
@@ -1732,7 +1743,7 @@
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="10" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="10" t="s">

</xml_diff>

<commit_message>
changed hotkey Tab to Backslash to allow page navigation
</commit_message>
<xml_diff>
--- a/images/hotkeys.xlsx
+++ b/images/hotkeys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crowe\Documents\GitHub\lifeviewer\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ECB76F-86F7-406B-90E7-E4850C5EBE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3471E4A-049F-49F7-8634-0971CBF8E7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="2" r:id="rId1"/>
@@ -1084,13 +1084,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1469,43 +1468,43 @@
   <dimension ref="B2:AD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ30" sqref="AJ30"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="0.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="0.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="0.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="0.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="0.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="0.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="0.42578125" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="0.42578125" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="0.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" customWidth="1"/>
-    <col min="22" max="22" width="0.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" customWidth="1"/>
-    <col min="24" max="24" width="0.42578125" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" customWidth="1"/>
-    <col min="26" max="26" width="0.42578125" customWidth="1"/>
-    <col min="27" max="27" width="15.7109375" customWidth="1"/>
-    <col min="28" max="28" width="0.42578125" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" customWidth="1"/>
-    <col min="30" max="30" width="2.7109375" customWidth="1"/>
+    <col min="1" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="0.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="0.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="0.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="0.44140625" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="0.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="0.44140625" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" customWidth="1"/>
+    <col min="16" max="16" width="0.44140625" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="0.44140625" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="0.44140625" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" customWidth="1"/>
+    <col min="22" max="22" width="0.44140625" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" customWidth="1"/>
+    <col min="24" max="24" width="0.44140625" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" customWidth="1"/>
+    <col min="26" max="26" width="0.44140625" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" customWidth="1"/>
+    <col min="28" max="28" width="0.44140625" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" customWidth="1"/>
+    <col min="30" max="30" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1536,242 +1535,242 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>145</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>161</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>162</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>163</v>
       </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>164</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6" t="s">
         <v>212</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="6" t="s">
         <v>255</v>
       </c>
       <c r="R3" s="1"/>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="6" t="s">
         <v>256</v>
       </c>
       <c r="T3" s="1"/>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="6" t="s">
         <v>257</v>
       </c>
       <c r="V3" s="1"/>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="8" t="s">
         <v>76</v>
       </c>
       <c r="X3" s="1"/>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="8" t="s">
         <v>77</v>
       </c>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="9" t="s">
+      <c r="AA3" s="8" t="s">
         <v>78</v>
       </c>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="9" t="s">
+      <c r="AC3" s="8" t="s">
         <v>79</v>
       </c>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="36"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="35"/>
       <c r="R4" s="1"/>
-      <c r="S4" s="36"/>
+      <c r="S4" s="35"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="35"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="34" t="s">
+      <c r="U4" s="35"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="33" t="s">
         <v>192</v>
       </c>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
-      <c r="C5" s="30"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="30"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="30"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="30"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="30"/>
+      <c r="K5" s="29"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="30"/>
+      <c r="M5" s="29"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="30"/>
+      <c r="O5" s="29"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="31" t="s">
+      <c r="Q5" s="30" t="s">
         <v>270</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="30"/>
+      <c r="S5" s="29"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="30"/>
+      <c r="U5" s="29"/>
       <c r="V5" s="1"/>
-      <c r="W5" s="29"/>
+      <c r="W5" s="28"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="29"/>
+      <c r="Y5" s="28"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="29"/>
+      <c r="AA5" s="28"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="31" t="s">
+      <c r="AC5" s="30" t="s">
         <v>205</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="22" t="s">
+      <c r="H6" s="20"/>
+      <c r="I6" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="20"/>
+      <c r="K6" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="22" t="s">
+      <c r="L6" s="20"/>
+      <c r="M6" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="22" t="s">
+      <c r="N6" s="20"/>
+      <c r="O6" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="22" t="s">
+      <c r="P6" s="20"/>
+      <c r="Q6" s="21" t="s">
         <v>268</v>
       </c>
       <c r="R6" s="1"/>
-      <c r="S6" s="22" t="s">
+      <c r="S6" s="21" t="s">
         <v>258</v>
       </c>
       <c r="T6" s="1"/>
-      <c r="U6" s="22" t="s">
+      <c r="U6" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="V6" s="21"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="20"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="20" t="s">
+      <c r="V6" s="20"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="19" t="s">
         <v>195</v>
       </c>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>109</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>165</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>167</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="9" t="s">
         <v>166</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>168</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="9" t="s">
         <v>213</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="9" t="s">
         <v>269</v>
       </c>
       <c r="R7" s="1"/>
-      <c r="S7" s="10" t="s">
+      <c r="S7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="T7" s="1"/>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="9" t="s">
         <v>263</v>
       </c>
       <c r="V7" s="1"/>
-      <c r="W7" s="11" t="s">
+      <c r="W7" s="10" t="s">
         <v>83</v>
       </c>
       <c r="X7" s="1"/>
-      <c r="Y7" s="11" t="s">
+      <c r="Y7" s="10" t="s">
         <v>84</v>
       </c>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="11" t="s">
+      <c r="AA7" s="10" t="s">
         <v>251</v>
       </c>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="11" t="s">
+      <c r="AC7" s="10" t="s">
         <v>200</v>
       </c>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1802,274 +1801,274 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="7" t="s">
         <v>29</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="7" t="s">
+      <c r="O9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P9" s="1"/>
-      <c r="Q9" s="7" t="s">
+      <c r="Q9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="7" t="s">
+      <c r="S9" s="6" t="s">
         <v>32</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="7" t="s">
+      <c r="U9" s="6" t="s">
         <v>33</v>
       </c>
       <c r="V9" s="1"/>
-      <c r="W9" s="7" t="s">
+      <c r="W9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="X9" s="1"/>
-      <c r="Y9" s="7" t="s">
+      <c r="Y9" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="7" t="s">
+      <c r="AA9" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AB9" s="1"/>
-      <c r="AC9" s="9" t="s">
+      <c r="AC9" s="8" t="s">
         <v>82</v>
       </c>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="36" t="s">
+      <c r="F10" s="34"/>
+      <c r="G10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="36" t="s">
+      <c r="H10" s="34"/>
+      <c r="I10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36" t="s">
+      <c r="J10" s="34"/>
+      <c r="K10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="36" t="s">
+      <c r="L10" s="34"/>
+      <c r="M10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="N10" s="35"/>
-      <c r="O10" s="36" t="s">
+      <c r="N10" s="34"/>
+      <c r="O10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="36" t="s">
+      <c r="P10" s="34"/>
+      <c r="Q10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="R10" s="35"/>
-      <c r="S10" s="36" t="s">
+      <c r="R10" s="34"/>
+      <c r="S10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="T10" s="35"/>
-      <c r="U10" s="36" t="s">
+      <c r="T10" s="34"/>
+      <c r="U10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="V10" s="35"/>
-      <c r="W10" s="36" t="s">
+      <c r="V10" s="34"/>
+      <c r="W10" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="35"/>
-      <c r="AA10" s="36"/>
-      <c r="AB10" s="35"/>
-      <c r="AC10" s="34"/>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="33"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="29"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="31" t="s">
+      <c r="K11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="31" t="s">
+      <c r="M11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="31" t="s">
+      <c r="O11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="P11" s="1"/>
-      <c r="Q11" s="31" t="s">
+      <c r="Q11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="R11" s="1"/>
-      <c r="S11" s="31" t="s">
+      <c r="S11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="T11" s="1"/>
-      <c r="U11" s="31" t="s">
+      <c r="U11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="V11" s="1"/>
-      <c r="W11" s="31" t="s">
+      <c r="W11" s="30" t="s">
         <v>203</v>
       </c>
       <c r="X11" s="1"/>
-      <c r="Y11" s="30"/>
+      <c r="Y11" s="29"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="30"/>
+      <c r="AA11" s="29"/>
       <c r="AB11" s="1"/>
-      <c r="AC11" s="29"/>
+      <c r="AC11" s="28"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22" t="s">
+      <c r="F12" s="20"/>
+      <c r="G12" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="22" t="s">
+      <c r="H12" s="20"/>
+      <c r="I12" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22" t="s">
+      <c r="J12" s="20"/>
+      <c r="K12" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="21"/>
-      <c r="M12" s="23" t="s">
+      <c r="L12" s="20"/>
+      <c r="M12" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="N12" s="21"/>
-      <c r="O12" s="22" t="s">
+      <c r="N12" s="20"/>
+      <c r="O12" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="22" t="s">
+      <c r="P12" s="20"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="T12" s="21"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="22" t="s">
+      <c r="T12" s="20"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="22" t="s">
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="AB12" s="21"/>
-      <c r="AC12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="19"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>149</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>150</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>151</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="9" t="s">
         <v>152</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="10" t="s">
+      <c r="M13" s="9" t="s">
         <v>91</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="10" t="s">
+      <c r="O13" s="9" t="s">
         <v>153</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="Q13" s="10" t="s">
+      <c r="Q13" s="9" t="s">
         <v>131</v>
       </c>
       <c r="R13" s="1"/>
-      <c r="S13" s="10" t="s">
+      <c r="S13" s="9" t="s">
         <v>154</v>
       </c>
       <c r="T13" s="1"/>
-      <c r="U13" s="10" t="s">
+      <c r="U13" s="9" t="s">
         <v>130</v>
       </c>
       <c r="V13" s="1"/>
-      <c r="W13" s="10" t="s">
+      <c r="W13" s="9" t="s">
         <v>126</v>
       </c>
       <c r="X13" s="1"/>
-      <c r="Y13" s="10" t="s">
+      <c r="Y13" s="9" t="s">
         <v>48</v>
       </c>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="10" t="s">
+      <c r="AA13" s="9" t="s">
         <v>49</v>
       </c>
       <c r="AB13" s="1"/>
-      <c r="AC13" s="11" t="s">
+      <c r="AC13" s="10" t="s">
         <v>113</v>
       </c>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2100,272 +2099,268 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>75</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="9" t="s">
+      <c r="M15" s="8" t="s">
         <v>4</v>
       </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="9" t="s">
+      <c r="O15" s="8" t="s">
         <v>5</v>
       </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="9" t="s">
+      <c r="Q15" s="8" t="s">
         <v>134</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="9" t="s">
+      <c r="S15" s="8" t="s">
         <v>6</v>
       </c>
       <c r="T15" s="1"/>
-      <c r="U15" s="9" t="s">
+      <c r="U15" s="8" t="s">
         <v>7</v>
       </c>
       <c r="V15" s="1"/>
-      <c r="W15" s="9" t="s">
+      <c r="W15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="X15" s="1"/>
-      <c r="Y15" s="9" t="s">
+      <c r="Y15" s="8" t="s">
         <v>37</v>
       </c>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="9" t="s">
+      <c r="AA15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="9" t="s">
+      <c r="AC15" s="8" t="s">
         <v>46</v>
       </c>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="34" t="s">
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="34" t="s">
+      <c r="F16" s="34"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="34" t="s">
+      <c r="L16" s="34"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="34" t="s">
+      <c r="P16" s="34"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="T16" s="35"/>
-      <c r="U16" s="34" t="s">
+      <c r="T16" s="34"/>
+      <c r="U16" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="V16" s="35"/>
-      <c r="W16" s="34" t="s">
+      <c r="V16" s="34"/>
+      <c r="W16" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="34"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="34"/>
+      <c r="X16" s="34"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="34"/>
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="34"/>
+      <c r="AC16" s="33"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="31" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="32" t="s">
+      <c r="H17" s="36"/>
+      <c r="I17" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="J17" s="37"/>
-      <c r="K17" s="32" t="s">
+      <c r="J17" s="36"/>
+      <c r="K17" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="L17" s="37"/>
-      <c r="M17" s="32" t="s">
+      <c r="L17" s="36"/>
+      <c r="M17" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="N17" s="37"/>
-      <c r="O17" s="32" t="s">
+      <c r="N17" s="36"/>
+      <c r="O17" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="32" t="s">
+      <c r="P17" s="36"/>
+      <c r="Q17" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="R17" s="37"/>
-      <c r="S17" s="32" t="s">
+      <c r="R17" s="36"/>
+      <c r="S17" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="T17" s="37"/>
-      <c r="U17" s="32" t="s">
+      <c r="T17" s="36"/>
+      <c r="U17" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="V17" s="37"/>
-      <c r="W17" s="32" t="s">
+      <c r="V17" s="36"/>
+      <c r="W17" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="37"/>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="37"/>
-      <c r="AC17" s="32"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="31"/>
+      <c r="AB17" s="36"/>
+      <c r="AC17" s="31"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="20" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="20" t="s">
+      <c r="H18" s="20"/>
+      <c r="I18" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="20" t="s">
+      <c r="J18" s="20"/>
+      <c r="K18" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="20" t="s">
+      <c r="L18" s="20"/>
+      <c r="M18" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="N18" s="21"/>
-      <c r="O18" s="20" t="s">
+      <c r="N18" s="20"/>
+      <c r="O18" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="20" t="s">
+      <c r="P18" s="20"/>
+      <c r="Q18" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="R18" s="21"/>
-      <c r="S18" s="20" t="s">
+      <c r="R18" s="20"/>
+      <c r="S18" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="T18" s="21"/>
-      <c r="U18" s="20" t="s">
+      <c r="T18" s="20"/>
+      <c r="U18" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="V18" s="21"/>
-      <c r="W18" s="20" t="s">
+      <c r="V18" s="20"/>
+      <c r="W18" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="20" t="s">
+      <c r="X18" s="20"/>
+      <c r="Y18" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="20" t="s">
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AB18" s="21"/>
-      <c r="AC18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="19"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="11" t="s">
-        <v>124</v>
-      </c>
+      <c r="C19" s="10"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>63</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>233</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>266</v>
       </c>
       <c r="J19" s="1"/>
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="10" t="s">
         <v>47</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="10" t="s">
         <v>69</v>
       </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="11" t="s">
+      <c r="O19" s="10" t="s">
         <v>128</v>
       </c>
       <c r="P19" s="1"/>
-      <c r="Q19" s="11" t="s">
+      <c r="Q19" s="10" t="s">
         <v>209</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="11" t="s">
+      <c r="S19" s="10" t="s">
         <v>70</v>
       </c>
       <c r="T19" s="1"/>
-      <c r="U19" s="11" t="s">
+      <c r="U19" s="10" t="s">
         <v>133</v>
       </c>
       <c r="V19" s="1"/>
-      <c r="W19" s="11" t="s">
+      <c r="W19" s="10" t="s">
         <v>65</v>
       </c>
       <c r="X19" s="1"/>
-      <c r="Y19" s="11" t="s">
+      <c r="Y19" s="10" t="s">
         <v>51</v>
       </c>
       <c r="Z19" s="1"/>
-      <c r="AA19" s="11" t="s">
+      <c r="AA19" s="10" t="s">
         <v>52</v>
       </c>
       <c r="AB19" s="1"/>
-      <c r="AC19" s="11" t="s">
+      <c r="AC19" s="10" t="s">
         <v>93</v>
       </c>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2396,258 +2391,258 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="8" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="1"/>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="8" t="s">
         <v>12</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="9" t="s">
+      <c r="M21" s="8" t="s">
         <v>13</v>
       </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="9" t="s">
+      <c r="O21" s="8" t="s">
         <v>14</v>
       </c>
       <c r="P21" s="1"/>
-      <c r="Q21" s="9" t="s">
+      <c r="Q21" s="8" t="s">
         <v>15</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="S21" s="9" t="s">
+      <c r="S21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="T21" s="1"/>
-      <c r="U21" s="9" t="s">
+      <c r="U21" s="8" t="s">
         <v>17</v>
       </c>
       <c r="V21" s="1"/>
-      <c r="W21" s="9" t="s">
+      <c r="W21" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X21" s="1"/>
-      <c r="Y21" s="7" t="s">
+      <c r="Y21" s="6" t="s">
         <v>41</v>
       </c>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="9" t="s">
+      <c r="AA21" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AB21" s="1"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="34" t="s">
+      <c r="F22" s="34"/>
+      <c r="G22" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="34" t="s">
+      <c r="H22" s="34"/>
+      <c r="I22" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="34" t="s">
+      <c r="J22" s="34"/>
+      <c r="K22" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="L22" s="35"/>
-      <c r="M22" s="34" t="s">
+      <c r="L22" s="34"/>
+      <c r="M22" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="N22" s="35"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="34" t="s">
+      <c r="N22" s="34"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="R22" s="35"/>
-      <c r="S22" s="34" t="s">
+      <c r="R22" s="34"/>
+      <c r="S22" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="T22" s="35"/>
-      <c r="U22" s="34" t="s">
+      <c r="T22" s="34"/>
+      <c r="U22" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="V22" s="35"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="35"/>
-      <c r="AA22" s="34"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="34"/>
+      <c r="AA22" s="33"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="31" t="s">
         <v>186</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="31" t="s">
         <v>185</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="32" t="s">
+      <c r="I23" s="31" t="s">
         <v>210</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="29"/>
+      <c r="K23" s="28"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="30" t="s">
         <v>228</v>
       </c>
       <c r="N23" s="1"/>
-      <c r="O23" s="31" t="s">
+      <c r="O23" s="30" t="s">
         <v>229</v>
       </c>
       <c r="P23" s="1"/>
-      <c r="Q23" s="31" t="s">
+      <c r="Q23" s="30" t="s">
         <v>232</v>
       </c>
       <c r="R23" s="1"/>
-      <c r="S23" s="31" t="s">
+      <c r="S23" s="30" t="s">
         <v>199</v>
       </c>
       <c r="T23" s="1"/>
-      <c r="U23" s="31" t="s">
+      <c r="U23" s="30" t="s">
         <v>144</v>
       </c>
       <c r="V23" s="1"/>
-      <c r="W23" s="29"/>
+      <c r="W23" s="28"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="30"/>
+      <c r="Y23" s="29"/>
       <c r="Z23" s="1"/>
-      <c r="AA23" s="29"/>
+      <c r="AA23" s="28"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="20" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="20" t="s">
+      <c r="F24" s="20"/>
+      <c r="G24" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="20" t="s">
+      <c r="H24" s="20"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="L24" s="21"/>
-      <c r="M24" s="20" t="s">
+      <c r="L24" s="20"/>
+      <c r="M24" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="N24" s="21"/>
-      <c r="O24" s="20" t="s">
+      <c r="N24" s="20"/>
+      <c r="O24" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="20" t="s">
+      <c r="P24" s="20"/>
+      <c r="Q24" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="R24" s="21"/>
-      <c r="S24" s="20" t="s">
+      <c r="R24" s="20"/>
+      <c r="S24" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="T24" s="21"/>
-      <c r="U24" s="20" t="s">
+      <c r="T24" s="20"/>
+      <c r="U24" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="21"/>
-      <c r="W24" s="20"/>
-      <c r="X24" s="21"/>
-      <c r="Y24" s="22" t="s">
+      <c r="V24" s="20"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="Z24" s="21"/>
-      <c r="AA24" s="20"/>
-      <c r="AB24" s="21"/>
-      <c r="AC24" s="24"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="23"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="4"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>64</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="10" t="s">
         <v>90</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="10" t="s">
         <v>265</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="10" t="s">
         <v>221</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="11" t="s">
+      <c r="M25" s="10" t="s">
         <v>68</v>
       </c>
       <c r="N25" s="1"/>
-      <c r="O25" s="11" t="s">
+      <c r="O25" s="10" t="s">
         <v>72</v>
       </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="11" t="s">
+      <c r="Q25" s="10" t="s">
         <v>115</v>
       </c>
       <c r="R25" s="1"/>
-      <c r="S25" s="11" t="s">
+      <c r="S25" s="10" t="s">
         <v>142</v>
       </c>
       <c r="T25" s="1"/>
-      <c r="U25" s="11" t="s">
+      <c r="U25" s="10" t="s">
         <v>66</v>
       </c>
       <c r="V25" s="1"/>
-      <c r="W25" s="11" t="s">
+      <c r="W25" s="10" t="s">
         <v>260</v>
       </c>
       <c r="X25" s="1"/>
-      <c r="Y25" s="11" t="s">
+      <c r="Y25" s="10" t="s">
         <v>239</v>
       </c>
       <c r="Z25" s="1"/>
-      <c r="AA25" s="11"/>
+      <c r="AA25" s="10"/>
       <c r="AB25" s="1"/>
-      <c r="AC25" s="6"/>
+      <c r="AC25" s="5"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2678,254 +2673,258 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>87</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="8" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="1"/>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="8" t="s">
         <v>21</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="9" t="s">
+      <c r="M27" s="8" t="s">
         <v>22</v>
       </c>
       <c r="N27" s="1"/>
-      <c r="O27" s="9" t="s">
+      <c r="O27" s="8" t="s">
         <v>23</v>
       </c>
       <c r="P27" s="1"/>
-      <c r="Q27" s="9" t="s">
+      <c r="Q27" s="8" t="s">
         <v>24</v>
       </c>
       <c r="R27" s="1"/>
-      <c r="S27" s="9" t="s">
+      <c r="S27" s="8" t="s">
         <v>42</v>
       </c>
       <c r="T27" s="1"/>
-      <c r="U27" s="9" t="s">
+      <c r="U27" s="8" t="s">
         <v>43</v>
       </c>
       <c r="V27" s="1"/>
-      <c r="W27" s="9" t="s">
+      <c r="W27" s="8" t="s">
         <v>44</v>
       </c>
       <c r="X27" s="1"/>
-      <c r="Y27" s="12"/>
+      <c r="Y27" s="11"/>
       <c r="Z27" s="1"/>
-      <c r="AA27" s="12"/>
+      <c r="AA27" s="11"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="2"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="34" t="s">
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="34" t="s">
+      <c r="F28" s="34"/>
+      <c r="G28" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="H28" s="35"/>
-      <c r="I28" s="34" t="s">
+      <c r="H28" s="34"/>
+      <c r="I28" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="35"/>
-      <c r="K28" s="34" t="s">
+      <c r="J28" s="34"/>
+      <c r="K28" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="L28" s="35"/>
-      <c r="M28" s="34" t="s">
+      <c r="L28" s="34"/>
+      <c r="M28" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="N28" s="35"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="34" t="s">
+      <c r="N28" s="34"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="R28" s="35"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="34"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="33"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="33"/>
       <c r="X28" s="1"/>
-      <c r="Y28" s="12"/>
+      <c r="Y28" s="11"/>
       <c r="Z28" s="1"/>
-      <c r="AA28" s="12"/>
+      <c r="AA28" s="11"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="2"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
-      <c r="C29" s="29"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="30" t="s">
         <v>211</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="30" t="s">
         <v>176</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="31" t="s">
+      <c r="I29" s="30" t="s">
         <v>114</v>
       </c>
       <c r="J29" s="1"/>
-      <c r="K29" s="29"/>
+      <c r="K29" s="28"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="31" t="s">
+      <c r="M29" s="30" t="s">
         <v>148</v>
       </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="31" t="s">
+      <c r="O29" s="30" t="s">
         <v>180</v>
       </c>
       <c r="P29" s="1"/>
-      <c r="Q29" s="31" t="s">
+      <c r="Q29" s="30" t="s">
         <v>252</v>
       </c>
       <c r="R29" s="1"/>
-      <c r="S29" s="31" t="s">
+      <c r="S29" s="30" t="s">
         <v>244</v>
       </c>
       <c r="T29" s="1"/>
-      <c r="U29" s="31" t="s">
+      <c r="U29" s="30" t="s">
         <v>245</v>
       </c>
       <c r="V29" s="1"/>
-      <c r="W29" s="31" t="s">
+      <c r="W29" s="30" t="s">
         <v>246</v>
       </c>
       <c r="X29" s="1"/>
-      <c r="Y29" s="12"/>
+      <c r="Y29" s="11"/>
       <c r="Z29" s="1"/>
-      <c r="AA29" s="12"/>
+      <c r="AA29" s="11"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="2"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="20" t="s">
+      <c r="C30" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="20" t="s">
+      <c r="F30" s="20"/>
+      <c r="G30" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="20" t="s">
+      <c r="H30" s="20"/>
+      <c r="I30" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="20" t="s">
+      <c r="J30" s="20"/>
+      <c r="K30" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="L30" s="21"/>
-      <c r="M30" s="20" t="s">
+      <c r="L30" s="20"/>
+      <c r="M30" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="N30" s="21"/>
-      <c r="O30" s="20" t="s">
+      <c r="N30" s="20"/>
+      <c r="O30" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="20" t="s">
+      <c r="P30" s="20"/>
+      <c r="Q30" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="R30" s="21"/>
-      <c r="S30" s="20" t="s">
+      <c r="R30" s="20"/>
+      <c r="S30" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="T30" s="21"/>
-      <c r="U30" s="20" t="s">
+      <c r="T30" s="20"/>
+      <c r="U30" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="V30" s="21"/>
-      <c r="W30" s="20" t="s">
+      <c r="V30" s="20"/>
+      <c r="W30" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="X30" s="21"/>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="21"/>
-      <c r="AA30" s="25"/>
-      <c r="AB30" s="21"/>
-      <c r="AC30" s="21"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="24"/>
+      <c r="Z30" s="20"/>
+      <c r="AA30" s="24"/>
+      <c r="AB30" s="20"/>
+      <c r="AC30" s="20"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
-      <c r="C31" s="5"/>
+      <c r="C31" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>71</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="10" t="s">
         <v>67</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="10" t="s">
         <v>112</v>
       </c>
       <c r="L31" s="1"/>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="10" t="s">
         <v>113</v>
       </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="11" t="s">
+      <c r="O31" s="10" t="s">
         <v>88</v>
       </c>
       <c r="P31" s="1"/>
-      <c r="Q31" s="11" t="s">
+      <c r="Q31" s="10" t="s">
         <v>74</v>
       </c>
       <c r="R31" s="1"/>
-      <c r="S31" s="11" t="s">
+      <c r="S31" s="10" t="s">
         <v>53</v>
       </c>
       <c r="T31" s="1"/>
-      <c r="U31" s="11" t="s">
+      <c r="U31" s="10" t="s">
         <v>54</v>
       </c>
       <c r="V31" s="1"/>
-      <c r="W31" s="11" t="s">
+      <c r="W31" s="10" t="s">
         <v>241</v>
       </c>
       <c r="X31" s="1"/>
-      <c r="Y31" s="13"/>
+      <c r="Y31" s="12"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="13"/>
+      <c r="AA31" s="12"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="4"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2958,31 +2957,31 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>136</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>253</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="8" t="s">
         <v>254</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="16"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="15"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="1"/>
@@ -2990,40 +2989,40 @@
       <c r="V33" s="1"/>
       <c r="W33" s="2"/>
       <c r="X33" s="1"/>
-      <c r="Y33" s="9" t="s">
+      <c r="Y33" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="9" t="s">
+      <c r="AA33" s="8" t="s">
         <v>55</v>
       </c>
       <c r="AB33" s="1"/>
-      <c r="AC33" s="9" t="s">
+      <c r="AC33" s="8" t="s">
         <v>81</v>
       </c>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
-      <c r="C34" s="29"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="33" t="s">
         <v>135</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="32"/>
+      <c r="G34" s="31"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="40" t="s">
+      <c r="I34" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="39"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="38"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
       <c r="T34" s="1"/>
@@ -3031,32 +3030,32 @@
       <c r="V34" s="1"/>
       <c r="W34" s="2"/>
       <c r="X34" s="1"/>
-      <c r="Y34" s="29"/>
+      <c r="Y34" s="28"/>
       <c r="Z34" s="1"/>
-      <c r="AA34" s="29"/>
+      <c r="AA34" s="28"/>
       <c r="AB34" s="1"/>
-      <c r="AC34" s="29"/>
+      <c r="AC34" s="28"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
-      <c r="C35" s="29"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="34"/>
+      <c r="E35" s="33"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="32" t="s">
+      <c r="G35" s="31" t="s">
         <v>135</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="38"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
       <c r="T35" s="1"/>
@@ -3064,75 +3063,75 @@
       <c r="V35" s="1"/>
       <c r="W35" s="2"/>
       <c r="X35" s="1"/>
-      <c r="Y35" s="29"/>
+      <c r="Y35" s="28"/>
       <c r="Z35" s="1"/>
-      <c r="AA35" s="32" t="s">
+      <c r="AA35" s="31" t="s">
         <v>216</v>
       </c>
       <c r="AB35" s="1"/>
-      <c r="AC35" s="29"/>
+      <c r="AC35" s="28"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="26" t="s">
+      <c r="D36" s="20"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="28"/>
-      <c r="R36" s="21"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
-      <c r="V36" s="21"/>
-      <c r="W36" s="21"/>
-      <c r="X36" s="21"/>
-      <c r="Y36" s="20" t="s">
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="Z36" s="21"/>
-      <c r="AA36" s="20" t="s">
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="AB36" s="21"/>
-      <c r="AC36" s="20" t="s">
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="19" t="s">
         <v>140</v>
       </c>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
-      <c r="C37" s="11"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="11"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="11"/>
+      <c r="G37" s="10"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="17" t="s">
+      <c r="I37" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="19"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="18"/>
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
       <c r="T37" s="1"/>
@@ -3140,20 +3139,20 @@
       <c r="V37" s="1"/>
       <c r="W37" s="4"/>
       <c r="X37" s="1"/>
-      <c r="Y37" s="11" t="s">
+      <c r="Y37" s="10" t="s">
         <v>85</v>
       </c>
       <c r="Z37" s="1"/>
-      <c r="AA37" s="11" t="s">
+      <c r="AA37" s="10" t="s">
         <v>59</v>
       </c>
       <c r="AB37" s="1"/>
-      <c r="AC37" s="11" t="s">
+      <c r="AC37" s="10" t="s">
         <v>86</v>
       </c>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="2:30" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:30" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -3184,7 +3183,7 @@
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="2"/>
       <c r="D39" s="1"/>
@@ -3208,20 +3207,20 @@
       <c r="V39" s="1"/>
       <c r="W39" s="2"/>
       <c r="X39" s="1"/>
-      <c r="Y39" s="9" t="s">
+      <c r="Y39" s="8" t="s">
         <v>56</v>
       </c>
       <c r="Z39" s="1"/>
-      <c r="AA39" s="9" t="s">
+      <c r="AA39" s="8" t="s">
         <v>57</v>
       </c>
       <c r="AB39" s="1"/>
-      <c r="AC39" s="9" t="s">
+      <c r="AC39" s="8" t="s">
         <v>58</v>
       </c>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="2"/>
       <c r="D40" s="1"/>
@@ -3245,16 +3244,16 @@
       <c r="V40" s="1"/>
       <c r="W40" s="2"/>
       <c r="X40" s="1"/>
-      <c r="Y40" s="32"/>
+      <c r="Y40" s="31"/>
       <c r="Z40" s="1"/>
-      <c r="AA40" s="32"/>
+      <c r="AA40" s="31"/>
       <c r="AB40" s="1"/>
-      <c r="AC40" s="32"/>
+      <c r="AC40" s="31"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="32" t="s">
         <v>219</v>
       </c>
       <c r="D41" s="1"/>
@@ -3264,7 +3263,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="33" t="s">
+      <c r="I41" s="32" t="s">
         <v>188</v>
       </c>
       <c r="J41" s="1"/>
@@ -3284,22 +3283,22 @@
       <c r="V41" s="1"/>
       <c r="W41" s="2"/>
       <c r="X41" s="1"/>
-      <c r="Y41" s="32" t="s">
+      <c r="Y41" s="31" t="s">
         <v>215</v>
       </c>
       <c r="Z41" s="1"/>
-      <c r="AA41" s="32" t="s">
+      <c r="AA41" s="31" t="s">
         <v>217</v>
       </c>
       <c r="AB41" s="1"/>
-      <c r="AC41" s="32" t="s">
+      <c r="AC41" s="31" t="s">
         <v>218</v>
       </c>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
-      <c r="C42" s="33" t="s">
+      <c r="C42" s="32" t="s">
         <v>155</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -3308,10 +3307,10 @@
       <c r="E42" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F42" s="21"/>
+      <c r="F42" s="20"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="33" t="s">
+      <c r="I42" s="32" t="s">
         <v>158</v>
       </c>
       <c r="J42" s="1"/>
@@ -3320,37 +3319,37 @@
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="21"/>
-      <c r="O42" s="33" t="s">
+      <c r="N42" s="20"/>
+      <c r="O42" s="32" t="s">
         <v>224</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="R42" s="21"/>
-      <c r="S42" s="21"/>
-      <c r="T42" s="21"/>
-      <c r="U42" s="21"/>
-      <c r="V42" s="21"/>
-      <c r="W42" s="21"/>
-      <c r="X42" s="21"/>
-      <c r="Y42" s="20" t="s">
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="Z42" s="21"/>
-      <c r="AA42" s="20" t="s">
+      <c r="Z42" s="20"/>
+      <c r="AA42" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="AB42" s="21"/>
-      <c r="AC42" s="20" t="s">
+      <c r="AB42" s="20"/>
+      <c r="AC42" s="19" t="s">
         <v>107</v>
       </c>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="32" t="s">
         <v>182</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -3362,7 +3361,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="33" t="s">
+      <c r="I43" s="32" t="s">
         <v>157</v>
       </c>
       <c r="J43" s="1"/>
@@ -3372,7 +3371,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="4"/>
-      <c r="O43" s="33" t="s">
+      <c r="O43" s="32" t="s">
         <v>201</v>
       </c>
       <c r="P43" s="4"/>
@@ -3386,20 +3385,20 @@
       <c r="V43" s="1"/>
       <c r="W43" s="4"/>
       <c r="X43" s="1"/>
-      <c r="Y43" s="11" t="s">
+      <c r="Y43" s="10" t="s">
         <v>60</v>
       </c>
       <c r="Z43" s="1"/>
-      <c r="AA43" s="11" t="s">
+      <c r="AA43" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AB43" s="1"/>
-      <c r="AC43" s="11" t="s">
+      <c r="AC43" s="10" t="s">
         <v>62</v>
       </c>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>

</xml_diff>